<commit_message>
add case type auth for FT_ComplexCollectionComplex
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/HMCTS/DEVLAB/WS/STS_HMCTS/CCD/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A43AAD6-54A5-CA41-9F00-B8E43DDCA23D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A5368C-6828-C34C-BFB0-ED5885B77CC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5619" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5622" uniqueCount="945">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -11939,7 +11939,7 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E19" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E20" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="41"/>
@@ -16483,7 +16483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="91" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="91" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -29099,10 +29099,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29401,6 +29401,21 @@
         <v>778</v>
       </c>
       <c r="E19" s="139" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="300">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="303"/>
+      <c r="C20" s="367" t="s">
+        <v>883</v>
+      </c>
+      <c r="D20" s="385" t="s">
+        <v>778</v>
+      </c>
+      <c r="E20" s="308" t="s">
         <v>339</v>
       </c>
     </row>
@@ -34030,8 +34045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
allow befta_master solicitors to access befta master case type
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/HMCTS/DEVLAB/WS/STS_HMCTS/CCD/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60E3F5E-4617-CD4E-BB06-FB3EB01BF774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E36F5D5-881A-0741-8136-F05A5819886D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5622" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5625" uniqueCount="946">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2971,6 +2971,9 @@
   </si>
   <si>
     <t>Update a case</t>
+  </si>
+  <si>
+    <t>caseworker-befta_master-solicitor</t>
   </si>
 </sst>
 </file>
@@ -11939,7 +11942,7 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E20" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E21" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="41"/>
@@ -13323,7 +13326,7 @@
   <dimension ref="A1:CR65"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29099,10 +29102,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29110,7 +29113,7 @@
     <col min="1" max="1" width="30.83203125" style="13" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="13" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" style="13" customWidth="1"/>
     <col min="5" max="5" width="28" style="13" customWidth="1"/>
     <col min="6" max="256" width="8.83203125" customWidth="1"/>
   </cols>
@@ -29416,6 +29419,21 @@
         <v>778</v>
       </c>
       <c r="E20" s="308" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="300">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="303"/>
+      <c r="C21" s="367" t="s">
+        <v>884</v>
+      </c>
+      <c r="D21" s="385" t="s">
+        <v>945</v>
+      </c>
+      <c r="E21" s="308" t="s">
         <v>339</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use mock for dynamic list to enable local testing
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1370AD97-5B7B-3943-ADB5-C96E8882FC00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B00532A-535D-094E-92EB-63ABCC323FAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5622" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5622" uniqueCount="946">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2971,6 +2971,9 @@
   </si>
   <si>
     <t>Update a case</t>
+  </si>
+  <si>
+    <t>https://run.mocky.io/v3/8f97e310-a289-487c-b2cf-be9616d8780a</t>
   </si>
 </sst>
 </file>
@@ -16651,8 +16654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16859,7 +16862,7 @@
         <v>489</v>
       </c>
       <c r="J4" s="113" t="s">
-        <v>532</v>
+        <v>945</v>
       </c>
       <c r="K4" s="114"/>
       <c r="L4" s="114"/>
@@ -18429,7 +18432,7 @@
   <hyperlinks>
     <hyperlink ref="J34" r:id="rId1" xr:uid="{D8CF8637-CA9E-D640-B8A5-0839120ED0E2}"/>
     <hyperlink ref="J35" r:id="rId2" xr:uid="{965A59DF-24BC-0646-830A-59FEE12B238C}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{B1AF49E4-49FA-C84C-94E6-3BBDD6902A47}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{7A935D76-EA43-7642-A3D0-D3F6903BBD83}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -34213,7 +34216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
copy authorusations from master caseworker for solicitor 1
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/HMCTS/DEVLAB/WS/STS_HMCTS/CCD/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1370AD97-5B7B-3943-ADB5-C96E8882FC00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC4F992-642F-3E49-952F-DF0A0D526CB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" firstSheet="13" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5622" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5717" uniqueCount="946">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2971,6 +2971,9 @@
   </si>
   <si>
     <t>Update a case</t>
+  </si>
+  <si>
+    <t>caseworker-befta_master-solicitor</t>
   </si>
 </sst>
 </file>
@@ -3661,7 +3664,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="429">
+  <cellXfs count="431">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -4781,6 +4784,12 @@
     <xf numFmtId="49" fontId="42" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -12106,7 +12115,7 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E20" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E21" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="41"/>
@@ -12119,7 +12128,7 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F130" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F150" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="33"/>
     <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="32"/>
@@ -12157,7 +12166,7 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F47" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F49" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
@@ -12171,7 +12180,7 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F35" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F36" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
@@ -29267,10 +29276,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29278,7 +29287,7 @@
     <col min="1" max="1" width="30.83203125" style="13" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="13" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" style="13" customWidth="1"/>
     <col min="6" max="256" width="8.83203125" customWidth="1"/>
   </cols>
@@ -29584,6 +29593,21 @@
         <v>778</v>
       </c>
       <c r="E20" s="294" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="72"/>
+      <c r="C21" s="265" t="s">
+        <v>884</v>
+      </c>
+      <c r="D21" s="429" t="s">
+        <v>945</v>
+      </c>
+      <c r="E21" s="125" t="s">
         <v>339</v>
       </c>
     </row>
@@ -29721,10 +29745,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29733,7 +29757,7 @@
     <col min="2" max="2" width="15.5" style="14" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" style="14" customWidth="1"/>
     <col min="4" max="4" width="40.83203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" style="14" customWidth="1"/>
     <col min="7" max="16384" width="8.83203125" style="19"/>
   </cols>
@@ -29975,38 +29999,38 @@
       </c>
     </row>
     <row r="14" spans="1:6" s="292" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="286">
-        <v>42736</v>
-      </c>
-      <c r="B14" s="287"/>
-      <c r="C14" s="288" t="s">
+      <c r="A14" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="61"/>
+      <c r="C14" s="62" t="s">
         <v>884</v>
       </c>
-      <c r="D14" s="293" t="s">
+      <c r="D14" s="65" t="s">
         <v>762</v>
       </c>
-      <c r="E14" s="289" t="s">
+      <c r="E14" s="81" t="s">
         <v>778</v>
       </c>
-      <c r="F14" s="294" t="s">
+      <c r="F14" s="115" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="292" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="286">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="287"/>
-      <c r="C15" s="288" t="s">
+      <c r="A15" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="61"/>
+      <c r="C15" s="62" t="s">
         <v>884</v>
       </c>
-      <c r="D15" s="293" t="s">
+      <c r="D15" s="65" t="s">
         <v>763</v>
       </c>
-      <c r="E15" s="289" t="s">
+      <c r="E15" s="81" t="s">
         <v>778</v>
       </c>
-      <c r="F15" s="294" t="s">
+      <c r="F15" s="115" t="s">
         <v>339</v>
       </c>
     </row>
@@ -30137,38 +30161,38 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="405">
-        <v>42736</v>
-      </c>
-      <c r="B23" s="406"/>
+      <c r="A23" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B23" s="81"/>
       <c r="C23" s="65" t="s">
         <v>884</v>
       </c>
-      <c r="D23" s="407" t="s">
+      <c r="D23" s="65" t="s">
         <v>939</v>
       </c>
-      <c r="E23" s="406" t="s">
+      <c r="E23" s="81" t="s">
         <v>778</v>
       </c>
-      <c r="F23" s="408" t="s">
+      <c r="F23" s="115" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="405">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="406"/>
+      <c r="A24" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="81"/>
       <c r="C24" s="65" t="s">
         <v>884</v>
       </c>
-      <c r="D24" s="407" t="s">
+      <c r="D24" s="65" t="s">
         <v>940</v>
       </c>
-      <c r="E24" s="406" t="s">
+      <c r="E24" s="81" t="s">
         <v>778</v>
       </c>
-      <c r="F24" s="408" t="s">
+      <c r="F24" s="115" t="s">
         <v>339</v>
       </c>
     </row>
@@ -32080,8 +32104,365 @@
         <v>339</v>
       </c>
     </row>
+    <row r="131" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A131" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B131" s="61"/>
+      <c r="C131" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D131" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="E131" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F131" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
     <row r="132" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="19"/>
+      <c r="A132" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B132" s="61"/>
+      <c r="C132" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D132" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="E132" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F132" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A133" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B133" s="61"/>
+      <c r="C133" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D133" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="E133" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F133" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A134" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B134" s="61"/>
+      <c r="C134" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D134" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="E134" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F134" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A135" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B135" s="61"/>
+      <c r="C135" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D135" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E135" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F135" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A136" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B136" s="61"/>
+      <c r="C136" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D136" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="E136" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F136" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A137" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B137" s="61"/>
+      <c r="C137" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D137" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E137" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F137" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A138" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B138" s="61"/>
+      <c r="C138" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D138" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="E138" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F138" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A139" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B139" s="61"/>
+      <c r="C139" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D139" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="E139" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F139" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A140" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B140" s="61"/>
+      <c r="C140" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D140" s="65" t="s">
+        <v>762</v>
+      </c>
+      <c r="E140" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F140" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A141" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B141" s="61"/>
+      <c r="C141" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D141" s="65" t="s">
+        <v>763</v>
+      </c>
+      <c r="E141" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F141" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A142" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B142" s="61"/>
+      <c r="C142" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D142" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="E142" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F142" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A143" s="143">
+        <v>42737</v>
+      </c>
+      <c r="B143" s="128"/>
+      <c r="C143" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D143" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="E143" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F143" s="199" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A144" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B144" s="61"/>
+      <c r="C144" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D144" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="E144" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F144" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A145" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B145" s="61"/>
+      <c r="C145" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D145" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="E145" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F145" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A146" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B146" s="61"/>
+      <c r="C146" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D146" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="E146" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F146" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A147" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B147" s="61"/>
+      <c r="C147" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D147" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="E147" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F147" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A148" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B148" s="67"/>
+      <c r="C148" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D148" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="E148" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F148" s="119" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A149" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B149" s="61"/>
+      <c r="C149" s="65" t="s">
+        <v>884</v>
+      </c>
+      <c r="D149" s="65" t="s">
+        <v>939</v>
+      </c>
+      <c r="E149" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F149" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A150" s="263">
+        <v>42736</v>
+      </c>
+      <c r="B150" s="324"/>
+      <c r="C150" s="73" t="s">
+        <v>884</v>
+      </c>
+      <c r="D150" s="73" t="s">
+        <v>940</v>
+      </c>
+      <c r="E150" s="81" t="s">
+        <v>945</v>
+      </c>
+      <c r="F150" s="266" t="s">
+        <v>339</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="58" type="noConversion"/>
@@ -32245,10 +32626,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:EK47"/>
+  <dimension ref="A1:EK49"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -33379,6 +33760,42 @@
         <v>339</v>
       </c>
     </row>
+    <row r="48" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="263">
+        <v>42736</v>
+      </c>
+      <c r="B48" s="430"/>
+      <c r="C48" s="73" t="s">
+        <v>884</v>
+      </c>
+      <c r="D48" s="265" t="s">
+        <v>392</v>
+      </c>
+      <c r="E48" s="429" t="s">
+        <v>945</v>
+      </c>
+      <c r="F48" s="266" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B49" s="81"/>
+      <c r="C49" s="62" t="s">
+        <v>884</v>
+      </c>
+      <c r="D49" s="65" t="s">
+        <v>943</v>
+      </c>
+      <c r="E49" s="429" t="s">
+        <v>945</v>
+      </c>
+      <c r="F49" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -33393,10 +33810,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:CF35"/>
+  <dimension ref="A1:CF36"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -34197,6 +34614,24 @@
         <v>339</v>
       </c>
     </row>
+    <row r="36" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="263">
+        <v>42736</v>
+      </c>
+      <c r="B36" s="430"/>
+      <c r="C36" s="265" t="s">
+        <v>884</v>
+      </c>
+      <c r="D36" s="265" t="s">
+        <v>489</v>
+      </c>
+      <c r="E36" s="429" t="s">
+        <v>945</v>
+      </c>
+      <c r="F36" s="266" t="s">
+        <v>339</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -34213,7 +34648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -43581,7 +44016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2A25AD-5D69-564D-9511-0323740C2E1F}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RDM-9309: Functional Tests for CaseLink           [RDM-9309] (https://tools.hmcts.net/jira/browse/RDM-9309).
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skynet/Desktop/mis_cosas/work/MoJ/repositories/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B47D9BB-96FF-4842-BE9B-A405B35790D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC470F67-B011-454A-9AAF-A0FB12110DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19940" firstSheet="10" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5798" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5798" uniqueCount="962">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3019,6 +3019,9 @@
   </si>
   <si>
     <t>Create Collection of Complex Case Links</t>
+  </si>
+  <si>
+    <t>https://run.mocky.io/v3/8f97e310-a289-487c-b2cf-be9616d8780a</t>
   </si>
 </sst>
 </file>
@@ -4907,442 +4910,6 @@
   </cellStyles>
   <dxfs count="303">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0432FF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -6724,6 +6291,442 @@
         <color theme="0"/>
         <name val="Arial"/>
         <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -12182,58 +12185,58 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I53" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I53" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="61"/>
+    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E21" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E21" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F153" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49" totalsRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F153" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12252,40 +12255,40 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="36" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="22" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F50" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F50" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F36" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F36" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16788,8 +16791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="91" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D2" zoomScale="109" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16996,7 +16999,7 @@
         <v>489</v>
       </c>
       <c r="J4" s="113" t="s">
-        <v>532</v>
+        <v>961</v>
       </c>
       <c r="K4" s="114"/>
       <c r="L4" s="114"/>
@@ -32988,7 +32991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:EK50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update def file again
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skynet/Desktop/mis_cosas/work/MoJ/repositories/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC470F67-B011-454A-9AAF-A0FB12110DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8802C10B-7446-B94F-BE41-F68B932BC91A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5798" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5809" uniqueCount="963">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3022,6 +3022,9 @@
   </si>
   <si>
     <t>https://run.mocky.io/v3/8f97e310-a289-487c-b2cf-be9616d8780a</t>
+  </si>
+  <si>
+    <t>Searchable</t>
   </si>
 </sst>
 </file>
@@ -3033,7 +3036,7 @@
     <numFmt numFmtId="165" formatCode="&quot;D/&quot;m&quot;/YY&quot;"/>
     <numFmt numFmtId="166" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
   </numFmts>
-  <fonts count="65" x14ac:knownFonts="1">
+  <fonts count="66" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -3435,6 +3438,11 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -3718,7 +3726,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="450">
+  <cellXfs count="451">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -4891,6 +4899,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="65" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -4908,7 +4919,31 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal 2 3" xfId="13" xr:uid="{983C50BB-8B6C-1941-95CA-614B186AEA1E}"/>
   </cellStyles>
-  <dxfs count="303">
+  <dxfs count="304">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -12056,374 +12091,375 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="302" dataDxfId="300" headerRowBorderDxfId="301" tableBorderDxfId="299" totalsRowBorderDxfId="298">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="303" dataDxfId="301" headerRowBorderDxfId="302" tableBorderDxfId="300" totalsRowBorderDxfId="299">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="297"/>
-    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="296"/>
-    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="295"/>
-    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="294"/>
-    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="293"/>
+    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="298"/>
+    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="297"/>
+    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="296"/>
+    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="295"/>
+    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="294"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H28" totalsRowShown="0" headerRowDxfId="170" dataDxfId="168" headerRowBorderDxfId="169" tableBorderDxfId="167" totalsRowBorderDxfId="166">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H28" totalsRowShown="0" headerRowDxfId="171" dataDxfId="169" headerRowBorderDxfId="170" tableBorderDxfId="168" totalsRowBorderDxfId="167">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="165"/>
-    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="164"/>
-    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="163"/>
-    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="162"/>
-    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="161"/>
-    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="160"/>
-    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="159"/>
-    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="158"/>
+    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="166"/>
+    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="165"/>
+    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="164"/>
+    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="163"/>
+    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="162"/>
+    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="161"/>
+    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="160"/>
+    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="159"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:T40" totalsRowShown="0" headerRowDxfId="157" dataDxfId="155" headerRowBorderDxfId="156" tableBorderDxfId="154" totalsRowBorderDxfId="153">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:T40" totalsRowShown="0" headerRowDxfId="158" dataDxfId="156" headerRowBorderDxfId="157" tableBorderDxfId="155" totalsRowBorderDxfId="154">
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="152"/>
-    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="151"/>
-    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="150"/>
-    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="149"/>
-    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="148"/>
-    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="147"/>
-    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="146"/>
-    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="145"/>
-    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="144"/>
-    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="143" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="142"/>
-    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="141"/>
-    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="140"/>
-    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="139"/>
-    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="138"/>
-    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="137"/>
-    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="136"/>
-    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="135"/>
-    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="134"/>
-    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="EndButtonLabel" dataDxfId="133"/>
+    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="153"/>
+    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="152"/>
+    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="151"/>
+    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="150"/>
+    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="149"/>
+    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="148"/>
+    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="147"/>
+    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="146"/>
+    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="145"/>
+    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="144" dataCellStyle="Hyperlink"/>
+    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="143"/>
+    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="142"/>
+    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="141"/>
+    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="140"/>
+    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="139"/>
+    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="138"/>
+    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="137"/>
+    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="136"/>
+    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="135"/>
+    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="EndButtonLabel" dataDxfId="134"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:Q159" totalsRowShown="0" headerRowDxfId="132" dataDxfId="130" headerRowBorderDxfId="131" tableBorderDxfId="129" totalsRowBorderDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:Q159" totalsRowShown="0" headerRowDxfId="133" dataDxfId="131" headerRowBorderDxfId="132" tableBorderDxfId="130" totalsRowBorderDxfId="129">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="127"/>
-    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="126"/>
-    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="125"/>
-    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="124"/>
-    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="123"/>
-    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="122"/>
-    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="121"/>
-    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="120"/>
-    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="119"/>
-    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="118"/>
-    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="117"/>
-    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="116"/>
-    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="115"/>
-    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="114"/>
-    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="113"/>
-    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="112"/>
-    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="111"/>
+    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="128"/>
+    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="127"/>
+    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="126"/>
+    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="125"/>
+    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="124"/>
+    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="123"/>
+    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="122"/>
+    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="121"/>
+    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="120"/>
+    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="119"/>
+    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="118"/>
+    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="117"/>
+    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="116"/>
+    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="115"/>
+    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="114"/>
+    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="113"/>
+    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H46" totalsRowShown="0" headerRowDxfId="110" dataDxfId="108" headerRowBorderDxfId="109" tableBorderDxfId="107" totalsRowBorderDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H46" totalsRowShown="0" headerRowDxfId="111" dataDxfId="109" headerRowBorderDxfId="110" tableBorderDxfId="108" totalsRowBorderDxfId="107">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="100"/>
-    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="99"/>
-    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="103"/>
+    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="102"/>
+    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:G35" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96" tableBorderDxfId="94" totalsRowBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:G35" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="89"/>
+    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="88"/>
+    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H52" totalsRowShown="0" headerRowDxfId="85" dataDxfId="83" headerRowBorderDxfId="84" tableBorderDxfId="82" totalsRowBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H52" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83" totalsRowBorderDxfId="82">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="75"/>
+    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I53" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I53" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="61"/>
-    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="62"/>
+    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E21" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E21" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F153" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F153" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="292" dataDxfId="290" headerRowBorderDxfId="291" tableBorderDxfId="289" totalsRowBorderDxfId="288">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="293" dataDxfId="291" headerRowBorderDxfId="292" tableBorderDxfId="290" totalsRowBorderDxfId="289">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="287"/>
-    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="286"/>
-    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="285"/>
-    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="284" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="288"/>
+    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="287"/>
+    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="286"/>
+    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="285" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="22" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="23" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F50" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F36" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F36" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I17" totalsRowShown="0" headerRowDxfId="283" dataDxfId="281" headerRowBorderDxfId="282" tableBorderDxfId="280" totalsRowBorderDxfId="279">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I17" totalsRowShown="0" headerRowDxfId="284" dataDxfId="282" headerRowBorderDxfId="283" tableBorderDxfId="281" totalsRowBorderDxfId="280">
   <autoFilter ref="A3:I17" xr:uid="{C0075E79-5DBE-654F-827E-CA137EF61FB4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="278"/>
-    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="277"/>
-    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="276"/>
-    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="275"/>
-    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="274"/>
-    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="273"/>
-    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="272"/>
-    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="271"/>
-    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="270"/>
+    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="279"/>
+    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="278"/>
+    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="277"/>
+    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="276"/>
+    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="275"/>
+    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="274"/>
+    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="273"/>
+    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="272"/>
+    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="271"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:M131" totalsRowShown="0" headerRowDxfId="269" dataDxfId="267" headerRowBorderDxfId="268" tableBorderDxfId="266" totalsRowBorderDxfId="265">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:M131" totalsRowShown="0" headerRowDxfId="270" dataDxfId="268" headerRowBorderDxfId="269" tableBorderDxfId="267" totalsRowBorderDxfId="266">
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="264"/>
-    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="263"/>
-    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="262"/>
-    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="261"/>
-    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="260"/>
-    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="259"/>
-    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="258"/>
-    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="257"/>
-    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="256"/>
-    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="255"/>
-    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="254"/>
-    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="253"/>
-    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="252"/>
+    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="265"/>
+    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="264"/>
+    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="263"/>
+    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="262"/>
+    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="261"/>
+    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="260"/>
+    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="259"/>
+    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="258"/>
+    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="257"/>
+    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="256"/>
+    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="255"/>
+    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="254"/>
+    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="253"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:R76" totalsRowShown="0" headerRowDxfId="251" dataDxfId="249" headerRowBorderDxfId="250" tableBorderDxfId="248" totalsRowBorderDxfId="247">
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="246"/>
-    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="245"/>
-    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="244"/>
-    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="243"/>
-    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="242"/>
-    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="241"/>
-    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="240"/>
-    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="239"/>
-    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="238"/>
-    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="237"/>
-    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="236"/>
-    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="235"/>
-    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="234"/>
-    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="233"/>
-    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="232"/>
-    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="231"/>
-    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="230"/>
-    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="229"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:S76" totalsRowShown="0" headerRowDxfId="252" dataDxfId="250" headerRowBorderDxfId="251" tableBorderDxfId="249" totalsRowBorderDxfId="248">
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="247"/>
+    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="246"/>
+    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="245"/>
+    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="244"/>
+    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="243"/>
+    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="242"/>
+    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="241"/>
+    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="240"/>
+    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="239"/>
+    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="238"/>
+    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="237"/>
+    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="236"/>
+    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="235"/>
+    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="234"/>
+    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="233"/>
+    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="232"/>
+    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="231"/>
+    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="230"/>
+    <tableColumn id="19" xr3:uid="{4721EA60-AB43-3A4D-9D3A-D995D789F1AA}" name="Searchable" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G41" totalsRowShown="0" headerRowDxfId="228" dataDxfId="226" headerRowBorderDxfId="227" tableBorderDxfId="225" totalsRowBorderDxfId="224" headerRowCellStyle="Normal 2 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G41" totalsRowShown="0" headerRowDxfId="229" dataDxfId="227" headerRowBorderDxfId="228" tableBorderDxfId="226" totalsRowBorderDxfId="225" headerRowCellStyle="Normal 2 3">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="223"/>
-    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="222"/>
-    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="221"/>
-    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="220"/>
-    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="219"/>
-    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="218"/>
-    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="217"/>
+    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="224"/>
+    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="223"/>
+    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="222"/>
+    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="221"/>
+    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="220"/>
+    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="219"/>
+    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="218"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:L58" totalsRowShown="0" headerRowDxfId="216" dataDxfId="214" headerRowBorderDxfId="215" tableBorderDxfId="213" totalsRowBorderDxfId="212">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:L58" totalsRowShown="0" headerRowDxfId="217" dataDxfId="215" headerRowBorderDxfId="216" tableBorderDxfId="214" totalsRowBorderDxfId="213">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="211"/>
-    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="210"/>
-    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="209"/>
-    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="208"/>
-    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="207"/>
-    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="206"/>
-    <tableColumn id="12" xr3:uid="{4E9EBE21-1E8A-8F42-8DBF-15D634A7D163}" name="DefaultValue" dataDxfId="205"/>
-    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="204"/>
-    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="203"/>
-    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="202"/>
-    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="201"/>
-    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="200"/>
+    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="212"/>
+    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="211"/>
+    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="210"/>
+    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="209"/>
+    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="208"/>
+    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="207"/>
+    <tableColumn id="12" xr3:uid="{4E9EBE21-1E8A-8F42-8DBF-15D634A7D163}" name="DefaultValue" dataDxfId="206"/>
+    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="205"/>
+    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="204"/>
+    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="203"/>
+    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="202"/>
+    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="201"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G24" totalsRowShown="0" headerRowDxfId="199" dataDxfId="197" headerRowBorderDxfId="198" tableBorderDxfId="196" totalsRowBorderDxfId="195">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G24" totalsRowShown="0" headerRowDxfId="200" dataDxfId="198" headerRowBorderDxfId="199" tableBorderDxfId="197" totalsRowBorderDxfId="196">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="194"/>
-    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="193"/>
-    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="192"/>
-    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="191"/>
-    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="190"/>
-    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="189"/>
-    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="188"/>
+    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="195"/>
+    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="194"/>
+    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="193"/>
+    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="192"/>
+    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="191"/>
+    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="190"/>
+    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="189"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L66" totalsRowShown="0" headerRowDxfId="187" dataDxfId="185" headerRowBorderDxfId="186" tableBorderDxfId="184" totalsRowBorderDxfId="183">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L66" totalsRowShown="0" headerRowDxfId="188" dataDxfId="186" headerRowBorderDxfId="187" tableBorderDxfId="185" totalsRowBorderDxfId="184">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="182"/>
-    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="181"/>
-    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="180"/>
-    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="179"/>
-    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="178"/>
-    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="177"/>
-    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="176"/>
-    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="175"/>
-    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="174"/>
-    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="173"/>
-    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="172"/>
-    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="171"/>
+    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="180"/>
+    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="179"/>
+    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="178"/>
+    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="177"/>
+    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="176"/>
+    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="175"/>
+    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="174"/>
+    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="173"/>
+    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="172"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16791,7 +16827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D2" zoomScale="109" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D4" zoomScale="109" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -35766,9 +35802,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IO131"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -35791,7 +35827,7 @@
     <col min="250" max="16384" width="8.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>36</v>
       </c>
@@ -35814,7 +35850,7 @@
       <c r="L1" s="34"/>
       <c r="M1" s="34"/>
     </row>
-    <row r="2" spans="1:14" ht="90.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="90.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="29" t="s">
         <v>4</v>
       </c>
@@ -35856,7 +35892,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="106" t="s">
         <v>9</v>
       </c>
@@ -35899,8 +35935,11 @@
       <c r="N3" s="300" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O3" s="20" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="60">
         <v>42736</v>
       </c>
@@ -35930,7 +35969,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="60">
         <v>42736</v>
       </c>
@@ -35960,7 +35999,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="60">
         <v>42736</v>
       </c>
@@ -35990,7 +36029,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="60">
         <v>42736</v>
       </c>
@@ -36020,7 +36059,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="60">
         <v>42736</v>
       </c>
@@ -36050,7 +36089,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="60">
         <v>42736</v>
       </c>
@@ -36080,7 +36119,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="60">
         <v>42736</v>
       </c>
@@ -36110,7 +36149,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="66">
         <v>42736</v>
       </c>
@@ -36142,7 +36181,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="60">
         <v>42736</v>
       </c>
@@ -36174,7 +36213,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="66">
         <v>42737</v>
       </c>
@@ -36204,7 +36243,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="60">
         <v>42736</v>
       </c>
@@ -36236,7 +36275,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="60">
         <v>42736</v>
       </c>
@@ -36266,7 +36305,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="60">
         <v>42736</v>
       </c>
@@ -37313,6 +37352,9 @@
       <c r="N34" s="17" t="s">
         <v>784</v>
       </c>
+      <c r="O34" s="20" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="35" spans="1:249" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="60">
@@ -37344,6 +37386,9 @@
       <c r="M35" s="64"/>
       <c r="N35" s="17" t="s">
         <v>784</v>
+      </c>
+      <c r="O35" s="20" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="36" spans="1:249" ht="17" customHeight="1" x14ac:dyDescent="0.15">
@@ -42643,10 +42688,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:R78"/>
+  <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView showGridLines="0" topLeftCell="E12" workbookViewId="0">
+      <selection activeCell="J34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -42665,11 +42710,13 @@
     <col min="13" max="13" width="18.83203125" style="20" customWidth="1"/>
     <col min="14" max="14" width="17.1640625" style="20" customWidth="1"/>
     <col min="15" max="15" width="64.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="249" width="8.83203125" style="19" customWidth="1"/>
+    <col min="16" max="18" width="8.83203125" style="19" customWidth="1"/>
+    <col min="19" max="19" width="10.5" style="19" customWidth="1"/>
+    <col min="20" max="249" width="8.83203125" style="19" customWidth="1"/>
     <col min="250" max="16384" width="8.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>219</v>
       </c>
@@ -42693,7 +42740,7 @@
       <c r="M1" s="35"/>
       <c r="N1" s="35"/>
     </row>
-    <row r="2" spans="1:18" ht="123.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" ht="123.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="46" t="s">
         <v>4</v>
       </c>
@@ -42735,7 +42782,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
         <v>9</v>
       </c>
@@ -42790,8 +42837,11 @@
       <c r="R3" s="301" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S3" s="450" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="60">
         <v>42736</v>
       </c>
@@ -42822,8 +42872,9 @@
       <c r="P4" s="103"/>
       <c r="Q4" s="103"/>
       <c r="R4" s="103"/>
-    </row>
-    <row r="5" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S4" s="103"/>
+    </row>
+    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="60">
         <v>42736</v>
       </c>
@@ -42854,8 +42905,9 @@
       <c r="P5" s="62"/>
       <c r="Q5" s="62"/>
       <c r="R5" s="62"/>
-    </row>
-    <row r="6" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S5" s="62"/>
+    </row>
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="60">
         <v>42736</v>
       </c>
@@ -42886,8 +42938,9 @@
       <c r="P6" s="62"/>
       <c r="Q6" s="62"/>
       <c r="R6" s="62"/>
-    </row>
-    <row r="7" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S6" s="62"/>
+    </row>
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="60">
         <v>42736</v>
       </c>
@@ -42918,8 +42971,9 @@
       <c r="P7" s="62"/>
       <c r="Q7" s="62"/>
       <c r="R7" s="62"/>
-    </row>
-    <row r="8" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S7" s="62"/>
+    </row>
+    <row r="8" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="60">
         <v>42736</v>
       </c>
@@ -42950,8 +43004,9 @@
       <c r="P8" s="62"/>
       <c r="Q8" s="62"/>
       <c r="R8" s="62"/>
-    </row>
-    <row r="9" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S8" s="62"/>
+    </row>
+    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="60">
         <v>42736</v>
       </c>
@@ -42982,8 +43037,9 @@
       <c r="P9" s="62"/>
       <c r="Q9" s="62"/>
       <c r="R9" s="62"/>
-    </row>
-    <row r="10" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S9" s="62"/>
+    </row>
+    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="60">
         <v>42736</v>
       </c>
@@ -43014,8 +43070,9 @@
       <c r="P10" s="62"/>
       <c r="Q10" s="62"/>
       <c r="R10" s="62"/>
-    </row>
-    <row r="11" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S10" s="62"/>
+    </row>
+    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="60">
         <v>42736</v>
       </c>
@@ -43046,8 +43103,9 @@
       <c r="P11" s="62"/>
       <c r="Q11" s="62"/>
       <c r="R11" s="62"/>
-    </row>
-    <row r="12" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S11" s="62"/>
+    </row>
+    <row r="12" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="66">
         <v>42736</v>
       </c>
@@ -43080,8 +43138,9 @@
       <c r="P12" s="68"/>
       <c r="Q12" s="68"/>
       <c r="R12" s="68"/>
-    </row>
-    <row r="13" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S12" s="68"/>
+    </row>
+    <row r="13" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="66">
         <v>42736</v>
       </c>
@@ -43114,8 +43173,9 @@
       <c r="P13" s="68"/>
       <c r="Q13" s="68"/>
       <c r="R13" s="68"/>
-    </row>
-    <row r="14" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S13" s="68"/>
+    </row>
+    <row r="14" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="60">
         <v>42736</v>
       </c>
@@ -43146,8 +43206,9 @@
       <c r="P14" s="62"/>
       <c r="Q14" s="62"/>
       <c r="R14" s="62"/>
-    </row>
-    <row r="15" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S14" s="62"/>
+    </row>
+    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="60">
         <v>42736</v>
       </c>
@@ -43178,8 +43239,9 @@
       <c r="P15" s="62"/>
       <c r="Q15" s="62"/>
       <c r="R15" s="62"/>
-    </row>
-    <row r="16" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S15" s="62"/>
+    </row>
+    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="60">
         <v>42736</v>
       </c>
@@ -43210,8 +43272,9 @@
       <c r="P16" s="62"/>
       <c r="Q16" s="62"/>
       <c r="R16" s="62"/>
-    </row>
-    <row r="17" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S16" s="62"/>
+    </row>
+    <row r="17" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="60">
         <v>42736</v>
       </c>
@@ -43242,8 +43305,9 @@
       <c r="P17" s="62"/>
       <c r="Q17" s="62"/>
       <c r="R17" s="62"/>
-    </row>
-    <row r="18" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S17" s="62"/>
+    </row>
+    <row r="18" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="60">
         <v>42736</v>
       </c>
@@ -43274,8 +43338,9 @@
       <c r="P18" s="62"/>
       <c r="Q18" s="62"/>
       <c r="R18" s="62"/>
-    </row>
-    <row r="19" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S18" s="62"/>
+    </row>
+    <row r="19" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="60">
         <v>42736</v>
       </c>
@@ -43306,8 +43371,9 @@
       <c r="P19" s="62"/>
       <c r="Q19" s="62"/>
       <c r="R19" s="62"/>
-    </row>
-    <row r="20" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S19" s="62"/>
+    </row>
+    <row r="20" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="60">
         <v>42736</v>
       </c>
@@ -43338,8 +43404,9 @@
       <c r="P20" s="62"/>
       <c r="Q20" s="62"/>
       <c r="R20" s="62"/>
-    </row>
-    <row r="21" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S20" s="62"/>
+    </row>
+    <row r="21" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="60">
         <v>42736</v>
       </c>
@@ -43370,8 +43437,9 @@
       <c r="P21" s="62"/>
       <c r="Q21" s="62"/>
       <c r="R21" s="62"/>
-    </row>
-    <row r="22" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S21" s="62"/>
+    </row>
+    <row r="22" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="60">
         <v>42736</v>
       </c>
@@ -43402,8 +43470,9 @@
       <c r="P22" s="62"/>
       <c r="Q22" s="62"/>
       <c r="R22" s="62"/>
-    </row>
-    <row r="23" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S22" s="62"/>
+    </row>
+    <row r="23" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="60">
         <v>42736</v>
       </c>
@@ -43434,8 +43503,9 @@
       <c r="P23" s="62"/>
       <c r="Q23" s="62"/>
       <c r="R23" s="62"/>
-    </row>
-    <row r="24" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S23" s="62"/>
+    </row>
+    <row r="24" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="60">
         <v>42736</v>
       </c>
@@ -43466,8 +43536,9 @@
       <c r="P24" s="62"/>
       <c r="Q24" s="62"/>
       <c r="R24" s="62"/>
-    </row>
-    <row r="25" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S24" s="62"/>
+    </row>
+    <row r="25" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="60">
         <v>42736</v>
       </c>
@@ -43498,8 +43569,11 @@
       <c r="P25" s="62"/>
       <c r="Q25" s="62"/>
       <c r="R25" s="62"/>
-    </row>
-    <row r="26" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S25" s="62" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="60">
         <v>42736</v>
       </c>
@@ -43532,8 +43606,11 @@
       <c r="P26" s="62"/>
       <c r="Q26" s="62"/>
       <c r="R26" s="62"/>
-    </row>
-    <row r="27" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S26" s="62" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="60">
         <v>42736</v>
       </c>
@@ -43564,8 +43641,9 @@
       <c r="P27" s="62"/>
       <c r="Q27" s="62"/>
       <c r="R27" s="62"/>
-    </row>
-    <row r="28" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S27" s="62"/>
+    </row>
+    <row r="28" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="60">
         <v>42736</v>
       </c>
@@ -43598,8 +43676,9 @@
       <c r="P28" s="62"/>
       <c r="Q28" s="62"/>
       <c r="R28" s="62"/>
-    </row>
-    <row r="29" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S28" s="62"/>
+    </row>
+    <row r="29" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="60">
         <v>42736</v>
       </c>
@@ -43630,8 +43709,9 @@
       <c r="P29" s="62"/>
       <c r="Q29" s="62"/>
       <c r="R29" s="62"/>
-    </row>
-    <row r="30" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S29" s="62"/>
+    </row>
+    <row r="30" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="60">
         <v>42736</v>
       </c>
@@ -43662,8 +43742,9 @@
       <c r="P30" s="62"/>
       <c r="Q30" s="62"/>
       <c r="R30" s="62"/>
-    </row>
-    <row r="31" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S30" s="62"/>
+    </row>
+    <row r="31" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="60">
         <v>42736</v>
       </c>
@@ -43694,8 +43775,9 @@
       <c r="P31" s="62"/>
       <c r="Q31" s="62"/>
       <c r="R31" s="62"/>
-    </row>
-    <row r="32" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S31" s="62"/>
+    </row>
+    <row r="32" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="60">
         <v>42736</v>
       </c>
@@ -43726,8 +43808,9 @@
       <c r="P32" s="62"/>
       <c r="Q32" s="62"/>
       <c r="R32" s="62"/>
-    </row>
-    <row r="33" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S32" s="62"/>
+    </row>
+    <row r="33" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="60">
         <v>42736</v>
       </c>
@@ -43758,8 +43841,11 @@
       <c r="P33" s="62"/>
       <c r="Q33" s="62"/>
       <c r="R33" s="62"/>
-    </row>
-    <row r="34" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S33" s="62" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="60">
         <v>42736</v>
       </c>
@@ -43790,8 +43876,11 @@
       <c r="P34" s="62"/>
       <c r="Q34" s="62"/>
       <c r="R34" s="62"/>
-    </row>
-    <row r="35" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S34" s="62" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="60">
         <v>42736</v>
       </c>
@@ -43822,8 +43911,11 @@
       <c r="P35" s="62"/>
       <c r="Q35" s="62"/>
       <c r="R35" s="62"/>
-    </row>
-    <row r="36" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S35" s="62" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="60">
         <v>42736</v>
       </c>
@@ -43854,8 +43946,11 @@
       <c r="P36" s="62"/>
       <c r="Q36" s="62"/>
       <c r="R36" s="62"/>
-    </row>
-    <row r="37" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S36" s="62" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="60">
         <v>42736</v>
       </c>
@@ -43886,8 +43981,11 @@
       <c r="P37" s="62"/>
       <c r="Q37" s="62"/>
       <c r="R37" s="62"/>
-    </row>
-    <row r="38" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S37" s="62" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="60">
         <v>42736</v>
       </c>
@@ -43920,8 +44018,9 @@
       <c r="P38" s="62"/>
       <c r="Q38" s="62"/>
       <c r="R38" s="62"/>
-    </row>
-    <row r="39" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S38" s="62"/>
+    </row>
+    <row r="39" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="66">
         <v>42736</v>
       </c>
@@ -43952,8 +44051,9 @@
       <c r="P39" s="68"/>
       <c r="Q39" s="68"/>
       <c r="R39" s="68"/>
-    </row>
-    <row r="40" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S39" s="68"/>
+    </row>
+    <row r="40" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="66">
         <v>42736</v>
       </c>
@@ -43986,8 +44086,9 @@
       <c r="P40" s="68"/>
       <c r="Q40" s="68"/>
       <c r="R40" s="68"/>
-    </row>
-    <row r="41" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S40" s="68"/>
+    </row>
+    <row r="41" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="66">
         <v>42736</v>
       </c>
@@ -44018,8 +44119,9 @@
       <c r="P41" s="68"/>
       <c r="Q41" s="68"/>
       <c r="R41" s="68"/>
-    </row>
-    <row r="42" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S41" s="68"/>
+    </row>
+    <row r="42" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="66">
         <v>42736</v>
       </c>
@@ -44050,8 +44152,9 @@
       <c r="P42" s="68"/>
       <c r="Q42" s="68"/>
       <c r="R42" s="68"/>
-    </row>
-    <row r="43" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S42" s="68"/>
+    </row>
+    <row r="43" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="66">
         <v>42736</v>
       </c>
@@ -44082,8 +44185,9 @@
       <c r="P43" s="68"/>
       <c r="Q43" s="68"/>
       <c r="R43" s="68"/>
-    </row>
-    <row r="44" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S43" s="68"/>
+    </row>
+    <row r="44" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="66">
         <v>42736</v>
       </c>
@@ -44114,8 +44218,9 @@
       <c r="P44" s="68"/>
       <c r="Q44" s="68"/>
       <c r="R44" s="68"/>
-    </row>
-    <row r="45" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S44" s="68"/>
+    </row>
+    <row r="45" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="66">
         <v>42736</v>
       </c>
@@ -44146,8 +44251,9 @@
       <c r="P45" s="68"/>
       <c r="Q45" s="68"/>
       <c r="R45" s="68"/>
-    </row>
-    <row r="46" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S45" s="68"/>
+    </row>
+    <row r="46" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="60">
         <v>42736</v>
       </c>
@@ -44178,8 +44284,9 @@
       <c r="P46" s="68"/>
       <c r="Q46" s="68"/>
       <c r="R46" s="68"/>
-    </row>
-    <row r="47" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S46" s="68"/>
+    </row>
+    <row r="47" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="60">
         <v>42736</v>
       </c>
@@ -44210,8 +44317,9 @@
       <c r="P47" s="68"/>
       <c r="Q47" s="68"/>
       <c r="R47" s="68"/>
-    </row>
-    <row r="48" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S47" s="68"/>
+    </row>
+    <row r="48" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="60">
         <v>42736</v>
       </c>
@@ -44244,8 +44352,9 @@
       <c r="P48" s="68"/>
       <c r="Q48" s="68"/>
       <c r="R48" s="68"/>
-    </row>
-    <row r="49" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S48" s="68"/>
+    </row>
+    <row r="49" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="66">
         <v>42736</v>
       </c>
@@ -44278,8 +44387,9 @@
       <c r="P49" s="68"/>
       <c r="Q49" s="68"/>
       <c r="R49" s="68"/>
-    </row>
-    <row r="50" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S49" s="68"/>
+    </row>
+    <row r="50" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="60">
         <v>42736</v>
       </c>
@@ -44310,8 +44420,9 @@
       <c r="P50" s="62"/>
       <c r="Q50" s="62"/>
       <c r="R50" s="62"/>
-    </row>
-    <row r="51" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S50" s="62"/>
+    </row>
+    <row r="51" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="66">
         <v>42736</v>
       </c>
@@ -44342,8 +44453,9 @@
       <c r="P51" s="62"/>
       <c r="Q51" s="62"/>
       <c r="R51" s="62"/>
-    </row>
-    <row r="52" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S51" s="62"/>
+    </row>
+    <row r="52" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="60">
         <v>42736</v>
       </c>
@@ -44374,8 +44486,9 @@
       <c r="P52" s="62"/>
       <c r="Q52" s="62"/>
       <c r="R52" s="62"/>
-    </row>
-    <row r="53" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S52" s="62"/>
+    </row>
+    <row r="53" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="60">
         <v>42736</v>
       </c>
@@ -44406,8 +44519,9 @@
       <c r="P53" s="68"/>
       <c r="Q53" s="68"/>
       <c r="R53" s="68"/>
-    </row>
-    <row r="54" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S53" s="68"/>
+    </row>
+    <row r="54" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="60">
         <v>42736</v>
       </c>
@@ -44440,8 +44554,9 @@
       <c r="P54" s="62"/>
       <c r="Q54" s="62"/>
       <c r="R54" s="62"/>
-    </row>
-    <row r="55" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S54" s="62"/>
+    </row>
+    <row r="55" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="66">
         <v>42736</v>
       </c>
@@ -44474,8 +44589,9 @@
       <c r="P55" s="62"/>
       <c r="Q55" s="62"/>
       <c r="R55" s="62"/>
-    </row>
-    <row r="56" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S55" s="62"/>
+    </row>
+    <row r="56" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="66">
         <v>42736</v>
       </c>
@@ -44506,8 +44622,9 @@
       <c r="P56" s="68"/>
       <c r="Q56" s="68"/>
       <c r="R56" s="68"/>
-    </row>
-    <row r="57" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S56" s="68"/>
+    </row>
+    <row r="57" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="66">
         <v>42736</v>
       </c>
@@ -44540,8 +44657,9 @@
       <c r="P57" s="68"/>
       <c r="Q57" s="68"/>
       <c r="R57" s="68"/>
-    </row>
-    <row r="58" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S57" s="68"/>
+    </row>
+    <row r="58" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="66">
         <v>42736</v>
       </c>
@@ -44572,8 +44690,9 @@
       <c r="P58" s="68"/>
       <c r="Q58" s="68"/>
       <c r="R58" s="68"/>
-    </row>
-    <row r="59" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S58" s="68"/>
+    </row>
+    <row r="59" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="66">
         <v>42736</v>
       </c>
@@ -44604,8 +44723,9 @@
       <c r="P59" s="68"/>
       <c r="Q59" s="68"/>
       <c r="R59" s="68"/>
-    </row>
-    <row r="60" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S59" s="68"/>
+    </row>
+    <row r="60" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="66">
         <v>42736</v>
       </c>
@@ -44636,8 +44756,9 @@
       <c r="P60" s="68"/>
       <c r="Q60" s="68"/>
       <c r="R60" s="68"/>
-    </row>
-    <row r="61" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S60" s="68"/>
+    </row>
+    <row r="61" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="66">
         <v>42736</v>
       </c>
@@ -44668,8 +44789,9 @@
       <c r="P61" s="68"/>
       <c r="Q61" s="68"/>
       <c r="R61" s="68"/>
-    </row>
-    <row r="62" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S61" s="68"/>
+    </row>
+    <row r="62" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="66">
         <v>42736</v>
       </c>
@@ -44702,8 +44824,9 @@
       <c r="P62" s="68"/>
       <c r="Q62" s="68"/>
       <c r="R62" s="68"/>
-    </row>
-    <row r="63" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S62" s="68"/>
+    </row>
+    <row r="63" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="66">
         <v>42736</v>
       </c>
@@ -44734,8 +44857,9 @@
       <c r="P63" s="68"/>
       <c r="Q63" s="68"/>
       <c r="R63" s="68"/>
-    </row>
-    <row r="64" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S63" s="68"/>
+    </row>
+    <row r="64" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="66">
         <v>42736</v>
       </c>
@@ -44766,8 +44890,9 @@
       <c r="P64" s="68"/>
       <c r="Q64" s="68"/>
       <c r="R64" s="68"/>
-    </row>
-    <row r="65" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S64" s="68"/>
+    </row>
+    <row r="65" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="66">
         <v>42736</v>
       </c>
@@ -44798,8 +44923,9 @@
       <c r="P65" s="68"/>
       <c r="Q65" s="68"/>
       <c r="R65" s="68"/>
-    </row>
-    <row r="66" spans="1:18" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S65" s="68"/>
+    </row>
+    <row r="66" spans="1:19" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="71">
         <v>42736</v>
       </c>
@@ -44830,8 +44956,9 @@
       <c r="P66" s="68"/>
       <c r="Q66" s="68"/>
       <c r="R66" s="68"/>
-    </row>
-    <row r="67" spans="1:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S66" s="68"/>
+    </row>
+    <row r="67" spans="1:19" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="71">
         <v>42737</v>
       </c>
@@ -44866,8 +44993,9 @@
       <c r="P67" s="68"/>
       <c r="Q67" s="68"/>
       <c r="R67" s="68"/>
-    </row>
-    <row r="68" spans="1:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S67" s="62"/>
+    </row>
+    <row r="68" spans="1:19" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="71">
         <v>42738</v>
       </c>
@@ -44902,8 +45030,9 @@
       <c r="P68" s="68"/>
       <c r="Q68" s="68"/>
       <c r="R68" s="68"/>
-    </row>
-    <row r="69" spans="1:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S68" s="62"/>
+    </row>
+    <row r="69" spans="1:19" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="71">
         <v>42739</v>
       </c>
@@ -44936,8 +45065,9 @@
       <c r="P69" s="68"/>
       <c r="Q69" s="68"/>
       <c r="R69" s="68"/>
-    </row>
-    <row r="70" spans="1:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S69" s="62"/>
+    </row>
+    <row r="70" spans="1:19" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="71">
         <v>42740</v>
       </c>
@@ -44970,8 +45100,9 @@
       <c r="P70" s="68"/>
       <c r="Q70" s="68"/>
       <c r="R70" s="68"/>
-    </row>
-    <row r="71" spans="1:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S70" s="62"/>
+    </row>
+    <row r="71" spans="1:19" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="71">
         <v>42741</v>
       </c>
@@ -45004,8 +45135,9 @@
       <c r="P71" s="68"/>
       <c r="Q71" s="68"/>
       <c r="R71" s="68"/>
-    </row>
-    <row r="72" spans="1:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S71" s="62"/>
+    </row>
+    <row r="72" spans="1:19" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="71">
         <v>42741</v>
       </c>
@@ -45040,8 +45172,9 @@
       <c r="P72" s="68"/>
       <c r="Q72" s="68"/>
       <c r="R72" s="68"/>
-    </row>
-    <row r="73" spans="1:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S72" s="62"/>
+    </row>
+    <row r="73" spans="1:19" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="71">
         <v>42742</v>
       </c>
@@ -45076,8 +45209,9 @@
       <c r="P73" s="68"/>
       <c r="Q73" s="68"/>
       <c r="R73" s="68"/>
-    </row>
-    <row r="74" spans="1:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S73" s="62"/>
+    </row>
+    <row r="74" spans="1:19" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="71">
         <v>42743</v>
       </c>
@@ -45110,8 +45244,9 @@
       <c r="P74" s="68"/>
       <c r="Q74" s="68"/>
       <c r="R74" s="68"/>
-    </row>
-    <row r="75" spans="1:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S74" s="62"/>
+    </row>
+    <row r="75" spans="1:19" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="71">
         <v>42744</v>
       </c>
@@ -45144,8 +45279,9 @@
       <c r="P75" s="68"/>
       <c r="Q75" s="68"/>
       <c r="R75" s="68"/>
-    </row>
-    <row r="76" spans="1:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S75" s="62"/>
+    </row>
+    <row r="76" spans="1:19" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="71">
         <v>42745</v>
       </c>
@@ -45176,8 +45312,9 @@
       <c r="P76" s="86"/>
       <c r="Q76" s="86"/>
       <c r="R76" s="86"/>
-    </row>
-    <row r="77" spans="1:18" s="434" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S76" s="265"/>
+    </row>
+    <row r="77" spans="1:19" s="434" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="436">
         <v>42745</v>
       </c>
@@ -45204,7 +45341,7 @@
       <c r="Q77" s="439"/>
       <c r="R77" s="439"/>
     </row>
-    <row r="78" spans="1:18" s="434" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:19" s="434" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="436">
         <v>42745</v>
       </c>

</xml_diff>

<commit_message>
RDM-9033: Updated excel file according to case link
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1DEC7E-748D-4B42-84FB-87FF4A5BDEFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5EEA19-02DA-C047-82D4-F1C7C79883C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="9" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5861" uniqueCount="974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5913" uniqueCount="974">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -12515,7 +12515,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:L68" totalsRowShown="0" headerRowDxfId="216" dataDxfId="214" headerRowBorderDxfId="215" tableBorderDxfId="213" totalsRowBorderDxfId="212">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:L78" totalsRowShown="0" headerRowDxfId="216" dataDxfId="214" headerRowBorderDxfId="215" tableBorderDxfId="213" totalsRowBorderDxfId="212">
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="211"/>
     <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="210"/>
@@ -30156,7 +30156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
@@ -46611,10 +46611,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -48131,21 +48131,19 @@
         <v>935</v>
       </c>
       <c r="D53" s="396" t="s">
-        <v>941</v>
+        <v>392</v>
       </c>
       <c r="E53" s="397" t="s">
         <v>937</v>
       </c>
       <c r="F53" s="398" t="s">
-        <v>913</v>
-      </c>
-      <c r="G53" s="398" t="s">
-        <v>693</v>
-      </c>
+        <v>915</v>
+      </c>
+      <c r="G53" s="398"/>
       <c r="H53" s="398"/>
       <c r="I53" s="395"/>
       <c r="J53" s="395">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K53" s="398" t="s">
         <v>375</v>
@@ -48161,19 +48159,19 @@
         <v>935</v>
       </c>
       <c r="D54" s="396" t="s">
-        <v>941</v>
+        <v>392</v>
       </c>
       <c r="E54" s="397" t="s">
         <v>937</v>
       </c>
       <c r="F54" s="398" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="G54" s="398"/>
       <c r="H54" s="398"/>
       <c r="I54" s="395"/>
       <c r="J54" s="395">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K54" s="398" t="s">
         <v>375</v>
@@ -48189,19 +48187,21 @@
         <v>935</v>
       </c>
       <c r="D55" s="396" t="s">
-        <v>941</v>
+        <v>392</v>
       </c>
       <c r="E55" s="397" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F55" s="398" t="s">
-        <v>915</v>
-      </c>
-      <c r="G55" s="398"/>
+        <v>913</v>
+      </c>
+      <c r="G55" s="398" t="s">
+        <v>685</v>
+      </c>
       <c r="H55" s="398"/>
       <c r="I55" s="395"/>
       <c r="J55" s="395">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K55" s="398" t="s">
         <v>375</v>
@@ -48217,19 +48217,19 @@
         <v>935</v>
       </c>
       <c r="D56" s="396" t="s">
-        <v>941</v>
+        <v>392</v>
       </c>
       <c r="E56" s="397" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F56" s="398" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="G56" s="398"/>
       <c r="H56" s="398"/>
       <c r="I56" s="395"/>
       <c r="J56" s="395">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K56" s="398" t="s">
         <v>375</v>
@@ -48245,21 +48245,19 @@
         <v>935</v>
       </c>
       <c r="D57" s="396" t="s">
-        <v>941</v>
+        <v>392</v>
       </c>
       <c r="E57" s="397" t="s">
         <v>938</v>
       </c>
       <c r="F57" s="398" t="s">
-        <v>913</v>
-      </c>
-      <c r="G57" s="398" t="s">
-        <v>685</v>
-      </c>
+        <v>915</v>
+      </c>
+      <c r="G57" s="398"/>
       <c r="H57" s="398"/>
       <c r="I57" s="395"/>
       <c r="J57" s="395">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K57" s="398" t="s">
         <v>375</v>
@@ -48275,308 +48273,594 @@
         <v>935</v>
       </c>
       <c r="D58" s="396" t="s">
-        <v>941</v>
+        <v>392</v>
       </c>
       <c r="E58" s="397" t="s">
         <v>938</v>
       </c>
       <c r="F58" s="398" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="G58" s="398"/>
       <c r="H58" s="398"/>
       <c r="I58" s="395"/>
       <c r="J58" s="395">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K58" s="398" t="s">
         <v>375</v>
       </c>
       <c r="L58" s="399"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A59" s="237">
+    <row r="59" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="394">
+        <v>43983</v>
+      </c>
+      <c r="B59" s="395"/>
+      <c r="C59" s="396" t="s">
+        <v>935</v>
+      </c>
+      <c r="D59" s="396" t="s">
+        <v>392</v>
+      </c>
+      <c r="E59" s="397" t="s">
+        <v>938</v>
+      </c>
+      <c r="F59" s="398" t="s">
+        <v>913</v>
+      </c>
+      <c r="G59" s="398" t="s">
+        <v>693</v>
+      </c>
+      <c r="H59" s="398"/>
+      <c r="I59" s="395"/>
+      <c r="J59" s="395">
+        <v>9</v>
+      </c>
+      <c r="K59" s="398" t="s">
+        <v>375</v>
+      </c>
+      <c r="L59" s="399"/>
+    </row>
+    <row r="60" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="394">
+        <v>43983</v>
+      </c>
+      <c r="B60" s="395"/>
+      <c r="C60" s="396" t="s">
+        <v>935</v>
+      </c>
+      <c r="D60" s="396" t="s">
+        <v>392</v>
+      </c>
+      <c r="E60" s="397" t="s">
+        <v>938</v>
+      </c>
+      <c r="F60" s="398" t="s">
+        <v>914</v>
+      </c>
+      <c r="G60" s="398"/>
+      <c r="H60" s="398"/>
+      <c r="I60" s="395"/>
+      <c r="J60" s="395">
+        <v>10</v>
+      </c>
+      <c r="K60" s="398" t="s">
+        <v>375</v>
+      </c>
+      <c r="L60" s="399"/>
+    </row>
+    <row r="61" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="394">
+        <v>43983</v>
+      </c>
+      <c r="B61" s="395"/>
+      <c r="C61" s="396" t="s">
+        <v>935</v>
+      </c>
+      <c r="D61" s="396" t="s">
+        <v>941</v>
+      </c>
+      <c r="E61" s="397" t="s">
+        <v>937</v>
+      </c>
+      <c r="F61" s="398" t="s">
+        <v>915</v>
+      </c>
+      <c r="G61" s="398"/>
+      <c r="H61" s="398"/>
+      <c r="I61" s="395"/>
+      <c r="J61" s="395">
+        <v>3</v>
+      </c>
+      <c r="K61" s="398" t="s">
+        <v>375</v>
+      </c>
+      <c r="L61" s="399"/>
+    </row>
+    <row r="62" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="394">
+        <v>43983</v>
+      </c>
+      <c r="B62" s="395"/>
+      <c r="C62" s="396" t="s">
+        <v>935</v>
+      </c>
+      <c r="D62" s="396" t="s">
+        <v>941</v>
+      </c>
+      <c r="E62" s="397" t="s">
+        <v>937</v>
+      </c>
+      <c r="F62" s="398" t="s">
+        <v>916</v>
+      </c>
+      <c r="G62" s="398"/>
+      <c r="H62" s="398"/>
+      <c r="I62" s="395"/>
+      <c r="J62" s="395">
+        <v>4</v>
+      </c>
+      <c r="K62" s="398" t="s">
+        <v>375</v>
+      </c>
+      <c r="L62" s="399"/>
+    </row>
+    <row r="63" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="394">
+        <v>43983</v>
+      </c>
+      <c r="B63" s="395"/>
+      <c r="C63" s="396" t="s">
+        <v>935</v>
+      </c>
+      <c r="D63" s="396" t="s">
+        <v>941</v>
+      </c>
+      <c r="E63" s="397" t="s">
+        <v>937</v>
+      </c>
+      <c r="F63" s="398" t="s">
+        <v>913</v>
+      </c>
+      <c r="G63" s="398" t="s">
+        <v>693</v>
+      </c>
+      <c r="H63" s="398"/>
+      <c r="I63" s="395"/>
+      <c r="J63" s="395">
+        <v>5</v>
+      </c>
+      <c r="K63" s="398" t="s">
+        <v>375</v>
+      </c>
+      <c r="L63" s="399"/>
+    </row>
+    <row r="64" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="394">
+        <v>43983</v>
+      </c>
+      <c r="B64" s="395"/>
+      <c r="C64" s="396" t="s">
+        <v>935</v>
+      </c>
+      <c r="D64" s="396" t="s">
+        <v>941</v>
+      </c>
+      <c r="E64" s="397" t="s">
+        <v>937</v>
+      </c>
+      <c r="F64" s="398" t="s">
+        <v>914</v>
+      </c>
+      <c r="G64" s="398"/>
+      <c r="H64" s="398"/>
+      <c r="I64" s="395"/>
+      <c r="J64" s="395">
+        <v>6</v>
+      </c>
+      <c r="K64" s="398" t="s">
+        <v>375</v>
+      </c>
+      <c r="L64" s="399"/>
+    </row>
+    <row r="65" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="394">
+        <v>43983</v>
+      </c>
+      <c r="B65" s="395"/>
+      <c r="C65" s="396" t="s">
+        <v>935</v>
+      </c>
+      <c r="D65" s="396" t="s">
+        <v>941</v>
+      </c>
+      <c r="E65" s="397" t="s">
+        <v>938</v>
+      </c>
+      <c r="F65" s="398" t="s">
+        <v>915</v>
+      </c>
+      <c r="G65" s="398"/>
+      <c r="H65" s="398"/>
+      <c r="I65" s="395"/>
+      <c r="J65" s="395">
+        <v>7</v>
+      </c>
+      <c r="K65" s="398" t="s">
+        <v>375</v>
+      </c>
+      <c r="L65" s="399"/>
+    </row>
+    <row r="66" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="394">
+        <v>43983</v>
+      </c>
+      <c r="B66" s="395"/>
+      <c r="C66" s="396" t="s">
+        <v>935</v>
+      </c>
+      <c r="D66" s="396" t="s">
+        <v>941</v>
+      </c>
+      <c r="E66" s="397" t="s">
+        <v>938</v>
+      </c>
+      <c r="F66" s="398" t="s">
+        <v>916</v>
+      </c>
+      <c r="G66" s="398"/>
+      <c r="H66" s="398"/>
+      <c r="I66" s="395"/>
+      <c r="J66" s="395">
+        <v>8</v>
+      </c>
+      <c r="K66" s="398" t="s">
+        <v>375</v>
+      </c>
+      <c r="L66" s="399"/>
+    </row>
+    <row r="67" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="394">
+        <v>43983</v>
+      </c>
+      <c r="B67" s="395"/>
+      <c r="C67" s="396" t="s">
+        <v>935</v>
+      </c>
+      <c r="D67" s="396" t="s">
+        <v>941</v>
+      </c>
+      <c r="E67" s="397" t="s">
+        <v>938</v>
+      </c>
+      <c r="F67" s="398" t="s">
+        <v>913</v>
+      </c>
+      <c r="G67" s="398" t="s">
+        <v>685</v>
+      </c>
+      <c r="H67" s="398"/>
+      <c r="I67" s="395"/>
+      <c r="J67" s="395">
+        <v>9</v>
+      </c>
+      <c r="K67" s="398" t="s">
+        <v>375</v>
+      </c>
+      <c r="L67" s="399"/>
+    </row>
+    <row r="68" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="394">
+        <v>43983</v>
+      </c>
+      <c r="B68" s="395"/>
+      <c r="C68" s="396" t="s">
+        <v>935</v>
+      </c>
+      <c r="D68" s="396" t="s">
+        <v>941</v>
+      </c>
+      <c r="E68" s="397" t="s">
+        <v>938</v>
+      </c>
+      <c r="F68" s="398" t="s">
+        <v>914</v>
+      </c>
+      <c r="G68" s="398"/>
+      <c r="H68" s="398"/>
+      <c r="I68" s="395"/>
+      <c r="J68" s="395">
+        <v>10</v>
+      </c>
+      <c r="K68" s="398" t="s">
+        <v>375</v>
+      </c>
+      <c r="L68" s="399"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A69" s="237">
         <v>43101</v>
       </c>
-      <c r="B59" s="84"/>
-      <c r="C59" s="84" t="s">
+      <c r="B69" s="84"/>
+      <c r="C69" s="84" t="s">
         <v>297</v>
       </c>
-      <c r="D59" s="118" t="s">
+      <c r="D69" s="118" t="s">
         <v>388</v>
       </c>
-      <c r="E59" s="118" t="s">
+      <c r="E69" s="118" t="s">
         <v>124</v>
       </c>
-      <c r="F59" s="118" t="s">
+      <c r="F69" s="118" t="s">
         <v>344</v>
       </c>
-      <c r="G59" s="118"/>
-      <c r="H59" s="84"/>
-      <c r="I59" s="84"/>
-      <c r="J59" s="84">
+      <c r="G69" s="118"/>
+      <c r="H69" s="84"/>
+      <c r="I69" s="84"/>
+      <c r="J69" s="84">
         <v>1</v>
       </c>
-      <c r="K59" s="118" t="s">
+      <c r="K69" s="118" t="s">
         <v>389</v>
       </c>
-      <c r="L59" s="217" t="s">
+      <c r="L69" s="217" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A60" s="237">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A70" s="237">
         <v>43101</v>
       </c>
-      <c r="B60" s="84"/>
-      <c r="C60" s="84" t="s">
+      <c r="B70" s="84"/>
+      <c r="C70" s="84" t="s">
         <v>297</v>
       </c>
-      <c r="D60" s="118" t="s">
+      <c r="D70" s="118" t="s">
         <v>388</v>
       </c>
-      <c r="E60" s="118" t="s">
+      <c r="E70" s="118" t="s">
         <v>124</v>
       </c>
-      <c r="F60" s="118" t="s">
+      <c r="F70" s="118" t="s">
         <v>341</v>
       </c>
-      <c r="G60" s="118"/>
-      <c r="H60" s="84"/>
-      <c r="I60" s="84"/>
-      <c r="J60" s="84">
+      <c r="G70" s="118"/>
+      <c r="H70" s="84"/>
+      <c r="I70" s="84"/>
+      <c r="J70" s="84">
         <v>1</v>
       </c>
-      <c r="K60" s="118" t="s">
+      <c r="K70" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="L60" s="217" t="s">
+      <c r="L70" s="217" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A61" s="237">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A71" s="237">
         <v>43101</v>
       </c>
-      <c r="B61" s="84"/>
-      <c r="C61" s="65" t="s">
+      <c r="B71" s="84"/>
+      <c r="C71" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="D61" s="68" t="s">
+      <c r="D71" s="68" t="s">
         <v>392</v>
       </c>
-      <c r="E61" s="82" t="s">
+      <c r="E71" s="82" t="s">
         <v>212</v>
       </c>
-      <c r="F61" s="118" t="s">
+      <c r="F71" s="118" t="s">
         <v>326</v>
       </c>
-      <c r="G61" s="118"/>
-      <c r="H61" s="84"/>
-      <c r="I61" s="84"/>
-      <c r="J61" s="84">
+      <c r="G71" s="118"/>
+      <c r="H71" s="84"/>
+      <c r="I71" s="84"/>
+      <c r="J71" s="84">
         <v>1</v>
       </c>
-      <c r="K61" s="118" t="s">
+      <c r="K71" s="118" t="s">
         <v>374</v>
       </c>
-      <c r="L61" s="63"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A62" s="237">
+      <c r="L71" s="63"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A72" s="237">
         <v>43101</v>
       </c>
-      <c r="B62" s="84"/>
-      <c r="C62" s="65" t="s">
+      <c r="B72" s="84"/>
+      <c r="C72" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="D62" s="68" t="s">
+      <c r="D72" s="68" t="s">
         <v>392</v>
       </c>
-      <c r="E62" s="82" t="s">
+      <c r="E72" s="82" t="s">
         <v>212</v>
       </c>
-      <c r="F62" s="118" t="s">
+      <c r="F72" s="118" t="s">
         <v>328</v>
       </c>
-      <c r="G62" s="118"/>
-      <c r="H62" s="84"/>
-      <c r="I62" s="84"/>
-      <c r="J62" s="84">
+      <c r="G72" s="118"/>
+      <c r="H72" s="84"/>
+      <c r="I72" s="84"/>
+      <c r="J72" s="84">
         <v>1</v>
       </c>
-      <c r="K62" s="118" t="s">
+      <c r="K72" s="118" t="s">
         <v>374</v>
       </c>
-      <c r="L62" s="63"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A63" s="237">
+      <c r="L72" s="63"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A73" s="237">
         <v>43101</v>
       </c>
-      <c r="B63" s="84"/>
-      <c r="C63" s="68" t="s">
+      <c r="B73" s="84"/>
+      <c r="C73" s="68" t="s">
         <v>218</v>
       </c>
-      <c r="D63" s="68" t="s">
+      <c r="D73" s="68" t="s">
         <v>392</v>
       </c>
-      <c r="E63" s="82" t="s">
+      <c r="E73" s="82" t="s">
         <v>216</v>
       </c>
-      <c r="F63" s="118" t="s">
+      <c r="F73" s="118" t="s">
         <v>330</v>
       </c>
-      <c r="G63" s="118"/>
-      <c r="H63" s="84"/>
-      <c r="I63" s="84"/>
-      <c r="J63" s="84">
+      <c r="G73" s="118"/>
+      <c r="H73" s="84"/>
+      <c r="I73" s="84"/>
+      <c r="J73" s="84">
         <v>2</v>
       </c>
-      <c r="K63" s="118" t="s">
+      <c r="K73" s="118" t="s">
         <v>374</v>
       </c>
-      <c r="L63" s="63"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A64" s="237">
+      <c r="L73" s="63"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A74" s="237">
         <v>43101</v>
       </c>
-      <c r="B64" s="84"/>
-      <c r="C64" s="65" t="s">
+      <c r="B74" s="84"/>
+      <c r="C74" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="D64" s="68" t="s">
+      <c r="D74" s="68" t="s">
         <v>393</v>
       </c>
-      <c r="E64" s="82" t="s">
+      <c r="E74" s="82" t="s">
         <v>212</v>
       </c>
-      <c r="F64" s="118" t="s">
+      <c r="F74" s="118" t="s">
         <v>326</v>
       </c>
-      <c r="G64" s="118"/>
-      <c r="H64" s="84"/>
-      <c r="I64" s="84"/>
-      <c r="J64" s="84">
+      <c r="G74" s="118"/>
+      <c r="H74" s="84"/>
+      <c r="I74" s="84"/>
+      <c r="J74" s="84">
         <v>1</v>
       </c>
-      <c r="K64" s="118" t="s">
+      <c r="K74" s="118" t="s">
         <v>374</v>
       </c>
-      <c r="L64" s="63"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A65" s="237">
+      <c r="L74" s="63"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A75" s="237">
         <v>43101</v>
       </c>
-      <c r="B65" s="84"/>
-      <c r="C65" s="65" t="s">
+      <c r="B75" s="84"/>
+      <c r="C75" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="D65" s="68" t="s">
+      <c r="D75" s="68" t="s">
         <v>393</v>
       </c>
-      <c r="E65" s="82" t="s">
+      <c r="E75" s="82" t="s">
         <v>212</v>
       </c>
-      <c r="F65" s="118" t="s">
+      <c r="F75" s="118" t="s">
         <v>328</v>
       </c>
-      <c r="G65" s="118"/>
-      <c r="H65" s="84"/>
-      <c r="I65" s="84"/>
-      <c r="J65" s="84">
+      <c r="G75" s="118"/>
+      <c r="H75" s="84"/>
+      <c r="I75" s="84"/>
+      <c r="J75" s="84">
         <v>1</v>
       </c>
-      <c r="K65" s="118" t="s">
+      <c r="K75" s="118" t="s">
         <v>374</v>
       </c>
-      <c r="L65" s="63"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A66" s="237">
+      <c r="L75" s="63"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A76" s="237">
         <v>43101</v>
       </c>
-      <c r="B66" s="84"/>
-      <c r="C66" s="68" t="s">
+      <c r="B76" s="84"/>
+      <c r="C76" s="68" t="s">
         <v>218</v>
       </c>
-      <c r="D66" s="68" t="s">
+      <c r="D76" s="68" t="s">
         <v>393</v>
       </c>
-      <c r="E66" s="82" t="s">
+      <c r="E76" s="82" t="s">
         <v>216</v>
       </c>
-      <c r="F66" s="118" t="s">
+      <c r="F76" s="118" t="s">
         <v>330</v>
       </c>
-      <c r="G66" s="118"/>
-      <c r="H66" s="84"/>
-      <c r="I66" s="84"/>
-      <c r="J66" s="84">
+      <c r="G76" s="118"/>
+      <c r="H76" s="84"/>
+      <c r="I76" s="84"/>
+      <c r="J76" s="84">
         <v>2</v>
       </c>
-      <c r="K66" s="118" t="s">
+      <c r="K76" s="118" t="s">
         <v>374</v>
       </c>
-      <c r="L66" s="63"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A67" s="237">
+      <c r="L76" s="63"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A77" s="237">
         <v>43101</v>
       </c>
-      <c r="B67" s="84"/>
-      <c r="C67" s="65" t="s">
+      <c r="B77" s="84"/>
+      <c r="C77" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="D67" s="68" t="s">
+      <c r="D77" s="68" t="s">
         <v>394</v>
       </c>
-      <c r="E67" s="82" t="s">
+      <c r="E77" s="82" t="s">
         <v>212</v>
       </c>
-      <c r="F67" s="118" t="s">
+      <c r="F77" s="118" t="s">
         <v>326</v>
       </c>
-      <c r="G67" s="118"/>
-      <c r="H67" s="84"/>
-      <c r="I67" s="84"/>
-      <c r="J67" s="84">
+      <c r="G77" s="118"/>
+      <c r="H77" s="84"/>
+      <c r="I77" s="84"/>
+      <c r="J77" s="84">
         <v>1</v>
       </c>
-      <c r="K67" s="118" t="s">
+      <c r="K77" s="118" t="s">
         <v>374</v>
       </c>
-      <c r="L67" s="63"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A68" s="238">
+      <c r="L77" s="63"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A78" s="238">
         <v>43101</v>
       </c>
-      <c r="B68" s="90"/>
-      <c r="C68" s="73" t="s">
+      <c r="B78" s="90"/>
+      <c r="C78" s="73" t="s">
         <v>214</v>
       </c>
-      <c r="D68" s="86" t="s">
+      <c r="D78" s="86" t="s">
         <v>394</v>
       </c>
-      <c r="E68" s="88" t="s">
+      <c r="E78" s="88" t="s">
         <v>212</v>
       </c>
-      <c r="F68" s="239" t="s">
+      <c r="F78" s="239" t="s">
         <v>328</v>
       </c>
-      <c r="G68" s="239"/>
-      <c r="H68" s="90"/>
-      <c r="I68" s="90"/>
-      <c r="J68" s="90">
+      <c r="G78" s="239"/>
+      <c r="H78" s="90"/>
+      <c r="I78" s="90"/>
+      <c r="J78" s="90">
         <v>1</v>
       </c>
-      <c r="K68" s="239" t="s">
+      <c r="K78" s="239" t="s">
         <v>374</v>
       </c>
-      <c r="L68" s="91"/>
+      <c r="L78" s="91"/>
     </row>
   </sheetData>
   <phoneticPr fontId="58" type="noConversion"/>

</xml_diff>

<commit_message>
RDM-9033: Updated excel and json according to new field
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5EEA19-02DA-C047-82D4-F1C7C79883C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AEEB6A-2665-A940-8E8A-7960C00F9594}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5913" uniqueCount="974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5913" uniqueCount="973">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3013,9 +3013,6 @@
   </si>
   <si>
     <t>Create Collection of Complex Case Links</t>
-  </si>
-  <si>
-    <t>https://run.mocky.io/v3/8f97e310-a289-487c-b2cf-be9616d8780a</t>
   </si>
   <si>
     <t>Searchable</t>
@@ -14827,16 +14824,16 @@
         <v>455</v>
       </c>
       <c r="E30" s="454" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F30" s="465" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="G30" s="466">
         <v>5</v>
       </c>
       <c r="H30" s="467" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="I30" s="468">
         <v>3</v>
@@ -16961,8 +16958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D4" zoomScale="109" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E2" zoomScale="109" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17169,7 +17166,7 @@
         <v>489</v>
       </c>
       <c r="J4" s="113" t="s">
-        <v>959</v>
+        <v>532</v>
       </c>
       <c r="K4" s="114"/>
       <c r="L4" s="114"/>
@@ -18779,7 +18776,6 @@
   <hyperlinks>
     <hyperlink ref="J35" r:id="rId1" xr:uid="{D8CF8637-CA9E-D640-B8A5-0839120ED0E2}"/>
     <hyperlink ref="J36" r:id="rId2" xr:uid="{965A59DF-24BC-0646-830A-59FEE12B238C}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{B1AF49E4-49FA-C84C-94E6-3BBDD6902A47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -18787,7 +18783,7 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -20370,7 +20366,7 @@
         <v>923</v>
       </c>
       <c r="E40" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F40" s="469">
         <v>1</v>
@@ -20487,7 +20483,7 @@
         <v>924</v>
       </c>
       <c r="E43" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F43" s="469">
         <v>1</v>
@@ -30992,7 +30988,7 @@
         <v>922</v>
       </c>
       <c r="D46" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E46" s="455" t="s">
         <v>776</v>
@@ -36018,7 +36014,7 @@
         <v>806</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
@@ -38698,14 +38694,14 @@
         <v>922</v>
       </c>
       <c r="D45" s="454" t="s">
+        <v>960</v>
+      </c>
+      <c r="E45" s="454" t="s">
         <v>961</v>
-      </c>
-      <c r="E45" s="454" t="s">
-        <v>962</v>
       </c>
       <c r="F45" s="455"/>
       <c r="G45" s="454" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="H45" s="453"/>
       <c r="I45" s="454"/>
@@ -43185,7 +43181,7 @@
         <v>817</v>
       </c>
       <c r="S3" s="450" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -46613,7 +46609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
@@ -47404,10 +47400,10 @@
         <v>923</v>
       </c>
       <c r="E27" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F27" s="462" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="G27" s="462"/>
       <c r="H27" s="460"/>
@@ -47432,10 +47428,10 @@
         <v>923</v>
       </c>
       <c r="E28" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F28" s="462" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="G28" s="462"/>
       <c r="H28" s="460"/>
@@ -47460,10 +47456,10 @@
         <v>923</v>
       </c>
       <c r="E29" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F29" s="462" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="G29" s="462"/>
       <c r="H29" s="460"/>
@@ -47488,10 +47484,10 @@
         <v>923</v>
       </c>
       <c r="E30" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F30" s="462" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="G30" s="462"/>
       <c r="H30" s="460"/>
@@ -47516,10 +47512,10 @@
         <v>923</v>
       </c>
       <c r="E31" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F31" s="462" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="G31" s="462"/>
       <c r="H31" s="460"/>
@@ -47544,10 +47540,10 @@
         <v>923</v>
       </c>
       <c r="E32" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F32" s="462" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="G32" s="462"/>
       <c r="H32" s="460"/>
@@ -47572,10 +47568,10 @@
         <v>923</v>
       </c>
       <c r="E33" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F33" s="462" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="G33" s="462"/>
       <c r="H33" s="460"/>
@@ -47600,10 +47596,10 @@
         <v>923</v>
       </c>
       <c r="E34" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F34" s="462" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="G34" s="462"/>
       <c r="H34" s="460"/>
@@ -47628,10 +47624,10 @@
         <v>923</v>
       </c>
       <c r="E35" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F35" s="462" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="G35" s="462"/>
       <c r="H35" s="460"/>
@@ -47656,10 +47652,10 @@
         <v>923</v>
       </c>
       <c r="E36" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F36" s="462" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="G36" s="462"/>
       <c r="H36" s="460"/>
@@ -47854,10 +47850,10 @@
         <v>924</v>
       </c>
       <c r="E43" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F43" s="462" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="G43" s="462"/>
       <c r="H43" s="460"/>
@@ -47882,10 +47878,10 @@
         <v>924</v>
       </c>
       <c r="E44" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F44" s="462" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="G44" s="462"/>
       <c r="H44" s="460"/>
@@ -47910,10 +47906,10 @@
         <v>924</v>
       </c>
       <c r="E45" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F45" s="462" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="G45" s="462"/>
       <c r="H45" s="460"/>
@@ -47938,10 +47934,10 @@
         <v>924</v>
       </c>
       <c r="E46" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F46" s="462" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="G46" s="462"/>
       <c r="H46" s="460"/>
@@ -47966,10 +47962,10 @@
         <v>924</v>
       </c>
       <c r="E47" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F47" s="462" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="G47" s="462"/>
       <c r="H47" s="460"/>
@@ -47994,10 +47990,10 @@
         <v>924</v>
       </c>
       <c r="E48" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F48" s="462" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="G48" s="462"/>
       <c r="H48" s="460"/>
@@ -48022,10 +48018,10 @@
         <v>924</v>
       </c>
       <c r="E49" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F49" s="462" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="G49" s="462"/>
       <c r="H49" s="460"/>
@@ -48050,10 +48046,10 @@
         <v>924</v>
       </c>
       <c r="E50" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F50" s="462" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="G50" s="462"/>
       <c r="H50" s="460"/>
@@ -48078,10 +48074,10 @@
         <v>924</v>
       </c>
       <c r="E51" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F51" s="462" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="G51" s="462"/>
       <c r="H51" s="460"/>
@@ -48106,10 +48102,10 @@
         <v>924</v>
       </c>
       <c r="E52" s="454" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F52" s="462" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="G52" s="462"/>
       <c r="H52" s="460"/>

</xml_diff>

<commit_message>
RDM-9338: Introduce NoC config tab
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,38 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AEEB6A-2665-A940-8E8A-7960C00F9594}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2104E141-5AE7-484D-A181-2608F16BE3CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="33600" windowHeight="19340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
     <sheet name="Banner" sheetId="22" r:id="rId2"/>
     <sheet name="CaseType" sheetId="2" r:id="rId3"/>
-    <sheet name="Category" sheetId="23" r:id="rId4"/>
-    <sheet name="CaseField" sheetId="3" r:id="rId5"/>
-    <sheet name="ComplexTypes" sheetId="4" r:id="rId6"/>
-    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId7"/>
-    <sheet name="EventToComplexTypes" sheetId="20" r:id="rId8"/>
-    <sheet name="FixedLists" sheetId="5" r:id="rId9"/>
-    <sheet name="CaseTypeTab" sheetId="6" r:id="rId10"/>
-    <sheet name="State" sheetId="7" r:id="rId11"/>
-    <sheet name="CaseEvent" sheetId="8" r:id="rId12"/>
-    <sheet name="CaseEventToFields" sheetId="9" r:id="rId13"/>
-    <sheet name="SearchInputFields" sheetId="10" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="11" r:id="rId15"/>
-    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId16"/>
-    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId20"/>
-    <sheet name="CaseRoles" sheetId="19" r:id="rId21"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId22"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId23"/>
+    <sheet name="NoCConfig" sheetId="24" r:id="rId4"/>
+    <sheet name="Category" sheetId="23" r:id="rId5"/>
+    <sheet name="CaseField" sheetId="3" r:id="rId6"/>
+    <sheet name="ComplexTypes" sheetId="4" r:id="rId7"/>
+    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId8"/>
+    <sheet name="EventToComplexTypes" sheetId="20" r:id="rId9"/>
+    <sheet name="FixedLists" sheetId="5" r:id="rId10"/>
+    <sheet name="CaseTypeTab" sheetId="6" r:id="rId11"/>
+    <sheet name="State" sheetId="7" r:id="rId12"/>
+    <sheet name="CaseEvent" sheetId="8" r:id="rId13"/>
+    <sheet name="CaseEventToFields" sheetId="9" r:id="rId14"/>
+    <sheet name="SearchInputFields" sheetId="10" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="11" r:id="rId16"/>
+    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId18"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId19"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId20"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId21"/>
+    <sheet name="CaseRoles" sheetId="19" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">CaseEvent!$A$22:$T$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CaseField!$A$3:$IO$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">CaseEvent!$A$22:$T$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseField!$A$3:$IO$119</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5913" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5923" uniqueCount="979">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3055,6 +3056,24 @@
   </si>
   <si>
     <t>NotesReason</t>
+  </si>
+  <si>
+    <t>NoCConfig</t>
+  </si>
+  <si>
+    <t>CaseTypeId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes or No, to enable or disable the reason field.                     </t>
+  </si>
+  <si>
+    <t>Yes or No, to enable or disable the noc action interpretaion</t>
+  </si>
+  <si>
+    <t>ReasonRequired</t>
+  </si>
+  <si>
+    <t>NoCActionInterpretationRequired</t>
   </si>
 </sst>
 </file>
@@ -3467,11 +3486,13 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -3768,7 +3789,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="472">
+  <cellXfs count="481">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -5003,6 +5024,29 @@
     <xf numFmtId="49" fontId="0" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="51" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="52" fillId="17" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="51" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="52" fillId="17" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -5020,7 +5064,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal 2 3" xfId="13" xr:uid="{983C50BB-8B6C-1941-95CA-614B186AEA1E}"/>
   </cellStyles>
-  <dxfs count="304">
+  <dxfs count="312">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -11302,6 +11346,220 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -12192,19 +12450,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="303" dataDxfId="301" headerRowBorderDxfId="302" tableBorderDxfId="300" totalsRowBorderDxfId="299">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="311" dataDxfId="309" headerRowBorderDxfId="310" tableBorderDxfId="308" totalsRowBorderDxfId="307">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="298"/>
-    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="297"/>
-    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="296"/>
-    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="295"/>
-    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="294"/>
+    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="306"/>
+    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="305"/>
+    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="304"/>
+    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="303"/>
+    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="302"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L67" totalsRowShown="0" headerRowDxfId="187" dataDxfId="185" headerRowBorderDxfId="186" tableBorderDxfId="184" totalsRowBorderDxfId="183">
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="182"/>
+    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="181"/>
+    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="180"/>
+    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="179"/>
+    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="178"/>
+    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="177"/>
+    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="176"/>
+    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="175"/>
+    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="174"/>
+    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="173"/>
+    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="172"/>
+    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="171"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H28" totalsRowShown="0" headerRowDxfId="170" dataDxfId="168" headerRowBorderDxfId="169" tableBorderDxfId="167" totalsRowBorderDxfId="166">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="165"/>
@@ -12220,7 +12498,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:T40" totalsRowShown="0" headerRowDxfId="157" dataDxfId="155" headerRowBorderDxfId="156" tableBorderDxfId="154" totalsRowBorderDxfId="153">
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="152"/>
@@ -12248,7 +12526,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:Q161" totalsRowShown="0" headerRowDxfId="132" dataDxfId="130" headerRowBorderDxfId="131" tableBorderDxfId="129" totalsRowBorderDxfId="128">
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="127"/>
@@ -12273,7 +12551,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H43" totalsRowShown="0" headerRowDxfId="110" dataDxfId="108" headerRowBorderDxfId="109" tableBorderDxfId="107" totalsRowBorderDxfId="106">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="105"/>
@@ -12289,7 +12567,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:G35" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96" tableBorderDxfId="94" totalsRowBorderDxfId="93">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="92"/>
@@ -12304,7 +12582,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H48" totalsRowShown="0" headerRowDxfId="85" dataDxfId="83" headerRowBorderDxfId="84" tableBorderDxfId="82" totalsRowBorderDxfId="81">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="80"/>
@@ -12320,7 +12598,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I53" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="67"/>
@@ -12337,7 +12615,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="53"/>
@@ -12351,7 +12629,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E21" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
@@ -12364,7 +12642,19 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="301" dataDxfId="299" headerRowBorderDxfId="300" tableBorderDxfId="298" totalsRowBorderDxfId="297">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="296"/>
+    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="295"/>
+    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="294"/>
+    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="293" dataCellStyle="Hyperlink"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F154" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="33"/>
@@ -12378,19 +12668,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="293" dataDxfId="291" headerRowBorderDxfId="292" tableBorderDxfId="290" totalsRowBorderDxfId="289">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="288"/>
-    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="287"/>
-    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="286"/>
-    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="285" dataCellStyle="Hyperlink"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="23"/>
@@ -12402,7 +12680,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F50" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
@@ -12416,7 +12694,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F36" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
@@ -12431,24 +12709,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I17" totalsRowShown="0" headerRowDxfId="284" dataDxfId="282" headerRowBorderDxfId="283" tableBorderDxfId="281" totalsRowBorderDxfId="280">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I17" totalsRowShown="0" headerRowDxfId="292" dataDxfId="290" headerRowBorderDxfId="291" tableBorderDxfId="289" totalsRowBorderDxfId="288">
   <autoFilter ref="A3:I17" xr:uid="{C0075E79-5DBE-654F-827E-CA137EF61FB4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="279"/>
-    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="278"/>
-    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="277"/>
-    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="276"/>
-    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="275"/>
-    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="274"/>
-    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="273"/>
-    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="272"/>
-    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="271"/>
+    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="287"/>
+    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="286"/>
+    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="285"/>
+    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="284"/>
+    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="283"/>
+    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="282"/>
+    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="281"/>
+    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="280"/>
+    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="279"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{F70D0623-0A9A-6C4C-9874-9A93D5DC3ACF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="278" dataDxfId="276" headerRowBorderDxfId="277" tableBorderDxfId="275" totalsRowBorderDxfId="274">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{24BEC596-8705-9C49-940B-FCCC2F2EB305}" name="CaseTypeId" dataDxfId="273"/>
+    <tableColumn id="2" xr3:uid="{C8273B71-59AA-7D4D-B60F-85A96E9E15D7}" name="ReasonRequired" dataDxfId="272"/>
+    <tableColumn id="4" xr3:uid="{4A0A9C2B-6C96-574F-BCC8-ACBC4B9E5EA7}" name="NoCActionInterpretationRequired" dataDxfId="271" dataCellStyle="Hyperlink"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:M132" totalsRowShown="0" headerRowDxfId="270" dataDxfId="268" headerRowBorderDxfId="269" tableBorderDxfId="267" totalsRowBorderDxfId="266">
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="265"/>
@@ -12469,7 +12758,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:S76" totalsRowShown="0" headerRowDxfId="252" dataDxfId="250" headerRowBorderDxfId="251" tableBorderDxfId="249" totalsRowBorderDxfId="248">
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="247"/>
@@ -12496,7 +12785,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G41" totalsRowShown="0" headerRowDxfId="228" dataDxfId="226" headerRowBorderDxfId="227" tableBorderDxfId="225" totalsRowBorderDxfId="224" headerRowCellStyle="Normal 2 3">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="223"/>
@@ -12511,7 +12800,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:L78" totalsRowShown="0" headerRowDxfId="216" dataDxfId="214" headerRowBorderDxfId="215" tableBorderDxfId="213" totalsRowBorderDxfId="212">
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="211"/>
@@ -12531,7 +12820,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G24" totalsRowShown="0" headerRowDxfId="199" dataDxfId="197" headerRowBorderDxfId="198" tableBorderDxfId="196" totalsRowBorderDxfId="195">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="194"/>
@@ -12541,26 +12830,6 @@
     <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="190"/>
     <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="189"/>
     <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="188"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L67" totalsRowShown="0" headerRowDxfId="187" dataDxfId="185" headerRowBorderDxfId="186" tableBorderDxfId="184" totalsRowBorderDxfId="183">
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="182"/>
-    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="181"/>
-    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="180"/>
-    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="179"/>
-    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="178"/>
-    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="177"/>
-    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="176"/>
-    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="175"/>
-    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="174"/>
-    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="173"/>
-    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="172"/>
-    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="171"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13734,6 +14003,533 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="4" customWidth="1"/>
+    <col min="3" max="4" width="31.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="4" customWidth="1"/>
+    <col min="8" max="252" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>395</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" ht="35.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>396</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>397</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>398</v>
+      </c>
+      <c r="F2" s="29"/>
+      <c r="G2" s="56"/>
+    </row>
+    <row r="3" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>399</v>
+      </c>
+      <c r="F3" s="110" t="s">
+        <v>739</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="61"/>
+      <c r="C4" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>401</v>
+      </c>
+      <c r="E4" s="62" t="s">
+        <v>402</v>
+      </c>
+      <c r="F4" s="115"/>
+      <c r="G4" s="63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>403</v>
+      </c>
+      <c r="E5" s="62" t="s">
+        <v>404</v>
+      </c>
+      <c r="F5" s="115"/>
+      <c r="G5" s="63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="61"/>
+      <c r="C6" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>405</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>406</v>
+      </c>
+      <c r="F6" s="115"/>
+      <c r="G6" s="63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="61"/>
+      <c r="C7" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>407</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>408</v>
+      </c>
+      <c r="F7" s="115"/>
+      <c r="G7" s="63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="61"/>
+      <c r="C8" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>409</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>410</v>
+      </c>
+      <c r="F8" s="115"/>
+      <c r="G8" s="63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="61"/>
+      <c r="C9" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>411</v>
+      </c>
+      <c r="E9" s="62" t="s">
+        <v>412</v>
+      </c>
+      <c r="F9" s="115"/>
+      <c r="G9" s="63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="61"/>
+      <c r="C10" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>413</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>414</v>
+      </c>
+      <c r="F10" s="115"/>
+      <c r="G10" s="63"/>
+    </row>
+    <row r="11" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="61"/>
+      <c r="C11" s="62" t="s">
+        <v>260</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>415</v>
+      </c>
+      <c r="E11" s="62" t="s">
+        <v>416</v>
+      </c>
+      <c r="F11" s="115"/>
+      <c r="G11" s="64"/>
+    </row>
+    <row r="12" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="61"/>
+      <c r="C12" s="62" t="s">
+        <v>260</v>
+      </c>
+      <c r="D12" s="62" t="s">
+        <v>417</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>418</v>
+      </c>
+      <c r="F12" s="115"/>
+      <c r="G12" s="64"/>
+    </row>
+    <row r="13" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="61"/>
+      <c r="C13" s="62" t="s">
+        <v>260</v>
+      </c>
+      <c r="D13" s="62" t="s">
+        <v>419</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>420</v>
+      </c>
+      <c r="F13" s="115"/>
+      <c r="G13" s="63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="61"/>
+      <c r="C14" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>421</v>
+      </c>
+      <c r="E14" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="F14" s="277"/>
+      <c r="G14" s="64"/>
+    </row>
+    <row r="15" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="61"/>
+      <c r="C15" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>423</v>
+      </c>
+      <c r="E15" s="65" t="s">
+        <v>424</v>
+      </c>
+      <c r="F15" s="277"/>
+      <c r="G15" s="64"/>
+    </row>
+    <row r="16" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="67"/>
+      <c r="C16" s="68" t="s">
+        <v>305</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>425</v>
+      </c>
+      <c r="E16" s="68" t="s">
+        <v>426</v>
+      </c>
+      <c r="F16" s="119"/>
+      <c r="G16" s="63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="68" t="s">
+        <v>305</v>
+      </c>
+      <c r="D17" s="68" t="s">
+        <v>427</v>
+      </c>
+      <c r="E17" s="68" t="s">
+        <v>428</v>
+      </c>
+      <c r="F17" s="119"/>
+      <c r="G17" s="63"/>
+    </row>
+    <row r="18" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="67"/>
+      <c r="C18" s="68" t="s">
+        <v>305</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>429</v>
+      </c>
+      <c r="E18" s="68" t="s">
+        <v>430</v>
+      </c>
+      <c r="F18" s="119"/>
+      <c r="G18" s="63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B19" s="67"/>
+      <c r="C19" s="68" t="s">
+        <v>286</v>
+      </c>
+      <c r="D19" s="68" t="s">
+        <v>431</v>
+      </c>
+      <c r="E19" s="68" t="s">
+        <v>432</v>
+      </c>
+      <c r="F19" s="119"/>
+      <c r="G19" s="63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="67"/>
+      <c r="C20" s="68" t="s">
+        <v>286</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>433</v>
+      </c>
+      <c r="E20" s="68" t="s">
+        <v>434</v>
+      </c>
+      <c r="F20" s="119"/>
+      <c r="G20" s="63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="67"/>
+      <c r="C21" s="68" t="s">
+        <v>286</v>
+      </c>
+      <c r="D21" s="68" t="s">
+        <v>435</v>
+      </c>
+      <c r="E21" s="68" t="s">
+        <v>436</v>
+      </c>
+      <c r="F21" s="119"/>
+      <c r="G21" s="63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B22" s="67"/>
+      <c r="C22" s="68" t="s">
+        <v>286</v>
+      </c>
+      <c r="D22" s="68" t="s">
+        <v>437</v>
+      </c>
+      <c r="E22" s="68" t="s">
+        <v>438</v>
+      </c>
+      <c r="F22" s="119"/>
+      <c r="G22" s="63">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69" t="s">
+        <v>720</v>
+      </c>
+      <c r="D23" s="65" t="s">
+        <v>721</v>
+      </c>
+      <c r="E23" s="65" t="s">
+        <v>722</v>
+      </c>
+      <c r="F23" s="277"/>
+      <c r="G23" s="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72" t="s">
+        <v>720</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>724</v>
+      </c>
+      <c r="E24" s="73" t="s">
+        <v>723</v>
+      </c>
+      <c r="F24" s="278"/>
+      <c r="G24" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B25" s="61"/>
+      <c r="C25" s="65" t="s">
+        <v>765</v>
+      </c>
+      <c r="D25" s="65" t="s">
+        <v>766</v>
+      </c>
+      <c r="E25" s="65" t="s">
+        <v>750</v>
+      </c>
+      <c r="F25" s="277" t="s">
+        <v>749</v>
+      </c>
+      <c r="G25" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="284" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="279">
+        <v>42736</v>
+      </c>
+      <c r="B26" s="280"/>
+      <c r="C26" s="285" t="s">
+        <v>765</v>
+      </c>
+      <c r="D26" s="281" t="s">
+        <v>767</v>
+      </c>
+      <c r="E26" s="281" t="s">
+        <v>768</v>
+      </c>
+      <c r="F26" s="282" t="s">
+        <v>771</v>
+      </c>
+      <c r="G26" s="283">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="G27" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:CR67"/>
   <sheetViews>
@@ -16113,7 +16909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:FH30"/>
   <sheetViews>
@@ -16954,11 +17750,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E2" zoomScale="109" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="E2" zoomScale="109" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -18788,7 +19584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q171"/>
   <sheetViews>
@@ -25210,7 +26006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
@@ -26228,7 +27024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:DS35"/>
   <sheetViews>
@@ -27215,7 +28011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
@@ -28253,7 +29049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:BL53"/>
   <sheetViews>
@@ -29547,7 +30343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -29675,355 +30471,6 @@
   </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="30.83203125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="13" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" style="13" customWidth="1"/>
-    <col min="6" max="256" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="191" t="s">
-        <v>682</v>
-      </c>
-      <c r="B1" s="192" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="193" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="194" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="76"/>
-    </row>
-    <row r="2" spans="1:5" ht="46.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="180" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="180" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="180" t="s">
-        <v>683</v>
-      </c>
-      <c r="D2" s="180" t="s">
-        <v>335</v>
-      </c>
-      <c r="E2" s="180" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>338</v>
-      </c>
-      <c r="E3" s="110" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="62" t="s">
-        <v>882</v>
-      </c>
-      <c r="D4" s="134" t="s">
-        <v>776</v>
-      </c>
-      <c r="E4" s="115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="62" t="s">
-        <v>882</v>
-      </c>
-      <c r="D5" s="81" t="s">
-        <v>685</v>
-      </c>
-      <c r="E5" s="115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="62" t="s">
-        <v>882</v>
-      </c>
-      <c r="D6" s="134" t="s">
-        <v>936</v>
-      </c>
-      <c r="E6" s="115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="62" t="s">
-        <v>880</v>
-      </c>
-      <c r="D7" s="134" t="s">
-        <v>776</v>
-      </c>
-      <c r="E7" s="115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="292" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="286">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="289"/>
-      <c r="C8" s="352" t="s">
-        <v>922</v>
-      </c>
-      <c r="D8" s="366" t="s">
-        <v>776</v>
-      </c>
-      <c r="E8" s="294" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="81"/>
-      <c r="C9" s="189" t="s">
-        <v>883</v>
-      </c>
-      <c r="D9" s="134" t="s">
-        <v>776</v>
-      </c>
-      <c r="E9" s="115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="189" t="s">
-        <v>884</v>
-      </c>
-      <c r="D10" s="134" t="s">
-        <v>776</v>
-      </c>
-      <c r="E10" s="115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="62" t="s">
-        <v>885</v>
-      </c>
-      <c r="D11" s="134" t="s">
-        <v>776</v>
-      </c>
-      <c r="E11" s="115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="81"/>
-      <c r="C12" s="62" t="s">
-        <v>886</v>
-      </c>
-      <c r="D12" s="134" t="s">
-        <v>776</v>
-      </c>
-      <c r="E12" s="115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B13" s="81"/>
-      <c r="C13" s="62" t="s">
-        <v>887</v>
-      </c>
-      <c r="D13" s="134" t="s">
-        <v>776</v>
-      </c>
-      <c r="E13" s="115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B14" s="81"/>
-      <c r="C14" s="62" t="s">
-        <v>888</v>
-      </c>
-      <c r="D14" s="134" t="s">
-        <v>776</v>
-      </c>
-      <c r="E14" s="115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="84"/>
-      <c r="C15" s="65" t="s">
-        <v>889</v>
-      </c>
-      <c r="D15" s="134" t="s">
-        <v>776</v>
-      </c>
-      <c r="E15" s="119" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="84"/>
-      <c r="C16" s="68" t="s">
-        <v>892</v>
-      </c>
-      <c r="D16" s="84" t="s">
-        <v>777</v>
-      </c>
-      <c r="E16" s="119" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B17" s="84"/>
-      <c r="C17" s="68" t="s">
-        <v>892</v>
-      </c>
-      <c r="D17" s="84" t="s">
-        <v>778</v>
-      </c>
-      <c r="E17" s="119" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="71">
-        <v>42736</v>
-      </c>
-      <c r="B18" s="90"/>
-      <c r="C18" s="86" t="s">
-        <v>890</v>
-      </c>
-      <c r="D18" s="195" t="s">
-        <v>776</v>
-      </c>
-      <c r="E18" s="125" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="71">
-        <v>42736</v>
-      </c>
-      <c r="B19" s="90"/>
-      <c r="C19" s="86" t="s">
-        <v>891</v>
-      </c>
-      <c r="D19" s="195" t="s">
-        <v>776</v>
-      </c>
-      <c r="E19" s="125" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="286">
-        <v>42736</v>
-      </c>
-      <c r="B20" s="289"/>
-      <c r="C20" s="352" t="s">
-        <v>881</v>
-      </c>
-      <c r="D20" s="366" t="s">
-        <v>776</v>
-      </c>
-      <c r="E20" s="294" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="71">
-        <v>42736</v>
-      </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="265" t="s">
-        <v>882</v>
-      </c>
-      <c r="D21" s="429" t="s">
-        <v>943</v>
-      </c>
-      <c r="E21" s="125" t="s">
-        <v>339</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -30149,6 +30596,355 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="13" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" style="13" customWidth="1"/>
+    <col min="6" max="256" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="191" t="s">
+        <v>682</v>
+      </c>
+      <c r="B1" s="192" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="193" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="194" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="76"/>
+    </row>
+    <row r="2" spans="1:5" ht="46.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="180" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="180" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="180" t="s">
+        <v>683</v>
+      </c>
+      <c r="D2" s="180" t="s">
+        <v>335</v>
+      </c>
+      <c r="E2" s="180" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3" s="110" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="81"/>
+      <c r="C4" s="62" t="s">
+        <v>882</v>
+      </c>
+      <c r="D4" s="134" t="s">
+        <v>776</v>
+      </c>
+      <c r="E4" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="81"/>
+      <c r="C5" s="62" t="s">
+        <v>882</v>
+      </c>
+      <c r="D5" s="81" t="s">
+        <v>685</v>
+      </c>
+      <c r="E5" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="81"/>
+      <c r="C6" s="62" t="s">
+        <v>882</v>
+      </c>
+      <c r="D6" s="134" t="s">
+        <v>936</v>
+      </c>
+      <c r="E6" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="81"/>
+      <c r="C7" s="62" t="s">
+        <v>880</v>
+      </c>
+      <c r="D7" s="134" t="s">
+        <v>776</v>
+      </c>
+      <c r="E7" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="292" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="286">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="289"/>
+      <c r="C8" s="352" t="s">
+        <v>922</v>
+      </c>
+      <c r="D8" s="366" t="s">
+        <v>776</v>
+      </c>
+      <c r="E8" s="294" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="81"/>
+      <c r="C9" s="189" t="s">
+        <v>883</v>
+      </c>
+      <c r="D9" s="134" t="s">
+        <v>776</v>
+      </c>
+      <c r="E9" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="81"/>
+      <c r="C10" s="189" t="s">
+        <v>884</v>
+      </c>
+      <c r="D10" s="134" t="s">
+        <v>776</v>
+      </c>
+      <c r="E10" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="81"/>
+      <c r="C11" s="62" t="s">
+        <v>885</v>
+      </c>
+      <c r="D11" s="134" t="s">
+        <v>776</v>
+      </c>
+      <c r="E11" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="81"/>
+      <c r="C12" s="62" t="s">
+        <v>886</v>
+      </c>
+      <c r="D12" s="134" t="s">
+        <v>776</v>
+      </c>
+      <c r="E12" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="81"/>
+      <c r="C13" s="62" t="s">
+        <v>887</v>
+      </c>
+      <c r="D13" s="134" t="s">
+        <v>776</v>
+      </c>
+      <c r="E13" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="62" t="s">
+        <v>888</v>
+      </c>
+      <c r="D14" s="134" t="s">
+        <v>776</v>
+      </c>
+      <c r="E14" s="115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="84"/>
+      <c r="C15" s="65" t="s">
+        <v>889</v>
+      </c>
+      <c r="D15" s="134" t="s">
+        <v>776</v>
+      </c>
+      <c r="E15" s="119" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="84"/>
+      <c r="C16" s="68" t="s">
+        <v>892</v>
+      </c>
+      <c r="D16" s="84" t="s">
+        <v>777</v>
+      </c>
+      <c r="E16" s="119" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="84"/>
+      <c r="C17" s="68" t="s">
+        <v>892</v>
+      </c>
+      <c r="D17" s="84" t="s">
+        <v>778</v>
+      </c>
+      <c r="E17" s="119" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="90"/>
+      <c r="C18" s="86" t="s">
+        <v>890</v>
+      </c>
+      <c r="D18" s="195" t="s">
+        <v>776</v>
+      </c>
+      <c r="E18" s="125" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B19" s="90"/>
+      <c r="C19" s="86" t="s">
+        <v>891</v>
+      </c>
+      <c r="D19" s="195" t="s">
+        <v>776</v>
+      </c>
+      <c r="E19" s="125" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="286">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="289"/>
+      <c r="C20" s="352" t="s">
+        <v>881</v>
+      </c>
+      <c r="D20" s="366" t="s">
+        <v>776</v>
+      </c>
+      <c r="E20" s="294" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="72"/>
+      <c r="C21" s="265" t="s">
+        <v>882</v>
+      </c>
+      <c r="D21" s="429" t="s">
+        <v>943</v>
+      </c>
+      <c r="E21" s="125" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F154"/>
   <sheetViews>
@@ -32954,7 +33750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -33101,7 +33897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:EK50"/>
   <sheetViews>
@@ -34303,7 +35099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:CF36"/>
   <sheetViews>
@@ -35144,7 +35940,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -35627,6 +36423,84 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235B542E-F9DA-F649-9998-3A7EA6C2B3CB}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="472" t="s">
+        <v>973</v>
+      </c>
+      <c r="B1" s="473"/>
+      <c r="C1" s="473"/>
+    </row>
+    <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A2" s="33" t="s">
+        <v>974</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>975</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A3" s="474" t="s">
+        <v>974</v>
+      </c>
+      <c r="B3" s="475" t="s">
+        <v>977</v>
+      </c>
+      <c r="C3" s="476" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A4" s="477" t="s">
+        <v>922</v>
+      </c>
+      <c r="B4" s="477" t="s">
+        <v>534</v>
+      </c>
+      <c r="C4" s="478" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A5" s="477"/>
+      <c r="B5" s="477"/>
+      <c r="C5" s="478"/>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A6" s="477"/>
+      <c r="B6" s="479"/>
+      <c r="C6" s="480"/>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A7" s="477"/>
+      <c r="B7" s="477"/>
+      <c r="C7" s="478"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E15BE1-896E-C94F-B2CD-122BE5CAB0E3}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -35876,7 +36750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IO132"/>
   <sheetViews>
@@ -43029,7 +43903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S78"/>
   <sheetViews>
@@ -45724,7 +46598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2A25AD-5D69-564D-9511-0323740C2E1F}">
   <dimension ref="A1:G41"/>
   <sheetViews>
@@ -46605,7 +47479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L78"/>
   <sheetViews>
@@ -48866,531 +49740,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="15.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="4" customWidth="1"/>
-    <col min="3" max="4" width="31.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="4" customWidth="1"/>
-    <col min="8" max="252" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>395</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:7" ht="35.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>396</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>397</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>398</v>
-      </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="56"/>
-    </row>
-    <row r="3" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>225</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>399</v>
-      </c>
-      <c r="F3" s="110" t="s">
-        <v>739</v>
-      </c>
-      <c r="G3" s="59" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>401</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>402</v>
-      </c>
-      <c r="F4" s="115"/>
-      <c r="G4" s="63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="62" t="s">
-        <v>403</v>
-      </c>
-      <c r="E5" s="62" t="s">
-        <v>404</v>
-      </c>
-      <c r="F5" s="115"/>
-      <c r="G5" s="63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="62" t="s">
-        <v>405</v>
-      </c>
-      <c r="E6" s="62" t="s">
-        <v>406</v>
-      </c>
-      <c r="F6" s="115"/>
-      <c r="G6" s="63">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="62" t="s">
-        <v>407</v>
-      </c>
-      <c r="E7" s="62" t="s">
-        <v>408</v>
-      </c>
-      <c r="F7" s="115"/>
-      <c r="G7" s="63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="62" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="62" t="s">
-        <v>409</v>
-      </c>
-      <c r="E8" s="62" t="s">
-        <v>410</v>
-      </c>
-      <c r="F8" s="115"/>
-      <c r="G8" s="63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="62" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="62" t="s">
-        <v>411</v>
-      </c>
-      <c r="E9" s="62" t="s">
-        <v>412</v>
-      </c>
-      <c r="F9" s="115"/>
-      <c r="G9" s="63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="62" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="62" t="s">
-        <v>413</v>
-      </c>
-      <c r="E10" s="62" t="s">
-        <v>414</v>
-      </c>
-      <c r="F10" s="115"/>
-      <c r="G10" s="63"/>
-    </row>
-    <row r="11" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="62" t="s">
-        <v>260</v>
-      </c>
-      <c r="D11" s="62" t="s">
-        <v>415</v>
-      </c>
-      <c r="E11" s="62" t="s">
-        <v>416</v>
-      </c>
-      <c r="F11" s="115"/>
-      <c r="G11" s="64"/>
-    </row>
-    <row r="12" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="62" t="s">
-        <v>260</v>
-      </c>
-      <c r="D12" s="62" t="s">
-        <v>417</v>
-      </c>
-      <c r="E12" s="62" t="s">
-        <v>418</v>
-      </c>
-      <c r="F12" s="115"/>
-      <c r="G12" s="64"/>
-    </row>
-    <row r="13" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="62" t="s">
-        <v>260</v>
-      </c>
-      <c r="D13" s="62" t="s">
-        <v>419</v>
-      </c>
-      <c r="E13" s="62" t="s">
-        <v>420</v>
-      </c>
-      <c r="F13" s="115"/>
-      <c r="G13" s="63">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="D14" s="65" t="s">
-        <v>421</v>
-      </c>
-      <c r="E14" s="65" t="s">
-        <v>422</v>
-      </c>
-      <c r="F14" s="277"/>
-      <c r="G14" s="64"/>
-    </row>
-    <row r="15" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>423</v>
-      </c>
-      <c r="E15" s="65" t="s">
-        <v>424</v>
-      </c>
-      <c r="F15" s="277"/>
-      <c r="G15" s="64"/>
-    </row>
-    <row r="16" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="67"/>
-      <c r="C16" s="68" t="s">
-        <v>305</v>
-      </c>
-      <c r="D16" s="68" t="s">
-        <v>425</v>
-      </c>
-      <c r="E16" s="68" t="s">
-        <v>426</v>
-      </c>
-      <c r="F16" s="119"/>
-      <c r="G16" s="63">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="68" t="s">
-        <v>305</v>
-      </c>
-      <c r="D17" s="68" t="s">
-        <v>427</v>
-      </c>
-      <c r="E17" s="68" t="s">
-        <v>428</v>
-      </c>
-      <c r="F17" s="119"/>
-      <c r="G17" s="63"/>
-    </row>
-    <row r="18" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68" t="s">
-        <v>305</v>
-      </c>
-      <c r="D18" s="68" t="s">
-        <v>429</v>
-      </c>
-      <c r="E18" s="68" t="s">
-        <v>430</v>
-      </c>
-      <c r="F18" s="119"/>
-      <c r="G18" s="63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="68" t="s">
-        <v>286</v>
-      </c>
-      <c r="D19" s="68" t="s">
-        <v>431</v>
-      </c>
-      <c r="E19" s="68" t="s">
-        <v>432</v>
-      </c>
-      <c r="F19" s="119"/>
-      <c r="G19" s="63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="68" t="s">
-        <v>286</v>
-      </c>
-      <c r="D20" s="68" t="s">
-        <v>433</v>
-      </c>
-      <c r="E20" s="68" t="s">
-        <v>434</v>
-      </c>
-      <c r="F20" s="119"/>
-      <c r="G20" s="63">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B21" s="67"/>
-      <c r="C21" s="68" t="s">
-        <v>286</v>
-      </c>
-      <c r="D21" s="68" t="s">
-        <v>435</v>
-      </c>
-      <c r="E21" s="68" t="s">
-        <v>436</v>
-      </c>
-      <c r="F21" s="119"/>
-      <c r="G21" s="63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="68" t="s">
-        <v>286</v>
-      </c>
-      <c r="D22" s="68" t="s">
-        <v>437</v>
-      </c>
-      <c r="E22" s="68" t="s">
-        <v>438</v>
-      </c>
-      <c r="F22" s="119"/>
-      <c r="G22" s="63">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69" t="s">
-        <v>720</v>
-      </c>
-      <c r="D23" s="65" t="s">
-        <v>721</v>
-      </c>
-      <c r="E23" s="65" t="s">
-        <v>722</v>
-      </c>
-      <c r="F23" s="277"/>
-      <c r="G23" s="70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="71">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72" t="s">
-        <v>720</v>
-      </c>
-      <c r="D24" s="73" t="s">
-        <v>724</v>
-      </c>
-      <c r="E24" s="73" t="s">
-        <v>723</v>
-      </c>
-      <c r="F24" s="278"/>
-      <c r="G24" s="74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B25" s="61"/>
-      <c r="C25" s="65" t="s">
-        <v>765</v>
-      </c>
-      <c r="D25" s="65" t="s">
-        <v>766</v>
-      </c>
-      <c r="E25" s="65" t="s">
-        <v>750</v>
-      </c>
-      <c r="F25" s="277" t="s">
-        <v>749</v>
-      </c>
-      <c r="G25" s="64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="284" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="279">
-        <v>42736</v>
-      </c>
-      <c r="B26" s="280"/>
-      <c r="C26" s="285" t="s">
-        <v>765</v>
-      </c>
-      <c r="D26" s="281" t="s">
-        <v>767</v>
-      </c>
-      <c r="E26" s="281" t="s">
-        <v>768</v>
-      </c>
-      <c r="F26" s="282" t="s">
-        <v>771</v>
-      </c>
-      <c r="G26" s="283">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="G27" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
RDM-9338: renamed tab from NoCConfig to NoticeOfChangeConfig
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2104E141-5AE7-484D-A181-2608F16BE3CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8184DE-B2E3-384C-B852-F406B8E08710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="460" windowWidth="33600" windowHeight="19340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
     <sheet name="Banner" sheetId="22" r:id="rId2"/>
     <sheet name="CaseType" sheetId="2" r:id="rId3"/>
-    <sheet name="NoCConfig" sheetId="24" r:id="rId4"/>
+    <sheet name="NoticeOfChangeConfig" sheetId="24" r:id="rId4"/>
     <sheet name="Category" sheetId="23" r:id="rId5"/>
     <sheet name="CaseField" sheetId="3" r:id="rId6"/>
     <sheet name="ComplexTypes" sheetId="4" r:id="rId7"/>
@@ -3058,9 +3058,6 @@
     <t>NotesReason</t>
   </si>
   <si>
-    <t>NoCConfig</t>
-  </si>
-  <si>
     <t>CaseTypeId</t>
   </si>
   <si>
@@ -3074,6 +3071,9 @@
   </si>
   <si>
     <t>NoCActionInterpretationRequired</t>
+  </si>
+  <si>
+    <t>NoticeOfChangeConfig</t>
   </si>
 </sst>
 </file>
@@ -36427,7 +36427,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -36439,31 +36439,31 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="472" t="s">
-        <v>973</v>
+        <v>978</v>
       </c>
       <c r="B1" s="473"/>
       <c r="C1" s="473"/>
     </row>
     <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
+        <v>973</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>974</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="C2" s="33" t="s">
         <v>975</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A3" s="474" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B3" s="475" t="s">
+        <v>976</v>
+      </c>
+      <c r="C3" s="476" t="s">
         <v>977</v>
-      </c>
-      <c r="C3" s="476" t="s">
-        <v>978</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
fix failing def file
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1510E04C-B713-7D47-BA96-A09803256488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF45DF8-DB8B-6F49-9003-5E9494DA3370}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -5081,31 +5081,6 @@
   </cellStyles>
   <dxfs count="313">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -8014,6 +7989,31 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -12581,103 +12581,103 @@
     <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="119"/>
     <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="118"/>
     <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="117"/>
-    <tableColumn id="18" xr3:uid="{E135335A-D7E2-F744-932E-E0627D2DBFE1}" name="RetainHiddenValue" dataDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="116"/>
-    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="115"/>
-    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="114"/>
-    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="113"/>
-    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="112"/>
+    <tableColumn id="18" xr3:uid="{E135335A-D7E2-F744-932E-E0627D2DBFE1}" name="RetainHiddenValue" dataDxfId="116"/>
+    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="115"/>
+    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="114"/>
+    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="113"/>
+    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="112"/>
+    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H43" totalsRowShown="0" headerRowDxfId="111" dataDxfId="109" headerRowBorderDxfId="110" tableBorderDxfId="108" totalsRowBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H43" totalsRowShown="0" headerRowDxfId="110" dataDxfId="108" headerRowBorderDxfId="109" tableBorderDxfId="107" totalsRowBorderDxfId="106">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="103"/>
-    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="102"/>
-    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="101"/>
-    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="100"/>
-    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="99"/>
+    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="101"/>
+    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="100"/>
+    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:G35" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:G35" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96" tableBorderDxfId="94" totalsRowBorderDxfId="93">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="88"/>
-    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="87"/>
+    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="87"/>
+    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H48" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83" totalsRowBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H48" totalsRowShown="0" headerRowDxfId="85" dataDxfId="83" headerRowBorderDxfId="84" tableBorderDxfId="82" totalsRowBorderDxfId="81">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="75"/>
-    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I53" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I53" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="62"/>
-    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="61"/>
-    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="61"/>
+    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E21" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E21" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12696,54 +12696,54 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F154" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F154" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="23" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="22" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F50" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F36" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F36" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -19630,7 +19630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R171"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E13" zoomScale="88" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C126" zoomScale="88" workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
@@ -44118,8 +44118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D51" workbookViewId="0">
+      <selection activeCell="M77" sqref="M77:M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -46853,7 +46853,7 @@
         <v>951</v>
       </c>
       <c r="K77" s="438"/>
-      <c r="L77" s="438" t="s">
+      <c r="M77" s="438" t="s">
         <v>783</v>
       </c>
       <c r="O77" s="439"/>
@@ -46880,7 +46880,7 @@
         <v>952</v>
       </c>
       <c r="K78" s="438"/>
-      <c r="L78" s="438" t="s">
+      <c r="M78" s="438" t="s">
         <v>783</v>
       </c>
       <c r="O78" s="439"/>

</xml_diff>

<commit_message>
updates and add challenge question tab
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A0B9E3-FD11-E043-AF9E-D9404BD76E1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCE7CFA-DB1B-AA41-82A1-E014FE4C5D85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19980" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,30 +18,34 @@
     <sheet name="CaseType" sheetId="2" r:id="rId3"/>
     <sheet name="NoticeOfChangeConfig" sheetId="24" r:id="rId4"/>
     <sheet name="Category" sheetId="23" r:id="rId5"/>
-    <sheet name="ChallengeQuestion" sheetId="25" r:id="rId6"/>
-    <sheet name="CaseField" sheetId="3" r:id="rId7"/>
-    <sheet name="ComplexTypes" sheetId="4" r:id="rId8"/>
-    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId9"/>
-    <sheet name="EventToComplexTypes" sheetId="20" r:id="rId10"/>
-    <sheet name="FixedLists" sheetId="5" r:id="rId11"/>
-    <sheet name="CaseTypeTab" sheetId="6" r:id="rId12"/>
-    <sheet name="State" sheetId="7" r:id="rId13"/>
-    <sheet name="CaseEvent" sheetId="8" r:id="rId14"/>
-    <sheet name="CaseEventToFields" sheetId="9" r:id="rId15"/>
-    <sheet name="SearchInputFields" sheetId="10" r:id="rId16"/>
-    <sheet name="SearchResultFields" sheetId="11" r:id="rId17"/>
-    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId18"/>
-    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId19"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId20"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId21"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId22"/>
-    <sheet name="CaseRoles" sheetId="19" r:id="rId23"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId24"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId25"/>
+    <sheet name="SearchCasesResultFields" sheetId="26" r:id="rId6"/>
+    <sheet name="ChallengeQuestion" sheetId="25" r:id="rId7"/>
+    <sheet name="CaseField" sheetId="3" r:id="rId8"/>
+    <sheet name="ComplexTypes" sheetId="4" r:id="rId9"/>
+    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId10"/>
+    <sheet name="EventToComplexTypes" sheetId="20" r:id="rId11"/>
+    <sheet name="FixedLists" sheetId="5" r:id="rId12"/>
+    <sheet name="CaseTypeTab" sheetId="6" r:id="rId13"/>
+    <sheet name="State" sheetId="7" r:id="rId14"/>
+    <sheet name="CaseEvent" sheetId="8" r:id="rId15"/>
+    <sheet name="CaseEventToFields" sheetId="9" r:id="rId16"/>
+    <sheet name="SearchInputFields" sheetId="10" r:id="rId17"/>
+    <sheet name="SearchResultFields" sheetId="11" r:id="rId18"/>
+    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId19"/>
+    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId20"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId21"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId22"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId23"/>
+    <sheet name="CaseRoles" sheetId="19" r:id="rId24"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId25"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId26"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId27"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">CaseEvent!$A$22:$T$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseField!$A$3:$IO$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">CaseEvent!$A$22:$T$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseField!$A$3:$IO$119</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -62,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5993" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6018" uniqueCount="1015">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3163,6 +3167,27 @@
   </si>
   <si>
     <t>NoCChallengeG2Q1</t>
+  </si>
+  <si>
+    <t>orgcases</t>
+  </si>
+  <si>
+    <t>`CaseReference` orgcases</t>
+  </si>
+  <si>
+    <t>`Email` orgcases</t>
+  </si>
+  <si>
+    <t>1:ASC</t>
+  </si>
+  <si>
+    <t>`Text` orgcases</t>
+  </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
+    <t>SearchCasesResultFields</t>
   </si>
 </sst>
 </file>
@@ -3175,7 +3200,7 @@
     <numFmt numFmtId="166" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="72" x14ac:knownFonts="1">
+  <fonts count="74" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -3629,6 +3654,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="20">
     <fill>
@@ -3746,7 +3784,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -3913,8 +3951,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3930,8 +3983,9 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="498">
+  <cellXfs count="505">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -5220,8 +5274,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="34" fillId="19" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="15"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="14" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="15" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="Explanatory Text" xfId="14" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -5237,6 +5298,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal 2 3" xfId="13" xr:uid="{983C50BB-8B6C-1941-95CA-614B186AEA1E}"/>
+    <cellStyle name="Normal 3" xfId="15" xr:uid="{740B127F-765C-6B48-8069-14FF6FB13A4B}"/>
   </cellStyles>
   <dxfs count="313">
     <dxf>
@@ -12646,6 +12708,59 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Jurisdiction"/>
+      <sheetName val="CaseType"/>
+      <sheetName val="CaseField"/>
+      <sheetName val="FixedLists"/>
+      <sheetName val="ComplexTypes"/>
+      <sheetName val="State"/>
+      <sheetName val="CaseEvent"/>
+      <sheetName val="CaseEventToFields"/>
+      <sheetName val="SearchInputFields"/>
+      <sheetName val="SearchCasesResultFields"/>
+      <sheetName val="SearchResultFields"/>
+      <sheetName val="WorkBasketInputFields"/>
+      <sheetName val="WorkBasketResultFields"/>
+      <sheetName val="CaseTypeTab"/>
+      <sheetName val="UserProfile"/>
+      <sheetName val="AuthorisationCaseType"/>
+      <sheetName val="AuthorisationCaseState"/>
+      <sheetName val="AuthorisationCaseEvent"/>
+      <sheetName val="AuthorisationCaseField"/>
+      <sheetName val="AuthorisationComplexType"/>
+      <sheetName val="SearchAlias"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14204,6 +14319,887 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2A25AD-5D69-564D-9511-0323740C2E1F}">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5" customWidth="1"/>
+    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="49" t="s">
+        <v>332</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+    </row>
+    <row r="2" spans="1:7" ht="126" x14ac:dyDescent="0.15">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="55" t="s">
+        <v>333</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>335</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="250" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="251" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="251" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="251" t="s">
+        <v>337</v>
+      </c>
+      <c r="E3" s="251" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="251" t="s">
+        <v>338</v>
+      </c>
+      <c r="G3" s="252" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="196"/>
+      <c r="C4" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D4" s="196" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>257</v>
+      </c>
+      <c r="F4" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G4" s="244" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="196"/>
+      <c r="C5" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D5" s="196" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="65" t="s">
+        <v>259</v>
+      </c>
+      <c r="F5" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G5" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="196"/>
+      <c r="C6" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D6" s="196" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G6" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="196"/>
+      <c r="C7" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D7" s="196" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="65" t="s">
+        <v>264</v>
+      </c>
+      <c r="F7" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G7" s="244" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="196"/>
+      <c r="C8" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D8" s="196" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G8" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="196"/>
+      <c r="C9" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D9" s="196" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="65" t="s">
+        <v>268</v>
+      </c>
+      <c r="F9" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G9" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="196"/>
+      <c r="C10" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D10" s="196" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="65" t="s">
+        <v>270</v>
+      </c>
+      <c r="F10" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G10" s="244" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="196"/>
+      <c r="C11" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D11" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="197" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G11" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="196"/>
+      <c r="C12" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D12" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="197" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G12" s="244" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="196"/>
+      <c r="C13" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D13" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="197" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G13" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="196"/>
+      <c r="C14" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D14" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="67" t="s">
+        <v>315</v>
+      </c>
+      <c r="F14" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G14" s="245" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="196"/>
+      <c r="C15" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D15" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="197" t="s">
+        <v>313</v>
+      </c>
+      <c r="F15" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G15" s="245" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="196"/>
+      <c r="C16" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D16" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>341</v>
+      </c>
+      <c r="F16" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G16" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="196"/>
+      <c r="C17" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D17" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="65" t="s">
+        <v>342</v>
+      </c>
+      <c r="F17" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G17" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="196"/>
+      <c r="C18" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D18" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>343</v>
+      </c>
+      <c r="F18" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G18" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B19" s="196"/>
+      <c r="C19" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D19" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="82" t="s">
+        <v>344</v>
+      </c>
+      <c r="F19" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G19" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="196"/>
+      <c r="C20" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D20" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="65" t="s">
+        <v>345</v>
+      </c>
+      <c r="F20" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G20" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="196"/>
+      <c r="C21" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D21" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="65" t="s">
+        <v>346</v>
+      </c>
+      <c r="F21" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G21" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B22" s="196"/>
+      <c r="C22" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D22" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="65" t="s">
+        <v>347</v>
+      </c>
+      <c r="F22" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G22" s="245" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B23" s="196"/>
+      <c r="C23" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D23" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="65" t="s">
+        <v>348</v>
+      </c>
+      <c r="F23" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G23" s="245" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="196"/>
+      <c r="C24" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D24" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="65" t="s">
+        <v>349</v>
+      </c>
+      <c r="F24" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G24" s="245" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B25" s="196"/>
+      <c r="C25" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D25" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="65" t="s">
+        <v>350</v>
+      </c>
+      <c r="F25" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G25" s="245" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B26" s="196"/>
+      <c r="C26" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D26" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="65" t="s">
+        <v>351</v>
+      </c>
+      <c r="F26" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G26" s="245" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B27" s="196"/>
+      <c r="C27" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D27" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="65" t="s">
+        <v>273</v>
+      </c>
+      <c r="F27" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G27" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B28" s="196"/>
+      <c r="C28" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D28" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="62" t="s">
+        <v>275</v>
+      </c>
+      <c r="F28" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G28" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B29" s="196"/>
+      <c r="C29" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D29" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="62" t="s">
+        <v>277</v>
+      </c>
+      <c r="F29" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G29" s="245" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="196"/>
+      <c r="C30" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D30" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="62" t="s">
+        <v>279</v>
+      </c>
+      <c r="F30" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G30" s="245" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B31" s="196"/>
+      <c r="C31" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D31" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="65" t="s">
+        <v>119</v>
+      </c>
+      <c r="F31" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G31" s="245" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="243">
+        <v>42736</v>
+      </c>
+      <c r="B32" s="196"/>
+      <c r="C32" s="196" t="s">
+        <v>887</v>
+      </c>
+      <c r="D32" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" s="65" t="s">
+        <v>282</v>
+      </c>
+      <c r="F32" s="84" t="s">
+        <v>776</v>
+      </c>
+      <c r="G32" s="245" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="17" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="246">
+        <v>42736</v>
+      </c>
+      <c r="B33" s="127"/>
+      <c r="C33" s="127" t="s">
+        <v>892</v>
+      </c>
+      <c r="D33" s="132" t="s">
+        <v>212</v>
+      </c>
+      <c r="E33" s="65" t="s">
+        <v>326</v>
+      </c>
+      <c r="F33" s="118" t="s">
+        <v>778</v>
+      </c>
+      <c r="G33" s="119" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="17" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="246">
+        <v>42736</v>
+      </c>
+      <c r="B34" s="127"/>
+      <c r="C34" s="127" t="s">
+        <v>892</v>
+      </c>
+      <c r="D34" s="132" t="s">
+        <v>212</v>
+      </c>
+      <c r="E34" s="65" t="s">
+        <v>326</v>
+      </c>
+      <c r="F34" s="118" t="s">
+        <v>777</v>
+      </c>
+      <c r="G34" s="119" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="17" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="246">
+        <v>42736</v>
+      </c>
+      <c r="B35" s="127"/>
+      <c r="C35" s="214" t="s">
+        <v>892</v>
+      </c>
+      <c r="D35" s="132" t="s">
+        <v>212</v>
+      </c>
+      <c r="E35" s="65" t="s">
+        <v>328</v>
+      </c>
+      <c r="F35" s="84" t="s">
+        <v>778</v>
+      </c>
+      <c r="G35" s="119" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="17" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="247">
+        <v>42736</v>
+      </c>
+      <c r="B36" s="248"/>
+      <c r="C36" s="248" t="s">
+        <v>892</v>
+      </c>
+      <c r="D36" s="249" t="s">
+        <v>212</v>
+      </c>
+      <c r="E36" s="73" t="s">
+        <v>328</v>
+      </c>
+      <c r="F36" s="90" t="s">
+        <v>777</v>
+      </c>
+      <c r="G36" s="125" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="292" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="335">
+        <v>42736</v>
+      </c>
+      <c r="B37" s="337"/>
+      <c r="C37" s="331" t="s">
+        <v>922</v>
+      </c>
+      <c r="D37" s="353" t="s">
+        <v>909</v>
+      </c>
+      <c r="E37" s="293" t="s">
+        <v>913</v>
+      </c>
+      <c r="F37" s="354" t="s">
+        <v>776</v>
+      </c>
+      <c r="G37" s="355" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="292" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="336">
+        <v>42736</v>
+      </c>
+      <c r="B38" s="334"/>
+      <c r="C38" s="331" t="s">
+        <v>922</v>
+      </c>
+      <c r="D38" s="353" t="s">
+        <v>909</v>
+      </c>
+      <c r="E38" s="293" t="s">
+        <v>914</v>
+      </c>
+      <c r="F38" s="354" t="s">
+        <v>776</v>
+      </c>
+      <c r="G38" s="355" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="292" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="335">
+        <v>42736</v>
+      </c>
+      <c r="B39" s="337"/>
+      <c r="C39" s="331" t="s">
+        <v>922</v>
+      </c>
+      <c r="D39" s="353" t="s">
+        <v>909</v>
+      </c>
+      <c r="E39" s="293" t="s">
+        <v>907</v>
+      </c>
+      <c r="F39" s="354" t="s">
+        <v>776</v>
+      </c>
+      <c r="G39" s="355" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="292" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="335">
+        <v>42736</v>
+      </c>
+      <c r="B40" s="337"/>
+      <c r="C40" s="331" t="s">
+        <v>922</v>
+      </c>
+      <c r="D40" s="353" t="s">
+        <v>909</v>
+      </c>
+      <c r="E40" s="293" t="s">
+        <v>915</v>
+      </c>
+      <c r="F40" s="354" t="s">
+        <v>776</v>
+      </c>
+      <c r="G40" s="355" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="292" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="338">
+        <v>42736</v>
+      </c>
+      <c r="B41" s="339"/>
+      <c r="C41" s="340" t="s">
+        <v>922</v>
+      </c>
+      <c r="D41" s="332" t="s">
+        <v>909</v>
+      </c>
+      <c r="E41" s="333" t="s">
+        <v>916</v>
+      </c>
+      <c r="F41" s="356" t="s">
+        <v>776</v>
+      </c>
+      <c r="G41" s="357" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L78"/>
   <sheetViews>
@@ -16466,7 +17462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -16993,7 +17989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:CR67"/>
   <sheetViews>
@@ -19373,7 +20369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:FH30"/>
   <sheetViews>
@@ -20214,7 +21210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
@@ -22048,7 +23044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R171"/>
   <sheetViews>
@@ -28639,7 +29635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
@@ -29657,7 +30653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:DS35"/>
   <sheetViews>
@@ -30644,7 +31640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
@@ -31682,7 +32678,127 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD87C05-4433-0B47-8359-B17D583CFB7A}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="31" style="17" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="48.6640625" style="17" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="30" t="s">
+        <v>708</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+    </row>
+    <row r="2" spans="1:4" ht="42" x14ac:dyDescent="0.15">
+      <c r="A2" s="33" t="s">
+        <v>709</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>711</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="257" t="s">
+        <v>713</v>
+      </c>
+      <c r="B3" s="258" t="s">
+        <v>714</v>
+      </c>
+      <c r="C3" s="258" t="s">
+        <v>715</v>
+      </c>
+      <c r="D3" s="259" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="260" t="s">
+        <v>422</v>
+      </c>
+      <c r="B4" s="261" t="s">
+        <v>717</v>
+      </c>
+      <c r="C4" s="261" t="s">
+        <v>718</v>
+      </c>
+      <c r="D4" s="262" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{76901EAB-8C8D-2C4E-B48C-A34C7A0DEE7E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:BL53"/>
   <sheetViews>
@@ -32976,127 +34092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD87C05-4433-0B47-8359-B17D583CFB7A}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="31" style="17" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="48.6640625" style="17" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="17"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="30" t="s">
-        <v>708</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-    </row>
-    <row r="2" spans="1:4" ht="42" x14ac:dyDescent="0.15">
-      <c r="A2" s="33" t="s">
-        <v>709</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>710</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>711</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="257" t="s">
-        <v>713</v>
-      </c>
-      <c r="B3" s="258" t="s">
-        <v>714</v>
-      </c>
-      <c r="C3" s="258" t="s">
-        <v>715</v>
-      </c>
-      <c r="D3" s="259" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="260" t="s">
-        <v>422</v>
-      </c>
-      <c r="B4" s="261" t="s">
-        <v>717</v>
-      </c>
-      <c r="C4" s="261" t="s">
-        <v>718</v>
-      </c>
-      <c r="D4" s="262" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{76901EAB-8C8D-2C4E-B48C-A34C7A0DEE7E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -33228,7 +34224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
@@ -33577,7 +34573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F154"/>
   <sheetViews>
@@ -36383,7 +37379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -36544,7 +37540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:EK50"/>
   <sheetViews>
@@ -37746,7 +38742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:CF36"/>
   <sheetViews>
@@ -39398,11 +40394,169 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590FB9C5-F50E-214B-A54B-0633B3E45C3F}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="21" style="498" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="498" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="498" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="498" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="498" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="498" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="498" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="498" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" style="498" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="498" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="498"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23" x14ac:dyDescent="0.25">
+      <c r="A1" s="504" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="503" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="503" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="503" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="503" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3" s="503" t="s">
+        <v>337</v>
+      </c>
+      <c r="F3" s="503" t="s">
+        <v>225</v>
+      </c>
+      <c r="G3" s="503" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="503" t="s">
+        <v>400</v>
+      </c>
+      <c r="I3" s="503" t="s">
+        <v>874</v>
+      </c>
+      <c r="J3" s="503" t="s">
+        <v>454</v>
+      </c>
+      <c r="K3" s="503" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="501">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="501">
+        <v>42736</v>
+      </c>
+      <c r="C4" s="498" t="s">
+        <v>882</v>
+      </c>
+      <c r="D4" s="499"/>
+      <c r="E4" s="498" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="500" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H4" s="498">
+        <v>1</v>
+      </c>
+      <c r="I4" s="502" t="s">
+        <v>1011</v>
+      </c>
+      <c r="K4" s="499" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="501">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="501">
+        <v>42736</v>
+      </c>
+      <c r="C5" s="498" t="s">
+        <v>882</v>
+      </c>
+      <c r="E5" s="498" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="500" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H5" s="498">
+        <v>2</v>
+      </c>
+      <c r="K5" s="499" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="501">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="501">
+        <v>42736</v>
+      </c>
+      <c r="C6" s="498" t="s">
+        <v>882</v>
+      </c>
+      <c r="E6" s="498" t="s">
+        <v>667</v>
+      </c>
+      <c r="G6" s="500" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H6" s="498">
+        <v>3</v>
+      </c>
+      <c r="K6" s="499" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:B6" xr:uid="{55AA11B3-7BE7-9B49-898D-8FBAB83ED961}">
+      <formula1>42736</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{A39E125B-D4A5-5B42-A9C3-D2C963D285C3}">
+          <x14:formula1>
+            <xm:f>'/Users/dev/Documents/Definition Files/[RDM-8509.xlsx]CaseField'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC343D0E-808F-8348-B776-EC7A2F9FD0AC}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -39556,7 +40710,7 @@
         <v>991</v>
       </c>
       <c r="D6" s="486">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>998</v>
@@ -39583,7 +40737,7 @@
         <v>1006</v>
       </c>
       <c r="D7" s="486">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>1001</v>
@@ -39608,7 +40762,7 @@
         <v>1003</v>
       </c>
       <c r="D8" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>1001</v>
@@ -39651,7 +40805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IO132"/>
   <sheetViews>
@@ -46804,7 +47958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T78"/>
   <sheetViews>
@@ -49589,885 +50743,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2A25AD-5D69-564D-9511-0323740C2E1F}">
-  <dimension ref="A1:G41"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.5" customWidth="1"/>
-    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
-        <v>332</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-    </row>
-    <row r="2" spans="1:7" ht="126" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="55" t="s">
-        <v>333</v>
-      </c>
-      <c r="D2" s="55" t="s">
-        <v>334</v>
-      </c>
-      <c r="E2" s="55" t="s">
-        <v>221</v>
-      </c>
-      <c r="F2" s="55" t="s">
-        <v>335</v>
-      </c>
-      <c r="G2" s="55" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="250" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="251" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="251" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="251" t="s">
-        <v>337</v>
-      </c>
-      <c r="E3" s="251" t="s">
-        <v>225</v>
-      </c>
-      <c r="F3" s="251" t="s">
-        <v>338</v>
-      </c>
-      <c r="G3" s="252" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="196"/>
-      <c r="C4" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D4" s="196" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>257</v>
-      </c>
-      <c r="F4" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G4" s="244" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="196"/>
-      <c r="C5" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D5" s="196" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="65" t="s">
-        <v>259</v>
-      </c>
-      <c r="F5" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G5" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="196"/>
-      <c r="C6" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D6" s="196" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" s="62" t="s">
-        <v>262</v>
-      </c>
-      <c r="F6" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G6" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="196"/>
-      <c r="C7" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D7" s="196" t="s">
-        <v>119</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>264</v>
-      </c>
-      <c r="F7" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G7" s="244" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="196"/>
-      <c r="C8" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D8" s="196" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" s="65" t="s">
-        <v>266</v>
-      </c>
-      <c r="F8" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G8" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="196"/>
-      <c r="C9" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D9" s="196" t="s">
-        <v>119</v>
-      </c>
-      <c r="E9" s="65" t="s">
-        <v>268</v>
-      </c>
-      <c r="F9" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G9" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="196"/>
-      <c r="C10" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D10" s="196" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" s="65" t="s">
-        <v>270</v>
-      </c>
-      <c r="F10" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G10" s="244" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="196"/>
-      <c r="C11" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D11" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" s="197" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G11" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="196"/>
-      <c r="C12" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D12" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E12" s="197" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G12" s="244" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B13" s="196"/>
-      <c r="C13" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D13" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E13" s="197" t="s">
-        <v>311</v>
-      </c>
-      <c r="F13" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G13" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B14" s="196"/>
-      <c r="C14" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D14" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E14" s="67" t="s">
-        <v>315</v>
-      </c>
-      <c r="F14" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G14" s="245" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="196"/>
-      <c r="C15" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D15" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" s="197" t="s">
-        <v>313</v>
-      </c>
-      <c r="F15" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G15" s="245" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="196"/>
-      <c r="C16" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D16" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E16" s="65" t="s">
-        <v>341</v>
-      </c>
-      <c r="F16" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G16" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B17" s="196"/>
-      <c r="C17" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D17" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E17" s="65" t="s">
-        <v>342</v>
-      </c>
-      <c r="F17" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G17" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B18" s="196"/>
-      <c r="C18" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D18" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="65" t="s">
-        <v>343</v>
-      </c>
-      <c r="F18" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G18" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B19" s="196"/>
-      <c r="C19" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D19" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" s="82" t="s">
-        <v>344</v>
-      </c>
-      <c r="F19" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G19" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B20" s="196"/>
-      <c r="C20" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D20" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="65" t="s">
-        <v>345</v>
-      </c>
-      <c r="F20" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G20" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B21" s="196"/>
-      <c r="C21" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D21" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E21" s="65" t="s">
-        <v>346</v>
-      </c>
-      <c r="F21" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G21" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B22" s="196"/>
-      <c r="C22" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D22" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E22" s="65" t="s">
-        <v>347</v>
-      </c>
-      <c r="F22" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G22" s="245" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B23" s="196"/>
-      <c r="C23" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D23" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" s="65" t="s">
-        <v>348</v>
-      </c>
-      <c r="F23" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G23" s="245" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="196"/>
-      <c r="C24" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D24" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E24" s="65" t="s">
-        <v>349</v>
-      </c>
-      <c r="F24" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G24" s="245" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B25" s="196"/>
-      <c r="C25" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D25" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E25" s="65" t="s">
-        <v>350</v>
-      </c>
-      <c r="F25" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G25" s="245" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B26" s="196"/>
-      <c r="C26" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D26" s="120" t="s">
-        <v>124</v>
-      </c>
-      <c r="E26" s="65" t="s">
-        <v>351</v>
-      </c>
-      <c r="F26" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G26" s="245" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B27" s="196"/>
-      <c r="C27" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D27" s="120" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" s="65" t="s">
-        <v>273</v>
-      </c>
-      <c r="F27" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G27" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B28" s="196"/>
-      <c r="C28" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D28" s="120" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" s="62" t="s">
-        <v>275</v>
-      </c>
-      <c r="F28" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G28" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B29" s="196"/>
-      <c r="C29" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D29" s="120" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="62" t="s">
-        <v>277</v>
-      </c>
-      <c r="F29" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G29" s="245" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B30" s="196"/>
-      <c r="C30" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D30" s="120" t="s">
-        <v>114</v>
-      </c>
-      <c r="E30" s="62" t="s">
-        <v>279</v>
-      </c>
-      <c r="F30" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G30" s="245" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B31" s="196"/>
-      <c r="C31" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D31" s="120" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" s="65" t="s">
-        <v>119</v>
-      </c>
-      <c r="F31" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G31" s="245" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="243">
-        <v>42736</v>
-      </c>
-      <c r="B32" s="196"/>
-      <c r="C32" s="196" t="s">
-        <v>887</v>
-      </c>
-      <c r="D32" s="120" t="s">
-        <v>114</v>
-      </c>
-      <c r="E32" s="65" t="s">
-        <v>282</v>
-      </c>
-      <c r="F32" s="84" t="s">
-        <v>776</v>
-      </c>
-      <c r="G32" s="245" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="17" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="246">
-        <v>42736</v>
-      </c>
-      <c r="B33" s="127"/>
-      <c r="C33" s="127" t="s">
-        <v>892</v>
-      </c>
-      <c r="D33" s="132" t="s">
-        <v>212</v>
-      </c>
-      <c r="E33" s="65" t="s">
-        <v>326</v>
-      </c>
-      <c r="F33" s="118" t="s">
-        <v>778</v>
-      </c>
-      <c r="G33" s="119" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="17" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="246">
-        <v>42736</v>
-      </c>
-      <c r="B34" s="127"/>
-      <c r="C34" s="127" t="s">
-        <v>892</v>
-      </c>
-      <c r="D34" s="132" t="s">
-        <v>212</v>
-      </c>
-      <c r="E34" s="65" t="s">
-        <v>326</v>
-      </c>
-      <c r="F34" s="118" t="s">
-        <v>777</v>
-      </c>
-      <c r="G34" s="119" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="17" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="246">
-        <v>42736</v>
-      </c>
-      <c r="B35" s="127"/>
-      <c r="C35" s="214" t="s">
-        <v>892</v>
-      </c>
-      <c r="D35" s="132" t="s">
-        <v>212</v>
-      </c>
-      <c r="E35" s="65" t="s">
-        <v>328</v>
-      </c>
-      <c r="F35" s="84" t="s">
-        <v>778</v>
-      </c>
-      <c r="G35" s="119" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="17" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="247">
-        <v>42736</v>
-      </c>
-      <c r="B36" s="248"/>
-      <c r="C36" s="248" t="s">
-        <v>892</v>
-      </c>
-      <c r="D36" s="249" t="s">
-        <v>212</v>
-      </c>
-      <c r="E36" s="73" t="s">
-        <v>328</v>
-      </c>
-      <c r="F36" s="90" t="s">
-        <v>777</v>
-      </c>
-      <c r="G36" s="125" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="292" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="335">
-        <v>42736</v>
-      </c>
-      <c r="B37" s="337"/>
-      <c r="C37" s="331" t="s">
-        <v>922</v>
-      </c>
-      <c r="D37" s="353" t="s">
-        <v>909</v>
-      </c>
-      <c r="E37" s="293" t="s">
-        <v>913</v>
-      </c>
-      <c r="F37" s="354" t="s">
-        <v>776</v>
-      </c>
-      <c r="G37" s="355" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="292" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="336">
-        <v>42736</v>
-      </c>
-      <c r="B38" s="334"/>
-      <c r="C38" s="331" t="s">
-        <v>922</v>
-      </c>
-      <c r="D38" s="353" t="s">
-        <v>909</v>
-      </c>
-      <c r="E38" s="293" t="s">
-        <v>914</v>
-      </c>
-      <c r="F38" s="354" t="s">
-        <v>776</v>
-      </c>
-      <c r="G38" s="355" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="292" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="335">
-        <v>42736</v>
-      </c>
-      <c r="B39" s="337"/>
-      <c r="C39" s="331" t="s">
-        <v>922</v>
-      </c>
-      <c r="D39" s="353" t="s">
-        <v>909</v>
-      </c>
-      <c r="E39" s="293" t="s">
-        <v>907</v>
-      </c>
-      <c r="F39" s="354" t="s">
-        <v>776</v>
-      </c>
-      <c r="G39" s="355" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="292" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="335">
-        <v>42736</v>
-      </c>
-      <c r="B40" s="337"/>
-      <c r="C40" s="331" t="s">
-        <v>922</v>
-      </c>
-      <c r="D40" s="353" t="s">
-        <v>909</v>
-      </c>
-      <c r="E40" s="293" t="s">
-        <v>915</v>
-      </c>
-      <c r="F40" s="354" t="s">
-        <v>776</v>
-      </c>
-      <c r="G40" s="355" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="292" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="338">
-        <v>42736</v>
-      </c>
-      <c r="B41" s="339"/>
-      <c r="C41" s="340" t="s">
-        <v>922</v>
-      </c>
-      <c r="D41" s="332" t="s">
-        <v>909</v>
-      </c>
-      <c r="E41" s="333" t="s">
-        <v>916</v>
-      </c>
-      <c r="F41" s="356" t="s">
-        <v>776</v>
-      </c>
-      <c r="G41" s="357" t="s">
-        <v>339</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
delete complex type retainHiddenField
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF45DF8-DB8B-6F49-9003-5E9494DA3370}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F49D13-3C2F-1A45-BBD4-3FB9859FE301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5935" uniqueCount="983">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5927" uniqueCount="981">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3079,13 +3079,7 @@
     <t>RetainHiddenValue</t>
   </si>
   <si>
-    <t>MotherFullName="Mary"</t>
-  </si>
-  <si>
     <t>Homeless="no"</t>
-  </si>
-  <si>
-    <t>ChildFullName="Jack"</t>
   </si>
 </sst>
 </file>
@@ -19630,8 +19624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R171"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C126" zoomScale="88" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView showGridLines="0" topLeftCell="D15" zoomScale="88" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20862,7 +20856,7 @@
       </c>
       <c r="K30" s="81"/>
       <c r="L30" s="81" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="M30" s="81" t="b">
         <v>1</v>
@@ -20906,7 +20900,7 @@
       </c>
       <c r="K31" s="81"/>
       <c r="L31" s="81" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="M31" s="81" t="b">
         <v>1</v>
@@ -44118,8 +44112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D51" workbookViewId="0">
-      <selection activeCell="M77" sqref="M77:M78"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J36" sqref="I36:J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -45047,12 +45041,8 @@
       <c r="H26" s="62" t="s">
         <v>261</v>
       </c>
-      <c r="I26" s="62" t="s">
-        <v>982</v>
-      </c>
-      <c r="J26" s="62" t="s">
-        <v>422</v>
-      </c>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
       <c r="K26" s="81"/>
       <c r="L26" s="81"/>
       <c r="M26" s="62" t="s">
@@ -45087,12 +45077,8 @@
       <c r="H27" s="62" t="s">
         <v>263</v>
       </c>
-      <c r="I27" s="62" t="s">
-        <v>982</v>
-      </c>
-      <c r="J27" s="62" t="s">
-        <v>424</v>
-      </c>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
       <c r="K27" s="81"/>
       <c r="L27" s="81"/>
       <c r="M27" s="62" t="s">
@@ -45369,12 +45355,8 @@
       <c r="H35" s="62" t="s">
         <v>276</v>
       </c>
-      <c r="I35" s="62" t="s">
-        <v>980</v>
-      </c>
-      <c r="J35" s="62" t="s">
-        <v>422</v>
-      </c>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
       <c r="K35" s="81"/>
       <c r="L35" s="81"/>
       <c r="M35" s="62" t="s">
@@ -45409,12 +45391,8 @@
       <c r="H36" s="62" t="s">
         <v>278</v>
       </c>
-      <c r="I36" s="62" t="s">
-        <v>980</v>
-      </c>
-      <c r="J36" s="62" t="s">
-        <v>424</v>
-      </c>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
       <c r="K36" s="81"/>
       <c r="L36" s="81"/>
       <c r="M36" s="62" t="s">

</xml_diff>

<commit_message>
remove retainHiddenFields and convert to json
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E817009-72EE-F24F-B859-A29EE77345EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D2E2AE-F54F-814B-86B7-1371FF08310C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="21380" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19980" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7195" uniqueCount="1110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7191" uniqueCount="1110">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -5772,992 +5772,6 @@
   </cellStyles>
   <dxfs count="317">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0432FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0432FF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;D/&quot;m&quot;/YY&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -8853,6 +7867,416 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -10333,6 +9757,283 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -12004,6 +11705,54 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13202,6 +12951,257 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;D/&quot;m&quot;/YY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -13354,392 +13354,392 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" headerRowBorderDxfId="35" tableBorderDxfId="36" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="316" dataDxfId="314" headerRowBorderDxfId="315" tableBorderDxfId="313" totalsRowBorderDxfId="312">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="311"/>
+    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="310"/>
+    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="309"/>
+    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="308"/>
+    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="307"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L78" totalsRowShown="0" headerRowDxfId="202" dataDxfId="200" headerRowBorderDxfId="201" tableBorderDxfId="199" totalsRowBorderDxfId="198">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L78" totalsRowShown="0" headerRowDxfId="190" dataDxfId="188" headerRowBorderDxfId="189" tableBorderDxfId="187" totalsRowBorderDxfId="186">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="197"/>
-    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="196"/>
-    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="195"/>
-    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="194"/>
-    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="193"/>
-    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="192"/>
-    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="191"/>
-    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="190"/>
-    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="189"/>
-    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="188"/>
-    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="187"/>
-    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="186"/>
+    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="185"/>
+    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="184"/>
+    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="183"/>
+    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="182"/>
+    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="181"/>
+    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="180"/>
+    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="179"/>
+    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="178"/>
+    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="177"/>
+    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="176"/>
+    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="175"/>
+    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="174"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H40" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" headerRowBorderDxfId="25" tableBorderDxfId="26" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H40" totalsRowShown="0" headerRowDxfId="173" dataDxfId="171" headerRowBorderDxfId="172" tableBorderDxfId="170" totalsRowBorderDxfId="169">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="168"/>
+    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="167"/>
+    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="166"/>
+    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="165"/>
+    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="164"/>
+    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="163"/>
+    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="162"/>
+    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="161"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:T55" totalsRowShown="0" headerRowDxfId="185" dataDxfId="183" headerRowBorderDxfId="184" tableBorderDxfId="182" totalsRowBorderDxfId="181">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:T55" totalsRowShown="0" headerRowDxfId="160" dataDxfId="158" headerRowBorderDxfId="159" tableBorderDxfId="157" totalsRowBorderDxfId="156">
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="180"/>
-    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="179"/>
-    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="178"/>
-    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="177"/>
-    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="176"/>
-    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="175"/>
-    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="174"/>
-    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="173"/>
-    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="172"/>
-    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="171" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="170"/>
-    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="169"/>
-    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="168"/>
-    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="167"/>
-    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="166"/>
-    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="165"/>
-    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="164"/>
-    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="163"/>
-    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="162"/>
-    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="EndButtonLabel" dataDxfId="161"/>
+    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="155"/>
+    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="154"/>
+    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="153"/>
+    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="152"/>
+    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="151"/>
+    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="150"/>
+    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="149"/>
+    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="148"/>
+    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="147"/>
+    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="146" dataCellStyle="Hyperlink"/>
+    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="145"/>
+    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="144"/>
+    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="143"/>
+    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="142"/>
+    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="141"/>
+    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="140"/>
+    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="139"/>
+    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="138"/>
+    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="137"/>
+    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="EndButtonLabel" dataDxfId="136"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:R183" totalsRowShown="0" headerRowDxfId="160" dataDxfId="158" headerRowBorderDxfId="159" tableBorderDxfId="157" totalsRowBorderDxfId="156">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:R183" totalsRowShown="0" headerRowDxfId="135" dataDxfId="133" headerRowBorderDxfId="134" tableBorderDxfId="132" totalsRowBorderDxfId="131">
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="155"/>
-    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="154"/>
-    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="153"/>
-    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="152"/>
-    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="151"/>
-    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="150"/>
-    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="149"/>
-    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="148"/>
-    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="147"/>
-    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="146"/>
-    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="145"/>
-    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="144"/>
-    <tableColumn id="18" xr3:uid="{E135335A-D7E2-F744-932E-E0627D2DBFE1}" name="RetainHiddenValue" dataDxfId="143"/>
-    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="142"/>
-    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="141"/>
-    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="140"/>
-    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="139"/>
-    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="138"/>
+    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="130"/>
+    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="129"/>
+    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="128"/>
+    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="127"/>
+    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="126"/>
+    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="125"/>
+    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="124"/>
+    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="123"/>
+    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="122"/>
+    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="121"/>
+    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="120"/>
+    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="119"/>
+    <tableColumn id="18" xr3:uid="{E135335A-D7E2-F744-932E-E0627D2DBFE1}" name="RetainHiddenValue" dataDxfId="118"/>
+    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="117"/>
+    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="116"/>
+    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="115"/>
+    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="114"/>
+    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H58" totalsRowShown="0" headerRowDxfId="137" dataDxfId="135" headerRowBorderDxfId="136" tableBorderDxfId="134" totalsRowBorderDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H58" totalsRowShown="0" headerRowDxfId="112" dataDxfId="110" headerRowBorderDxfId="111" tableBorderDxfId="109" totalsRowBorderDxfId="108">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="132"/>
-    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="131"/>
-    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="130"/>
-    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="129"/>
-    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="128"/>
-    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="127"/>
-    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="126"/>
-    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="125"/>
+    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="106"/>
+    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="105"/>
+    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="104"/>
+    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="103"/>
+    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="102"/>
+    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="101"/>
+    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:I48" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:I48" totalsRowShown="0" headerRowDxfId="99" dataDxfId="97" headerRowBorderDxfId="98" tableBorderDxfId="96" totalsRowBorderDxfId="95">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{4DAFD93D-577A-F041-B588-5C995BA5B65E}" name="ResultsOrdering" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{98FE8C07-877C-564D-B37F-388027F0E2FE}" name="DisplayContextParameter" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="91"/>
+    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="89"/>
+    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="88"/>
+    <tableColumn id="8" xr3:uid="{4DAFD93D-577A-F041-B588-5C995BA5B65E}" name="ResultsOrdering" dataDxfId="87"/>
+    <tableColumn id="9" xr3:uid="{98FE8C07-877C-564D-B37F-388027F0E2FE}" name="DisplayContextParameter" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H57" totalsRowShown="0" headerRowDxfId="124" dataDxfId="122" headerRowBorderDxfId="123" tableBorderDxfId="121" totalsRowBorderDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H57" totalsRowShown="0" headerRowDxfId="85" dataDxfId="83" headerRowBorderDxfId="84" tableBorderDxfId="82" totalsRowBorderDxfId="81">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="117"/>
-    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="116"/>
-    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="115"/>
-    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="114"/>
-    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="113"/>
-    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="112"/>
+    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I62" totalsRowShown="0" headerRowDxfId="111" dataDxfId="109" headerRowBorderDxfId="110" tableBorderDxfId="108" totalsRowBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I62" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="103"/>
-    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="100"/>
-    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="99"/>
-    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="61"/>
+    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96" tableBorderDxfId="94" totalsRowBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="87"/>
+    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E28" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83" totalsRowBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E28" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="316" dataDxfId="314" headerRowBorderDxfId="315" tableBorderDxfId="313" totalsRowBorderDxfId="312">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="306" dataDxfId="304" headerRowBorderDxfId="305" tableBorderDxfId="303" totalsRowBorderDxfId="302">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="311"/>
-    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="310"/>
-    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="309"/>
-    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="308" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="301"/>
+    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="300"/>
+    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="299"/>
+    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="298" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F186" totalsRowShown="0" headerRowDxfId="76" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F186" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D18" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64" totalsRowBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D18" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="61" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="22" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F69" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56" totalsRowBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F69" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F43" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F43" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I21" totalsRowShown="0" headerRowDxfId="307" dataDxfId="305" headerRowBorderDxfId="306" tableBorderDxfId="304" totalsRowBorderDxfId="303">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I21" totalsRowShown="0" headerRowDxfId="297" dataDxfId="295" headerRowBorderDxfId="296" tableBorderDxfId="294" totalsRowBorderDxfId="293">
   <autoFilter ref="A3:I21" xr:uid="{C0075E79-5DBE-654F-827E-CA137EF61FB4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="302"/>
-    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="301"/>
-    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="300"/>
-    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="299"/>
-    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="298"/>
-    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="297"/>
-    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="296"/>
-    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="295"/>
-    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="294"/>
+    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="292"/>
+    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="291"/>
+    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="290"/>
+    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="289"/>
+    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="288"/>
+    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="287"/>
+    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="286"/>
+    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="285"/>
+    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="284"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{F70D0623-0A9A-6C4C-9874-9A93D5DC3ACF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="293" dataDxfId="291" headerRowBorderDxfId="292" tableBorderDxfId="290" totalsRowBorderDxfId="289">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{F70D0623-0A9A-6C4C-9874-9A93D5DC3ACF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="283" dataDxfId="281" headerRowBorderDxfId="282" tableBorderDxfId="280" totalsRowBorderDxfId="279">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{24BEC596-8705-9C49-940B-FCCC2F2EB305}" name="CaseTypeId" dataDxfId="288"/>
-    <tableColumn id="2" xr3:uid="{C8273B71-59AA-7D4D-B60F-85A96E9E15D7}" name="ReasonRequired" dataDxfId="287"/>
-    <tableColumn id="4" xr3:uid="{4A0A9C2B-6C96-574F-BCC8-ACBC4B9E5EA7}" name="NoCActionInterpretationRequired" dataDxfId="286" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{24BEC596-8705-9C49-940B-FCCC2F2EB305}" name="CaseTypeId" dataDxfId="278"/>
+    <tableColumn id="2" xr3:uid="{C8273B71-59AA-7D4D-B60F-85A96E9E15D7}" name="ReasonRequired" dataDxfId="277"/>
+    <tableColumn id="4" xr3:uid="{4A0A9C2B-6C96-574F-BCC8-ACBC4B9E5EA7}" name="NoCActionInterpretationRequired" dataDxfId="276" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:O154" totalsRowShown="0" headerRowDxfId="285" dataDxfId="283" headerRowBorderDxfId="284" tableBorderDxfId="282" totalsRowBorderDxfId="281">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:O154" totalsRowShown="0" headerRowDxfId="275" dataDxfId="273" headerRowBorderDxfId="274" tableBorderDxfId="272" totalsRowBorderDxfId="271">
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="280"/>
-    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="279"/>
-    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="278"/>
-    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="277"/>
-    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="276"/>
-    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="275"/>
-    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="274"/>
-    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="273"/>
-    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="272"/>
-    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="271"/>
-    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="270"/>
-    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="269"/>
-    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="268"/>
-    <tableColumn id="14" xr3:uid="{4541E6DA-EAB5-7443-A660-006BEE34C855}" name="DefaultHidden" dataDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{294BBB22-F970-A34E-A077-D51352647008}" name="Searchable" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="270"/>
+    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="269"/>
+    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="268"/>
+    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="267"/>
+    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="266"/>
+    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="265"/>
+    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="264"/>
+    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="263"/>
+    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="262"/>
+    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="261"/>
+    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="260"/>
+    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="259"/>
+    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="258"/>
+    <tableColumn id="14" xr3:uid="{4541E6DA-EAB5-7443-A660-006BEE34C855}" name="DefaultHidden" dataDxfId="257"/>
+    <tableColumn id="15" xr3:uid="{294BBB22-F970-A34E-A077-D51352647008}" name="Searchable" dataDxfId="256"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:T88" totalsRowShown="0" headerRowDxfId="267" dataDxfId="265" headerRowBorderDxfId="266" tableBorderDxfId="264" totalsRowBorderDxfId="263">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:T88" totalsRowShown="0" headerRowDxfId="255" dataDxfId="253" headerRowBorderDxfId="254" tableBorderDxfId="252" totalsRowBorderDxfId="251">
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="262"/>
-    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="261"/>
-    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="260"/>
-    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="259"/>
-    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="258"/>
-    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="257"/>
-    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="256"/>
-    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="255"/>
-    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="254"/>
+    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="250"/>
+    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="249"/>
+    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="248"/>
+    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="247"/>
+    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="246"/>
+    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="245"/>
+    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="244"/>
+    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="243"/>
+    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="242"/>
     <tableColumn id="20" xr3:uid="{3056D2D9-052A-4948-A9B6-EA6D4AEEE813}" name="RetainHiddenValue"/>
-    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="253"/>
-    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="252"/>
-    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="251"/>
-    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="250"/>
-    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="249"/>
-    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="248"/>
-    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="247"/>
-    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="246"/>
-    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="245"/>
-    <tableColumn id="19" xr3:uid="{4721EA60-AB43-3A4D-9D3A-D995D789F1AA}" name="Searchable" dataDxfId="244"/>
+    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="241"/>
+    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="240"/>
+    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="239"/>
+    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="238"/>
+    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="237"/>
+    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="236"/>
+    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="235"/>
+    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="234"/>
+    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="233"/>
+    <tableColumn id="19" xr3:uid="{4721EA60-AB43-3A4D-9D3A-D995D789F1AA}" name="Searchable" dataDxfId="232"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G46" totalsRowShown="0" headerRowDxfId="243" dataDxfId="241" headerRowBorderDxfId="242" tableBorderDxfId="240" totalsRowBorderDxfId="239" headerRowCellStyle="Normal 2 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G46" totalsRowShown="0" headerRowDxfId="231" dataDxfId="229" headerRowBorderDxfId="230" tableBorderDxfId="228" totalsRowBorderDxfId="227" headerRowCellStyle="Normal 2 3">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="238"/>
-    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="237"/>
-    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="236"/>
-    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="235"/>
-    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="234"/>
-    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="233"/>
-    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="232"/>
+    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="226"/>
+    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="225"/>
+    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="224"/>
+    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="223"/>
+    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="222"/>
+    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="221"/>
+    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="220"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:L153" totalsRowShown="0" headerRowDxfId="231" dataDxfId="229" headerRowBorderDxfId="230" tableBorderDxfId="228" totalsRowBorderDxfId="227">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:L153" totalsRowShown="0" headerRowDxfId="219" dataDxfId="217" headerRowBorderDxfId="218" tableBorderDxfId="216" totalsRowBorderDxfId="215">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="226"/>
-    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="225"/>
-    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="224"/>
-    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="223"/>
-    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="222"/>
-    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="221"/>
-    <tableColumn id="12" xr3:uid="{4E9EBE21-1E8A-8F42-8DBF-15D634A7D163}" name="DefaultValue" dataDxfId="220"/>
-    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="219"/>
-    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="218"/>
-    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="217"/>
-    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="216"/>
-    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="215"/>
+    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="214"/>
+    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="213"/>
+    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="212"/>
+    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="211"/>
+    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="210"/>
+    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="209"/>
+    <tableColumn id="12" xr3:uid="{4E9EBE21-1E8A-8F42-8DBF-15D634A7D163}" name="DefaultValue" dataDxfId="208"/>
+    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="207"/>
+    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="206"/>
+    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="205"/>
+    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="204"/>
+    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="203"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G36" totalsRowShown="0" headerRowDxfId="214" dataDxfId="212" headerRowBorderDxfId="213" tableBorderDxfId="211" totalsRowBorderDxfId="210">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G36" totalsRowShown="0" headerRowDxfId="202" dataDxfId="200" headerRowBorderDxfId="201" tableBorderDxfId="199" totalsRowBorderDxfId="198">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="209"/>
-    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="208"/>
-    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="207"/>
-    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="206"/>
-    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="205"/>
-    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="204"/>
-    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="203"/>
+    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="197"/>
+    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="196"/>
+    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="195"/>
+    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="194"/>
+    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="193"/>
+    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="192"/>
+    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="191"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -21559,8 +21559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R183"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A110" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C178" sqref="C178:C181"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E95" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -22793,9 +22793,7 @@
       <c r="L30" s="81" t="s">
         <v>981</v>
       </c>
-      <c r="M30" s="81" t="b">
-        <v>1</v>
-      </c>
+      <c r="M30" s="81"/>
       <c r="N30" s="81"/>
       <c r="O30" s="81"/>
       <c r="P30" s="62" t="s">
@@ -41929,7 +41927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IO154"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C145" sqref="C145"/>
     </sheetView>
@@ -50320,8 +50318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T88"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView showGridLines="0" topLeftCell="B68" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -51252,9 +51250,7 @@
       <c r="I26" s="62" t="s">
         <v>982</v>
       </c>
-      <c r="J26" s="62" t="s">
-        <v>422</v>
-      </c>
+      <c r="J26" s="62"/>
       <c r="K26" s="81"/>
       <c r="L26" s="81"/>
       <c r="M26" s="62" t="s">
@@ -51292,9 +51288,7 @@
       <c r="I27" s="62" t="s">
         <v>982</v>
       </c>
-      <c r="J27" s="62" t="s">
-        <v>424</v>
-      </c>
+      <c r="J27" s="62"/>
       <c r="K27" s="81"/>
       <c r="L27" s="81"/>
       <c r="M27" s="62" t="s">
@@ -51574,9 +51568,7 @@
       <c r="I35" s="62" t="s">
         <v>980</v>
       </c>
-      <c r="J35" s="62" t="s">
-        <v>422</v>
-      </c>
+      <c r="J35" s="62"/>
       <c r="K35" s="81"/>
       <c r="L35" s="81"/>
       <c r="M35" s="62" t="s">
@@ -51614,9 +51606,7 @@
       <c r="I36" s="62" t="s">
         <v>980</v>
       </c>
-      <c r="J36" s="62" t="s">
-        <v>424</v>
-      </c>
+      <c r="J36" s="62"/>
       <c r="K36" s="81"/>
       <c r="L36" s="81"/>
       <c r="M36" s="62" t="s">
@@ -54358,7 +54348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H121" sqref="H121"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove retainHiddenFields and bump version
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F9D2AB-2B9D-6B46-A2C2-608B88F731A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3B2154-43D5-8942-A3D4-06B269D11151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6679" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6675" uniqueCount="1062">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -15408,7 +15408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:CR69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
@@ -20844,8 +20844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R184"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A144" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C168" sqref="C168"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -22078,9 +22078,7 @@
       <c r="L30" s="81" t="s">
         <v>981</v>
       </c>
-      <c r="M30" s="81" t="b">
-        <v>1</v>
-      </c>
+      <c r="M30" s="81"/>
       <c r="N30" s="81"/>
       <c r="O30" s="81"/>
       <c r="P30" s="62" t="s">
@@ -22122,9 +22120,7 @@
       <c r="L31" s="81" t="s">
         <v>981</v>
       </c>
-      <c r="M31" s="81" t="b">
-        <v>1</v>
-      </c>
+      <c r="M31" s="81"/>
       <c r="N31" s="81"/>
       <c r="O31" s="81"/>
       <c r="P31" s="62" t="s">
@@ -40017,7 +40013,7 @@
   <dimension ref="A1:IO147"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
@@ -50678,8 +50674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView showGridLines="0" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -51610,9 +51606,7 @@
       <c r="I26" s="62" t="s">
         <v>982</v>
       </c>
-      <c r="J26" s="62" t="s">
-        <v>422</v>
-      </c>
+      <c r="J26" s="62"/>
       <c r="K26" s="81"/>
       <c r="L26" s="81"/>
       <c r="M26" s="62" t="s">
@@ -51650,9 +51644,7 @@
       <c r="I27" s="62" t="s">
         <v>982</v>
       </c>
-      <c r="J27" s="62" t="s">
-        <v>424</v>
-      </c>
+      <c r="J27" s="62"/>
       <c r="K27" s="81"/>
       <c r="L27" s="81"/>
       <c r="M27" s="62" t="s">
@@ -51932,9 +51924,7 @@
       <c r="I35" s="62" t="s">
         <v>980</v>
       </c>
-      <c r="J35" s="62" t="s">
-        <v>422</v>
-      </c>
+      <c r="J35" s="62"/>
       <c r="K35" s="81"/>
       <c r="L35" s="81"/>
       <c r="M35" s="62" t="s">
@@ -51972,9 +51962,7 @@
       <c r="I36" s="62" t="s">
         <v>980</v>
       </c>
-      <c r="J36" s="62" t="s">
-        <v>424</v>
-      </c>
+      <c r="J36" s="62"/>
       <c r="K36" s="81"/>
       <c r="L36" s="81"/>
       <c r="M36" s="62" t="s">

</xml_diff>

<commit_message>
ACA-68 - BEFTA_Master_definition callbacks corrected to use aat url
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CABCB4-7E6B-8242-BB58-860C154C0251}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBD6678-5101-5741-B4E3-4003600BA8D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="16" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,16 +47,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">CaseEvent!$A$22:$T$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseField!$A$3:$IO$123</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -3478,9 +3472,6 @@
     <t>Notice of Change Request</t>
   </si>
   <si>
-    <t>http://host.docker.internal:5555/callback_returning_simulated_completed_noc_request</t>
-  </si>
-  <si>
     <t>individual.FirstName</t>
   </si>
   <si>
@@ -3524,6 +3515,9 @@
   </si>
   <si>
     <t>The other party solicitor</t>
+  </si>
+  <si>
+    <t>http://ccd-test-stubs-service-aat.service.core-compute-aat.internal/callback_returning_simulated_completed_noc_request</t>
   </si>
 </sst>
 </file>
@@ -5849,9 +5843,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5882,6 +5873,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="21" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="21" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -19301,8 +19295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="109" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J24" zoomScale="109" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21624,8 +21618,8 @@
       </c>
       <c r="J55" s="117"/>
       <c r="K55" s="114"/>
-      <c r="L55" s="580" t="s">
-        <v>1111</v>
+      <c r="L55" s="591" t="s">
+        <v>1126</v>
       </c>
       <c r="M55" s="114"/>
       <c r="N55" s="114"/>
@@ -21651,6 +21645,7 @@
   <hyperlinks>
     <hyperlink ref="J35" r:id="rId1" xr:uid="{D8CF8637-CA9E-D640-B8A5-0839120ED0E2}"/>
     <hyperlink ref="J36" r:id="rId2" xr:uid="{965A59DF-24BC-0646-830A-59FEE12B238C}"/>
+    <hyperlink ref="L55" r:id="rId3" xr:uid="{CDE2BD3A-FA56-BB44-9DE4-19C11ADAD442}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -21658,7 +21653,7 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -30528,10 +30523,10 @@
         <v>1068</v>
       </c>
       <c r="E50" s="78" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F50" s="78" t="s">
         <v>1112</v>
-      </c>
-      <c r="F50" s="78" t="s">
-        <v>1113</v>
       </c>
       <c r="G50" s="153">
         <v>1</v>
@@ -30550,10 +30545,10 @@
         <v>1068</v>
       </c>
       <c r="E51" s="78" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F51" s="78" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="G51" s="153">
         <v>2</v>
@@ -30572,10 +30567,10 @@
         <v>1068</v>
       </c>
       <c r="E52" s="78" t="s">
+        <v>1114</v>
+      </c>
+      <c r="F52" s="78" t="s">
         <v>1115</v>
-      </c>
-      <c r="F52" s="78" t="s">
-        <v>1116</v>
       </c>
       <c r="G52" s="153">
         <v>3</v>
@@ -30594,10 +30589,10 @@
         <v>1068</v>
       </c>
       <c r="E53" s="78" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F53" s="78" t="s">
         <v>1117</v>
-      </c>
-      <c r="F53" s="78" t="s">
-        <v>1118</v>
       </c>
       <c r="G53" s="153">
         <v>4</v>
@@ -30616,10 +30611,10 @@
         <v>1068</v>
       </c>
       <c r="E54" s="78" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F54" s="78" t="s">
         <v>1112</v>
-      </c>
-      <c r="F54" s="78" t="s">
-        <v>1113</v>
       </c>
       <c r="G54" s="153">
         <v>1</v>
@@ -30638,10 +30633,10 @@
         <v>1068</v>
       </c>
       <c r="E55" s="78" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F55" s="78" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="G55" s="153">
         <v>2</v>
@@ -30660,10 +30655,10 @@
         <v>1068</v>
       </c>
       <c r="E56" s="78" t="s">
+        <v>1114</v>
+      </c>
+      <c r="F56" s="78" t="s">
         <v>1115</v>
-      </c>
-      <c r="F56" s="78" t="s">
-        <v>1116</v>
       </c>
       <c r="G56" s="153">
         <v>3</v>
@@ -30682,10 +30677,10 @@
         <v>1068</v>
       </c>
       <c r="E57" s="78" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F57" s="78" t="s">
         <v>1117</v>
-      </c>
-      <c r="F57" s="78" t="s">
-        <v>1118</v>
       </c>
       <c r="G57" s="153">
         <v>4</v>
@@ -31913,8 +31908,8 @@
       <c r="G38" s="173">
         <v>1</v>
       </c>
-      <c r="H38" s="581"/>
-      <c r="I38" s="581"/>
+      <c r="H38" s="580"/>
+      <c r="I38" s="580"/>
     </row>
     <row r="39" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="169">
@@ -31934,8 +31929,8 @@
       <c r="G39" s="174">
         <v>2</v>
       </c>
-      <c r="H39" s="581"/>
-      <c r="I39" s="581"/>
+      <c r="H39" s="580"/>
+      <c r="I39" s="580"/>
     </row>
     <row r="40" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="169">
@@ -31955,8 +31950,8 @@
       <c r="G40" s="174">
         <v>3</v>
       </c>
-      <c r="H40" s="581"/>
-      <c r="I40" s="581"/>
+      <c r="H40" s="580"/>
+      <c r="I40" s="580"/>
     </row>
     <row r="41" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="169">
@@ -31976,8 +31971,8 @@
       <c r="G41" s="174">
         <v>4</v>
       </c>
-      <c r="H41" s="581"/>
-      <c r="I41" s="581"/>
+      <c r="H41" s="580"/>
+      <c r="I41" s="580"/>
     </row>
     <row r="42" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="169">
@@ -31991,14 +31986,14 @@
         <v>1073</v>
       </c>
       <c r="E42" s="171" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F42" s="171"/>
       <c r="G42" s="174">
         <v>5</v>
       </c>
-      <c r="H42" s="581"/>
-      <c r="I42" s="581"/>
+      <c r="H42" s="580"/>
+      <c r="I42" s="580"/>
     </row>
     <row r="43" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="169">
@@ -32018,8 +32013,8 @@
       <c r="G43" s="173">
         <v>1</v>
       </c>
-      <c r="H43" s="581"/>
-      <c r="I43" s="581"/>
+      <c r="H43" s="580"/>
+      <c r="I43" s="580"/>
     </row>
     <row r="44" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="169">
@@ -32039,8 +32034,8 @@
       <c r="G44" s="174">
         <v>2</v>
       </c>
-      <c r="H44" s="581"/>
-      <c r="I44" s="581"/>
+      <c r="H44" s="580"/>
+      <c r="I44" s="580"/>
     </row>
     <row r="45" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="169">
@@ -32060,8 +32055,8 @@
       <c r="G45" s="174">
         <v>3</v>
       </c>
-      <c r="H45" s="581"/>
-      <c r="I45" s="581"/>
+      <c r="H45" s="580"/>
+      <c r="I45" s="580"/>
     </row>
     <row r="46" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="169">
@@ -32081,8 +32076,8 @@
       <c r="G46" s="174">
         <v>4</v>
       </c>
-      <c r="H46" s="581"/>
-      <c r="I46" s="581"/>
+      <c r="H46" s="580"/>
+      <c r="I46" s="580"/>
     </row>
     <row r="47" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="169">
@@ -32096,14 +32091,14 @@
         <v>1073</v>
       </c>
       <c r="E47" s="171" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F47" s="171"/>
       <c r="G47" s="174">
         <v>5</v>
       </c>
-      <c r="H47" s="581"/>
-      <c r="I47" s="581"/>
+      <c r="H47" s="580"/>
+      <c r="I47" s="580"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -33234,7 +33229,7 @@
       </c>
       <c r="E53" s="141"/>
       <c r="F53" s="141" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="G53" s="172">
         <v>3</v>
@@ -33294,7 +33289,7 @@
       </c>
       <c r="E56" s="141"/>
       <c r="F56" s="141" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="G56" s="172">
         <v>3</v>
@@ -35396,17 +35391,17 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="582">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="583"/>
+      <c r="A24" s="581">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="582"/>
       <c r="C24" s="568" t="s">
         <v>1062</v>
       </c>
-      <c r="D24" s="584" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E24" s="585" t="s">
+      <c r="D24" s="583" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E24" s="584" t="s">
         <v>339</v>
       </c>
     </row>
@@ -35418,7 +35413,7 @@
       <c r="C25" s="62" t="s">
         <v>1062</v>
       </c>
-      <c r="D25" s="586" t="s">
+      <c r="D25" s="585" t="s">
         <v>936</v>
       </c>
       <c r="E25" s="115" t="s">
@@ -35433,7 +35428,7 @@
       <c r="C26" s="62" t="s">
         <v>1062</v>
       </c>
-      <c r="D26" s="586" t="s">
+      <c r="D26" s="585" t="s">
         <v>776</v>
       </c>
       <c r="E26" s="115" t="s">
@@ -35441,17 +35436,17 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="582">
-        <v>42736</v>
-      </c>
-      <c r="B27" s="583"/>
-      <c r="C27" s="587" t="s">
+      <c r="A27" s="581">
+        <v>42736</v>
+      </c>
+      <c r="B27" s="582"/>
+      <c r="C27" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D27" s="584" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E27" s="585" t="s">
+      <c r="D27" s="583" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E27" s="584" t="s">
         <v>339</v>
       </c>
     </row>
@@ -35463,7 +35458,7 @@
       <c r="C28" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D28" s="586" t="s">
+      <c r="D28" s="585" t="s">
         <v>936</v>
       </c>
       <c r="E28" s="115" t="s">
@@ -35478,7 +35473,7 @@
       <c r="C29" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D29" s="586" t="s">
+      <c r="D29" s="585" t="s">
         <v>776</v>
       </c>
       <c r="E29" s="115" t="s">
@@ -38561,128 +38556,128 @@
       </c>
     </row>
     <row r="170" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A170" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B170" s="589"/>
-      <c r="C170" s="587" t="s">
+      <c r="A170" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B170" s="588"/>
+      <c r="C170" s="586" t="s">
         <v>1062</v>
       </c>
-      <c r="D170" s="587" t="s">
+      <c r="D170" s="586" t="s">
         <v>100</v>
       </c>
-      <c r="E170" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F170" s="585" t="s">
+      <c r="E170" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F170" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A171" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B171" s="589"/>
-      <c r="C171" s="587" t="s">
+      <c r="A171" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B171" s="588"/>
+      <c r="C171" s="586" t="s">
         <v>1062</v>
       </c>
-      <c r="D171" s="587" t="s">
+      <c r="D171" s="586" t="s">
         <v>1068</v>
       </c>
-      <c r="E171" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F171" s="585" t="s">
+      <c r="E171" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F171" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A172" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B172" s="589"/>
-      <c r="C172" s="587" t="s">
+      <c r="A172" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B172" s="588"/>
+      <c r="C172" s="586" t="s">
         <v>1062</v>
       </c>
-      <c r="D172" s="587" t="s">
+      <c r="D172" s="586" t="s">
         <v>1071</v>
       </c>
-      <c r="E172" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F172" s="585" t="s">
+      <c r="E172" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F172" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A173" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B173" s="589"/>
-      <c r="C173" s="587" t="s">
+      <c r="A173" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B173" s="588"/>
+      <c r="C173" s="586" t="s">
         <v>1062</v>
       </c>
-      <c r="D173" s="587" t="s">
+      <c r="D173" s="586" t="s">
         <v>1073</v>
       </c>
-      <c r="E173" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F173" s="585" t="s">
+      <c r="E173" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F173" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A174" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B174" s="589"/>
-      <c r="C174" s="587" t="s">
+      <c r="A174" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B174" s="588"/>
+      <c r="C174" s="586" t="s">
         <v>1062</v>
       </c>
-      <c r="D174" s="587" t="s">
+      <c r="D174" s="586" t="s">
         <v>1075</v>
       </c>
-      <c r="E174" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F174" s="585" t="s">
+      <c r="E174" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F174" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A175" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B175" s="589"/>
-      <c r="C175" s="587" t="s">
+      <c r="A175" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B175" s="588"/>
+      <c r="C175" s="586" t="s">
         <v>1062</v>
       </c>
-      <c r="D175" s="587" t="s">
+      <c r="D175" s="586" t="s">
         <v>1077</v>
       </c>
-      <c r="E175" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F175" s="585" t="s">
+      <c r="E175" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F175" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A176" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B176" s="589"/>
-      <c r="C176" s="587" t="s">
+      <c r="A176" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B176" s="588"/>
+      <c r="C176" s="586" t="s">
         <v>1062</v>
       </c>
-      <c r="D176" s="587" t="s">
+      <c r="D176" s="586" t="s">
         <v>1079</v>
       </c>
-      <c r="E176" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F176" s="585" t="s">
+      <c r="E176" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F176" s="584" t="s">
         <v>339</v>
       </c>
     </row>
@@ -38903,56 +38898,56 @@
       </c>
     </row>
     <row r="189" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A189" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B189" s="589"/>
-      <c r="C189" s="587" t="s">
+      <c r="A189" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B189" s="588"/>
+      <c r="C189" s="586" t="s">
         <v>1062</v>
       </c>
-      <c r="D189" s="587" t="s">
+      <c r="D189" s="586" t="s">
         <v>1075</v>
       </c>
-      <c r="E189" s="583" t="s">
+      <c r="E189" s="582" t="s">
         <v>776</v>
       </c>
-      <c r="F189" s="585" t="s">
+      <c r="F189" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A190" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B190" s="589"/>
-      <c r="C190" s="587" t="s">
+      <c r="A190" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B190" s="588"/>
+      <c r="C190" s="586" t="s">
         <v>1062</v>
       </c>
-      <c r="D190" s="587" t="s">
+      <c r="D190" s="586" t="s">
         <v>1077</v>
       </c>
-      <c r="E190" s="583" t="s">
+      <c r="E190" s="582" t="s">
         <v>776</v>
       </c>
-      <c r="F190" s="585" t="s">
+      <c r="F190" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A191" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B191" s="589"/>
-      <c r="C191" s="587" t="s">
+      <c r="A191" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B191" s="588"/>
+      <c r="C191" s="586" t="s">
         <v>1062</v>
       </c>
-      <c r="D191" s="587" t="s">
+      <c r="D191" s="586" t="s">
         <v>1079</v>
       </c>
-      <c r="E191" s="583" t="s">
+      <c r="E191" s="582" t="s">
         <v>776</v>
       </c>
-      <c r="F191" s="585" t="s">
+      <c r="F191" s="584" t="s">
         <v>339</v>
       </c>
     </row>
@@ -38975,128 +38970,128 @@
       </c>
     </row>
     <row r="193" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A193" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B193" s="589"/>
-      <c r="C193" s="587" t="s">
+      <c r="A193" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B193" s="588"/>
+      <c r="C193" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D193" s="587" t="s">
+      <c r="D193" s="586" t="s">
         <v>100</v>
       </c>
-      <c r="E193" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F193" s="585" t="s">
+      <c r="E193" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F193" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A194" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B194" s="589"/>
-      <c r="C194" s="587" t="s">
+      <c r="A194" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B194" s="588"/>
+      <c r="C194" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D194" s="587" t="s">
+      <c r="D194" s="586" t="s">
         <v>1068</v>
       </c>
-      <c r="E194" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F194" s="585" t="s">
+      <c r="E194" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F194" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="195" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A195" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B195" s="589"/>
-      <c r="C195" s="587" t="s">
+      <c r="A195" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B195" s="588"/>
+      <c r="C195" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D195" s="587" t="s">
+      <c r="D195" s="586" t="s">
         <v>1071</v>
       </c>
-      <c r="E195" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F195" s="585" t="s">
+      <c r="E195" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F195" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A196" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B196" s="589"/>
-      <c r="C196" s="587" t="s">
+      <c r="A196" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B196" s="588"/>
+      <c r="C196" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D196" s="587" t="s">
+      <c r="D196" s="586" t="s">
         <v>1073</v>
       </c>
-      <c r="E196" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F196" s="585" t="s">
+      <c r="E196" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F196" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A197" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B197" s="590"/>
-      <c r="C197" s="587" t="s">
+      <c r="A197" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B197" s="589"/>
+      <c r="C197" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D197" s="587" t="s">
+      <c r="D197" s="586" t="s">
         <v>1075</v>
       </c>
-      <c r="E197" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F197" s="585" t="s">
+      <c r="E197" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F197" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A198" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B198" s="589"/>
-      <c r="C198" s="587" t="s">
+      <c r="A198" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B198" s="588"/>
+      <c r="C198" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D198" s="587" t="s">
+      <c r="D198" s="586" t="s">
         <v>1077</v>
       </c>
-      <c r="E198" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F198" s="585" t="s">
+      <c r="E198" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F198" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A199" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B199" s="589"/>
-      <c r="C199" s="587" t="s">
+      <c r="A199" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B199" s="588"/>
+      <c r="C199" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D199" s="587" t="s">
+      <c r="D199" s="586" t="s">
         <v>1079</v>
       </c>
-      <c r="E199" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F199" s="585" t="s">
+      <c r="E199" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F199" s="584" t="s">
         <v>339</v>
       </c>
     </row>
@@ -39317,56 +39312,56 @@
       </c>
     </row>
     <row r="212" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A212" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B212" s="589"/>
-      <c r="C212" s="587" t="s">
+      <c r="A212" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B212" s="588"/>
+      <c r="C212" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D212" s="587" t="s">
+      <c r="D212" s="586" t="s">
         <v>1075</v>
       </c>
-      <c r="E212" s="583" t="s">
+      <c r="E212" s="582" t="s">
         <v>776</v>
       </c>
-      <c r="F212" s="585" t="s">
+      <c r="F212" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A213" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B213" s="589"/>
-      <c r="C213" s="587" t="s">
+      <c r="A213" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B213" s="588"/>
+      <c r="C213" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D213" s="587" t="s">
+      <c r="D213" s="586" t="s">
         <v>1077</v>
       </c>
-      <c r="E213" s="583" t="s">
+      <c r="E213" s="582" t="s">
         <v>776</v>
       </c>
-      <c r="F213" s="585" t="s">
+      <c r="F213" s="584" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A214" s="588">
-        <v>42736</v>
-      </c>
-      <c r="B214" s="589"/>
-      <c r="C214" s="587" t="s">
+      <c r="A214" s="587">
+        <v>42736</v>
+      </c>
+      <c r="B214" s="588"/>
+      <c r="C214" s="586" t="s">
         <v>1065</v>
       </c>
-      <c r="D214" s="587" t="s">
+      <c r="D214" s="586" t="s">
         <v>1079</v>
       </c>
-      <c r="E214" s="583" t="s">
+      <c r="E214" s="582" t="s">
         <v>776</v>
       </c>
-      <c r="F214" s="585" t="s">
+      <c r="F214" s="584" t="s">
         <v>339</v>
       </c>
     </row>
@@ -39562,10 +39557,10 @@
         <v>1082</v>
       </c>
       <c r="C11" s="142" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D11" s="173" t="s">
         <v>1121</v>
-      </c>
-      <c r="D11" s="173" t="s">
-        <v>1122</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
@@ -39576,10 +39571,10 @@
         <v>1084</v>
       </c>
       <c r="C12" s="142" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D12" s="173" t="s">
         <v>1123</v>
-      </c>
-      <c r="D12" s="173" t="s">
-        <v>1124</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
@@ -39590,10 +39585,10 @@
         <v>1086</v>
       </c>
       <c r="C13" s="142" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D13" s="173" t="s">
         <v>1125</v>
-      </c>
-      <c r="D13" s="173" t="s">
-        <v>1126</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
@@ -39604,10 +39599,10 @@
         <v>1082</v>
       </c>
       <c r="C14" s="142" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D14" s="173" t="s">
         <v>1121</v>
-      </c>
-      <c r="D14" s="173" t="s">
-        <v>1122</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
@@ -39618,10 +39613,10 @@
         <v>1084</v>
       </c>
       <c r="C15" s="142" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D15" s="173" t="s">
         <v>1123</v>
-      </c>
-      <c r="D15" s="173" t="s">
-        <v>1124</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -39632,10 +39627,10 @@
         <v>1086</v>
       </c>
       <c r="C16" s="142" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D16" s="173" t="s">
         <v>1125</v>
-      </c>
-      <c r="D16" s="173" t="s">
-        <v>1126</v>
       </c>
     </row>
   </sheetData>
@@ -40999,20 +40994,20 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="582">
-        <v>42736</v>
-      </c>
-      <c r="B60" s="583"/>
-      <c r="C60" s="587" t="s">
+      <c r="A60" s="581">
+        <v>42736</v>
+      </c>
+      <c r="B60" s="582"/>
+      <c r="C60" s="586" t="s">
         <v>1062</v>
       </c>
       <c r="D60" s="568" t="s">
         <v>392</v>
       </c>
-      <c r="E60" s="584" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F60" s="585" t="s">
+      <c r="E60" s="583" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F60" s="584" t="s">
         <v>339</v>
       </c>
     </row>
@@ -41027,7 +41022,7 @@
       <c r="D61" s="62" t="s">
         <v>1088</v>
       </c>
-      <c r="E61" s="586" t="s">
+      <c r="E61" s="585" t="s">
         <v>936</v>
       </c>
       <c r="F61" s="115" t="s">
@@ -41045,7 +41040,7 @@
       <c r="D62" s="62" t="s">
         <v>392</v>
       </c>
-      <c r="E62" s="586" t="s">
+      <c r="E62" s="585" t="s">
         <v>776</v>
       </c>
       <c r="F62" s="115" t="s">
@@ -41063,7 +41058,7 @@
       <c r="D63" s="62" t="s">
         <v>1088</v>
       </c>
-      <c r="E63" s="586" t="s">
+      <c r="E63" s="585" t="s">
         <v>776</v>
       </c>
       <c r="F63" s="115" t="s">
@@ -41071,20 +41066,20 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="582">
+      <c r="A64" s="581">
         <v>42737</v>
       </c>
-      <c r="B64" s="583"/>
-      <c r="C64" s="587" t="s">
+      <c r="B64" s="582"/>
+      <c r="C64" s="586" t="s">
         <v>1065</v>
       </c>
       <c r="D64" s="568" t="s">
         <v>392</v>
       </c>
-      <c r="E64" s="584" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F64" s="585" t="s">
+      <c r="E64" s="583" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F64" s="584" t="s">
         <v>339</v>
       </c>
     </row>
@@ -41099,7 +41094,7 @@
       <c r="D65" s="568" t="s">
         <v>1089</v>
       </c>
-      <c r="E65" s="586" t="s">
+      <c r="E65" s="585" t="s">
         <v>936</v>
       </c>
       <c r="F65" s="115" t="s">
@@ -41117,7 +41112,7 @@
       <c r="D66" s="62" t="s">
         <v>392</v>
       </c>
-      <c r="E66" s="586" t="s">
+      <c r="E66" s="585" t="s">
         <v>776</v>
       </c>
       <c r="F66" s="115" t="s">
@@ -41135,7 +41130,7 @@
       <c r="D67" s="568" t="s">
         <v>1089</v>
       </c>
-      <c r="E67" s="586" t="s">
+      <c r="E67" s="585" t="s">
         <v>776</v>
       </c>
       <c r="F67" s="115" t="s">
@@ -41158,7 +41153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:CF47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:XFD47"/>
     </sheetView>
   </sheetViews>
@@ -42069,20 +42064,20 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="582">
-        <v>42736</v>
-      </c>
-      <c r="B42" s="583"/>
+      <c r="A42" s="581">
+        <v>42736</v>
+      </c>
+      <c r="B42" s="582"/>
       <c r="C42" s="568" t="s">
         <v>1062</v>
       </c>
       <c r="D42" s="568" t="s">
         <v>489</v>
       </c>
-      <c r="E42" s="583" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F42" s="585" t="s">
+      <c r="E42" s="582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F42" s="584" t="s">
         <v>339</v>
       </c>
     </row>
@@ -42133,8 +42128,8 @@
       <c r="D45" s="265" t="s">
         <v>489</v>
       </c>
-      <c r="E45" s="591" t="s">
-        <v>1120</v>
+      <c r="E45" s="590" t="s">
+        <v>1119</v>
       </c>
       <c r="F45" s="266" t="s">
         <v>339</v>

</xml_diff>

<commit_message>
ACA-68 - Use valid LiveFrom dates in ChallengeQuestion
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBD6678-5101-5741-B4E3-4003600BA8D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9402CB-F7D6-1144-B7B4-6CC8A91E0285}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -5741,7 +5741,6 @@
     <xf numFmtId="167" fontId="74" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="36" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5877,6 +5876,7 @@
     <xf numFmtId="1" fontId="21" fillId="21" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="36" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Explanatory Text" xfId="14" builtinId="53"/>
@@ -14919,7 +14919,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD29"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15494,8 +15494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE0C02E-59B7-9148-BB65-087866DFAC16}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15586,7 +15586,9 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="210" x14ac:dyDescent="0.15">
-      <c r="A4" s="540"/>
+      <c r="A4" s="591">
+        <v>44562</v>
+      </c>
       <c r="B4" s="17" t="s">
         <v>922</v>
       </c>
@@ -15605,7 +15607,7 @@
       <c r="G4" s="531" t="s">
         <v>849</v>
       </c>
-      <c r="H4" s="541" t="s">
+      <c r="H4" s="540" t="s">
         <v>1035</v>
       </c>
       <c r="I4" s="531" t="s">
@@ -15613,7 +15615,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="112" x14ac:dyDescent="0.15">
-      <c r="A5" s="540"/>
+      <c r="A5" s="591">
+        <v>44562</v>
+      </c>
       <c r="B5" s="17" t="s">
         <v>922</v>
       </c>
@@ -15632,7 +15636,7 @@
       <c r="G5" s="531" t="s">
         <v>849</v>
       </c>
-      <c r="H5" s="541" t="s">
+      <c r="H5" s="540" t="s">
         <v>1038</v>
       </c>
       <c r="I5" s="531" t="s">
@@ -15640,7 +15644,9 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="56" x14ac:dyDescent="0.15">
-      <c r="A6" s="540"/>
+      <c r="A6" s="591">
+        <v>44562</v>
+      </c>
       <c r="B6" s="17" t="s">
         <v>922</v>
       </c>
@@ -15659,7 +15665,7 @@
       <c r="G6" s="531" t="s">
         <v>849</v>
       </c>
-      <c r="H6" s="541" t="s">
+      <c r="H6" s="540" t="s">
         <v>1041</v>
       </c>
       <c r="I6" s="531" t="s">
@@ -15667,7 +15673,9 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="56" x14ac:dyDescent="0.15">
-      <c r="A7" s="540"/>
+      <c r="A7" s="591">
+        <v>44562</v>
+      </c>
       <c r="B7" s="17" t="s">
         <v>922</v>
       </c>
@@ -15684,7 +15692,7 @@
         <v>1045</v>
       </c>
       <c r="G7" s="531"/>
-      <c r="H7" s="541" t="s">
+      <c r="H7" s="540" t="s">
         <v>1041</v>
       </c>
       <c r="I7" s="531" t="s">
@@ -15692,8 +15700,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="42" x14ac:dyDescent="0.15">
-      <c r="A8" s="540"/>
-      <c r="B8" s="542" t="s">
+      <c r="A8" s="591">
+        <v>44562</v>
+      </c>
+      <c r="B8" s="541" t="s">
         <v>881</v>
       </c>
       <c r="C8" s="17" t="s">
@@ -15709,7 +15719,7 @@
         <v>56</v>
       </c>
       <c r="G8" s="531"/>
-      <c r="H8" s="541" t="s">
+      <c r="H8" s="540" t="s">
         <v>1048</v>
       </c>
       <c r="I8" s="531" t="s">
@@ -15717,54 +15727,60 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14" x14ac:dyDescent="0.15">
-      <c r="B9" s="569" t="s">
+      <c r="A9" s="591">
+        <v>44562</v>
+      </c>
+      <c r="B9" s="568" t="s">
         <v>1062</v>
       </c>
-      <c r="C9" s="570" t="s">
+      <c r="C9" s="569" t="s">
         <v>1033</v>
       </c>
-      <c r="D9" s="571">
+      <c r="D9" s="570">
         <v>4</v>
       </c>
-      <c r="E9" s="572" t="s">
+      <c r="E9" s="571" t="s">
         <v>1034</v>
       </c>
-      <c r="F9" s="573" t="s">
+      <c r="F9" s="572" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="572"/>
-      <c r="H9" s="572" t="s">
+      <c r="G9" s="571"/>
+      <c r="H9" s="571" t="s">
         <v>1104</v>
       </c>
-      <c r="I9" s="571" t="s">
+      <c r="I9" s="570" t="s">
         <v>1105</v>
       </c>
-      <c r="J9" s="572"/>
+      <c r="J9" s="571"/>
     </row>
     <row r="10" spans="1:10" ht="14" x14ac:dyDescent="0.15">
-      <c r="B10" s="569" t="s">
+      <c r="A10" s="591">
+        <v>44562</v>
+      </c>
+      <c r="B10" s="568" t="s">
         <v>1065</v>
       </c>
-      <c r="C10" s="570" t="s">
+      <c r="C10" s="569" t="s">
         <v>1033</v>
       </c>
-      <c r="D10" s="571">
+      <c r="D10" s="570">
         <v>5</v>
       </c>
-      <c r="E10" s="572" t="s">
+      <c r="E10" s="571" t="s">
         <v>1034</v>
       </c>
-      <c r="F10" s="573" t="s">
+      <c r="F10" s="572" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="572"/>
-      <c r="H10" s="572" t="s">
+      <c r="G10" s="571"/>
+      <c r="H10" s="571" t="s">
         <v>1104</v>
       </c>
-      <c r="I10" s="571" t="s">
+      <c r="I10" s="570" t="s">
         <v>1106</v>
       </c>
-      <c r="J10" s="572"/>
+      <c r="J10" s="571"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15775,7 +15791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:CR77"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A45" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A118" workbookViewId="0">
       <selection activeCell="A70" sqref="A70:XFD77"/>
     </sheetView>
   </sheetViews>
@@ -18294,7 +18310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:FH38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A37" sqref="A37:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -19295,7 +19311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J24" zoomScale="109" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A23" zoomScale="109" workbookViewId="0">
       <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
@@ -21105,86 +21121,86 @@
       <c r="T42" s="479"/>
     </row>
     <row r="43" spans="1:20" s="389" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="543">
-        <v>42736</v>
-      </c>
-      <c r="B43" s="544"/>
-      <c r="C43" s="544" t="s">
+      <c r="A43" s="542">
+        <v>42736</v>
+      </c>
+      <c r="B43" s="543"/>
+      <c r="C43" s="543" t="s">
         <v>1060</v>
       </c>
-      <c r="D43" s="551" t="s">
+      <c r="D43" s="550" t="s">
         <v>392</v>
       </c>
-      <c r="E43" s="551" t="s">
+      <c r="E43" s="550" t="s">
         <v>531</v>
       </c>
-      <c r="F43" s="545" t="s">
+      <c r="F43" s="544" t="s">
         <v>531</v>
       </c>
-      <c r="G43" s="546">
+      <c r="G43" s="545">
         <v>1</v>
       </c>
-      <c r="H43" s="547"/>
-      <c r="I43" s="547" t="s">
+      <c r="H43" s="546"/>
+      <c r="I43" s="546" t="s">
         <v>489</v>
       </c>
-      <c r="J43" s="548"/>
-      <c r="K43" s="548"/>
-      <c r="L43" s="548"/>
-      <c r="M43" s="548"/>
-      <c r="N43" s="548"/>
-      <c r="O43" s="548"/>
-      <c r="P43" s="547" t="s">
+      <c r="J43" s="547"/>
+      <c r="K43" s="547"/>
+      <c r="L43" s="547"/>
+      <c r="M43" s="547"/>
+      <c r="N43" s="547"/>
+      <c r="O43" s="547"/>
+      <c r="P43" s="546" t="s">
         <v>26</v>
       </c>
-      <c r="Q43" s="547" t="s">
+      <c r="Q43" s="546" t="s">
         <v>533</v>
       </c>
-      <c r="R43" s="549"/>
-      <c r="S43" s="549"/>
-      <c r="T43" s="550"/>
+      <c r="R43" s="548"/>
+      <c r="S43" s="548"/>
+      <c r="T43" s="549"/>
     </row>
     <row r="44" spans="1:20" s="389" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="543">
-        <v>42736</v>
-      </c>
-      <c r="B44" s="544"/>
-      <c r="C44" s="544" t="s">
+      <c r="A44" s="542">
+        <v>42736</v>
+      </c>
+      <c r="B44" s="543"/>
+      <c r="C44" s="543" t="s">
         <v>1060</v>
       </c>
-      <c r="D44" s="551" t="s">
+      <c r="D44" s="550" t="s">
         <v>941</v>
       </c>
-      <c r="E44" s="551" t="s">
+      <c r="E44" s="550" t="s">
         <v>942</v>
       </c>
-      <c r="F44" s="545" t="s">
+      <c r="F44" s="544" t="s">
         <v>942</v>
       </c>
-      <c r="G44" s="546">
+      <c r="G44" s="545">
         <v>2</v>
       </c>
-      <c r="H44" s="547" t="s">
+      <c r="H44" s="546" t="s">
         <v>489</v>
       </c>
-      <c r="I44" s="547" t="s">
+      <c r="I44" s="546" t="s">
         <v>1058</v>
       </c>
-      <c r="J44" s="548"/>
-      <c r="K44" s="548"/>
-      <c r="L44" s="548"/>
-      <c r="M44" s="548"/>
-      <c r="N44" s="548"/>
-      <c r="O44" s="548"/>
-      <c r="P44" s="547" t="s">
+      <c r="J44" s="547"/>
+      <c r="K44" s="547"/>
+      <c r="L44" s="547"/>
+      <c r="M44" s="547"/>
+      <c r="N44" s="547"/>
+      <c r="O44" s="547"/>
+      <c r="P44" s="546" t="s">
         <v>26</v>
       </c>
-      <c r="Q44" s="547" t="s">
+      <c r="Q44" s="546" t="s">
         <v>533</v>
       </c>
-      <c r="R44" s="549"/>
-      <c r="S44" s="549"/>
-      <c r="T44" s="550"/>
+      <c r="R44" s="548"/>
+      <c r="S44" s="548"/>
+      <c r="T44" s="549"/>
     </row>
     <row r="45" spans="1:20" s="481" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="480">
@@ -21470,8 +21486,8 @@
       <c r="A52" s="60">
         <v>42736</v>
       </c>
-      <c r="B52" s="574"/>
-      <c r="C52" s="575" t="s">
+      <c r="B52" s="573"/>
+      <c r="C52" s="574" t="s">
         <v>1062</v>
       </c>
       <c r="D52" s="103" t="s">
@@ -21481,29 +21497,29 @@
         <v>1108</v>
       </c>
       <c r="F52" s="103"/>
-      <c r="G52" s="576">
+      <c r="G52" s="575">
         <v>1</v>
       </c>
       <c r="H52" s="103"/>
       <c r="I52" s="103" t="s">
         <v>489</v>
       </c>
-      <c r="J52" s="577"/>
-      <c r="K52" s="578"/>
-      <c r="L52" s="578"/>
-      <c r="M52" s="578"/>
-      <c r="N52" s="578"/>
-      <c r="O52" s="578"/>
+      <c r="J52" s="576"/>
+      <c r="K52" s="577"/>
+      <c r="L52" s="577"/>
+      <c r="M52" s="577"/>
+      <c r="N52" s="577"/>
+      <c r="O52" s="577"/>
       <c r="P52" s="103" t="s">
         <v>26</v>
       </c>
       <c r="Q52" s="103" t="s">
         <v>533</v>
       </c>
-      <c r="R52" s="579" t="s">
+      <c r="R52" s="578" t="s">
         <v>533</v>
       </c>
-      <c r="S52" s="579"/>
+      <c r="S52" s="578"/>
       <c r="T52" s="105"/>
     </row>
     <row r="53" spans="1:20" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -21565,29 +21581,29 @@
         <v>1108</v>
       </c>
       <c r="F54" s="103"/>
-      <c r="G54" s="576">
+      <c r="G54" s="575">
         <v>1</v>
       </c>
       <c r="H54" s="103"/>
       <c r="I54" s="103" t="s">
         <v>489</v>
       </c>
-      <c r="J54" s="577"/>
-      <c r="K54" s="578"/>
-      <c r="L54" s="578"/>
-      <c r="M54" s="578"/>
-      <c r="N54" s="578"/>
-      <c r="O54" s="578"/>
+      <c r="J54" s="576"/>
+      <c r="K54" s="577"/>
+      <c r="L54" s="577"/>
+      <c r="M54" s="577"/>
+      <c r="N54" s="577"/>
+      <c r="O54" s="577"/>
       <c r="P54" s="103" t="s">
         <v>26</v>
       </c>
       <c r="Q54" s="103" t="s">
         <v>533</v>
       </c>
-      <c r="R54" s="579" t="s">
+      <c r="R54" s="578" t="s">
         <v>533</v>
       </c>
-      <c r="S54" s="579"/>
+      <c r="S54" s="578"/>
       <c r="T54" s="105"/>
     </row>
     <row r="55" spans="1:20" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -21598,7 +21614,7 @@
       <c r="C55" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D55" s="568" t="s">
+      <c r="D55" s="567" t="s">
         <v>1089</v>
       </c>
       <c r="E55" s="62" t="s">
@@ -21618,7 +21634,7 @@
       </c>
       <c r="J55" s="117"/>
       <c r="K55" s="114"/>
-      <c r="L55" s="591" t="s">
+      <c r="L55" s="590" t="s">
         <v>1126</v>
       </c>
       <c r="M55" s="114"/>
@@ -21662,8 +21678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R192"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A158" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A185" sqref="A185:XFD192"/>
+    <sheetView showGridLines="0" topLeftCell="A172" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D206" sqref="D206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -28228,444 +28244,444 @@
       <c r="R161" s="17"/>
     </row>
     <row r="162" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="552">
+      <c r="A162" s="551">
         <v>42741</v>
       </c>
-      <c r="B162" s="553"/>
-      <c r="C162" s="545" t="s">
+      <c r="B162" s="552"/>
+      <c r="C162" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D162" s="547" t="s">
+      <c r="D162" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E162" s="545" t="s">
+      <c r="E162" s="544" t="s">
         <v>54</v>
       </c>
-      <c r="F162" s="544">
+      <c r="F162" s="543">
         <v>1</v>
       </c>
-      <c r="G162" s="545" t="s">
+      <c r="G162" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H162" s="554" t="s">
+      <c r="H162" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I162" s="554" t="s">
+      <c r="I162" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J162" s="405">
         <v>1</v>
       </c>
-      <c r="K162" s="544"/>
-      <c r="L162" s="544"/>
-      <c r="M162" s="555"/>
-      <c r="N162" s="544"/>
-      <c r="O162" s="544"/>
-      <c r="P162" s="554" t="s">
+      <c r="K162" s="543"/>
+      <c r="L162" s="543"/>
+      <c r="M162" s="554"/>
+      <c r="N162" s="543"/>
+      <c r="O162" s="543"/>
+      <c r="P162" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q162" s="544"/>
-      <c r="R162" s="556"/>
+      <c r="Q162" s="543"/>
+      <c r="R162" s="555"/>
     </row>
     <row r="163" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="552">
+      <c r="A163" s="551">
         <v>42741</v>
       </c>
-      <c r="B163" s="553"/>
-      <c r="C163" s="545" t="s">
+      <c r="B163" s="552"/>
+      <c r="C163" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D163" s="547" t="s">
+      <c r="D163" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E163" s="545" t="s">
+      <c r="E163" s="544" t="s">
         <v>57</v>
       </c>
-      <c r="F163" s="544">
+      <c r="F163" s="543">
         <v>2</v>
       </c>
-      <c r="G163" s="545" t="s">
+      <c r="G163" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H163" s="554" t="s">
+      <c r="H163" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I163" s="554" t="s">
+      <c r="I163" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J163" s="405">
         <v>2</v>
       </c>
-      <c r="K163" s="544"/>
-      <c r="L163" s="544"/>
-      <c r="M163" s="555"/>
-      <c r="N163" s="544"/>
-      <c r="O163" s="544"/>
-      <c r="P163" s="554" t="s">
+      <c r="K163" s="543"/>
+      <c r="L163" s="543"/>
+      <c r="M163" s="554"/>
+      <c r="N163" s="543"/>
+      <c r="O163" s="543"/>
+      <c r="P163" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q163" s="544"/>
-      <c r="R163" s="556"/>
+      <c r="Q163" s="543"/>
+      <c r="R163" s="555"/>
     </row>
     <row r="164" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="552">
+      <c r="A164" s="551">
         <v>42741</v>
       </c>
-      <c r="B164" s="553"/>
-      <c r="C164" s="545" t="s">
+      <c r="B164" s="552"/>
+      <c r="C164" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D164" s="547" t="s">
+      <c r="D164" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E164" s="545" t="s">
+      <c r="E164" s="544" t="s">
         <v>60</v>
       </c>
-      <c r="F164" s="544">
+      <c r="F164" s="543">
         <v>3</v>
       </c>
-      <c r="G164" s="545" t="s">
+      <c r="G164" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H164" s="554" t="s">
+      <c r="H164" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I164" s="554" t="s">
+      <c r="I164" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J164" s="405">
         <v>3</v>
       </c>
-      <c r="K164" s="544"/>
-      <c r="L164" s="544"/>
-      <c r="M164" s="555"/>
-      <c r="N164" s="544"/>
-      <c r="O164" s="544"/>
-      <c r="P164" s="554" t="s">
+      <c r="K164" s="543"/>
+      <c r="L164" s="543"/>
+      <c r="M164" s="554"/>
+      <c r="N164" s="543"/>
+      <c r="O164" s="543"/>
+      <c r="P164" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q164" s="544"/>
-      <c r="R164" s="556"/>
+      <c r="Q164" s="543"/>
+      <c r="R164" s="555"/>
     </row>
     <row r="165" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="552">
+      <c r="A165" s="551">
         <v>42741</v>
       </c>
-      <c r="B165" s="553"/>
-      <c r="C165" s="545" t="s">
+      <c r="B165" s="552"/>
+      <c r="C165" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D165" s="547" t="s">
+      <c r="D165" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E165" s="545" t="s">
+      <c r="E165" s="544" t="s">
         <v>63</v>
       </c>
-      <c r="F165" s="544">
+      <c r="F165" s="543">
         <v>4</v>
       </c>
-      <c r="G165" s="545" t="s">
+      <c r="G165" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H165" s="554" t="s">
+      <c r="H165" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I165" s="554" t="s">
+      <c r="I165" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J165" s="405">
         <v>4</v>
       </c>
-      <c r="K165" s="544"/>
-      <c r="L165" s="544"/>
-      <c r="M165" s="555"/>
-      <c r="N165" s="544"/>
-      <c r="O165" s="544"/>
-      <c r="P165" s="554" t="s">
+      <c r="K165" s="543"/>
+      <c r="L165" s="543"/>
+      <c r="M165" s="554"/>
+      <c r="N165" s="543"/>
+      <c r="O165" s="543"/>
+      <c r="P165" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q165" s="544"/>
-      <c r="R165" s="556"/>
+      <c r="Q165" s="543"/>
+      <c r="R165" s="555"/>
     </row>
     <row r="166" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="552">
+      <c r="A166" s="551">
         <v>42741</v>
       </c>
-      <c r="B166" s="553"/>
-      <c r="C166" s="545" t="s">
+      <c r="B166" s="552"/>
+      <c r="C166" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D166" s="547" t="s">
+      <c r="D166" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E166" s="545" t="s">
+      <c r="E166" s="544" t="s">
         <v>66</v>
       </c>
-      <c r="F166" s="544">
+      <c r="F166" s="543">
         <v>5</v>
       </c>
-      <c r="G166" s="545" t="s">
+      <c r="G166" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H166" s="554" t="s">
+      <c r="H166" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I166" s="554" t="s">
+      <c r="I166" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J166" s="405">
         <v>5</v>
       </c>
-      <c r="K166" s="544"/>
-      <c r="L166" s="544"/>
-      <c r="M166" s="555"/>
-      <c r="N166" s="544"/>
-      <c r="O166" s="544"/>
-      <c r="P166" s="554" t="s">
+      <c r="K166" s="543"/>
+      <c r="L166" s="543"/>
+      <c r="M166" s="554"/>
+      <c r="N166" s="543"/>
+      <c r="O166" s="543"/>
+      <c r="P166" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q166" s="544"/>
-      <c r="R166" s="556"/>
+      <c r="Q166" s="543"/>
+      <c r="R166" s="555"/>
     </row>
     <row r="167" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A167" s="552">
+      <c r="A167" s="551">
         <v>42741</v>
       </c>
-      <c r="B167" s="553"/>
-      <c r="C167" s="545" t="s">
+      <c r="B167" s="552"/>
+      <c r="C167" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D167" s="547" t="s">
+      <c r="D167" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E167" s="545" t="s">
+      <c r="E167" s="544" t="s">
         <v>69</v>
       </c>
-      <c r="F167" s="544">
+      <c r="F167" s="543">
         <v>6</v>
       </c>
-      <c r="G167" s="545" t="s">
+      <c r="G167" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H167" s="554" t="s">
+      <c r="H167" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I167" s="554" t="s">
+      <c r="I167" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J167" s="405">
         <v>6</v>
       </c>
-      <c r="K167" s="544"/>
-      <c r="L167" s="544"/>
-      <c r="M167" s="555"/>
-      <c r="N167" s="544"/>
-      <c r="O167" s="544"/>
-      <c r="P167" s="554" t="s">
+      <c r="K167" s="543"/>
+      <c r="L167" s="543"/>
+      <c r="M167" s="554"/>
+      <c r="N167" s="543"/>
+      <c r="O167" s="543"/>
+      <c r="P167" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q167" s="544"/>
-      <c r="R167" s="556"/>
+      <c r="Q167" s="543"/>
+      <c r="R167" s="555"/>
     </row>
     <row r="168" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A168" s="552">
+      <c r="A168" s="551">
         <v>42741</v>
       </c>
-      <c r="B168" s="553"/>
-      <c r="C168" s="545" t="s">
+      <c r="B168" s="552"/>
+      <c r="C168" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D168" s="547" t="s">
+      <c r="D168" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E168" s="545" t="s">
+      <c r="E168" s="544" t="s">
         <v>72</v>
       </c>
-      <c r="F168" s="544">
+      <c r="F168" s="543">
         <v>7</v>
       </c>
-      <c r="G168" s="545" t="s">
+      <c r="G168" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H168" s="554" t="s">
+      <c r="H168" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I168" s="554" t="s">
+      <c r="I168" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J168" s="405">
         <v>7</v>
       </c>
-      <c r="K168" s="544"/>
-      <c r="L168" s="544"/>
-      <c r="M168" s="555"/>
-      <c r="N168" s="544"/>
-      <c r="O168" s="544"/>
-      <c r="P168" s="554" t="s">
+      <c r="K168" s="543"/>
+      <c r="L168" s="543"/>
+      <c r="M168" s="554"/>
+      <c r="N168" s="543"/>
+      <c r="O168" s="543"/>
+      <c r="P168" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q168" s="544"/>
-      <c r="R168" s="556"/>
+      <c r="Q168" s="543"/>
+      <c r="R168" s="555"/>
     </row>
     <row r="169" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A169" s="552">
+      <c r="A169" s="551">
         <v>42741</v>
       </c>
-      <c r="B169" s="553"/>
-      <c r="C169" s="545" t="s">
+      <c r="B169" s="552"/>
+      <c r="C169" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D169" s="547" t="s">
+      <c r="D169" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E169" s="545" t="s">
+      <c r="E169" s="544" t="s">
         <v>83</v>
       </c>
-      <c r="F169" s="544">
+      <c r="F169" s="543">
         <v>8</v>
       </c>
-      <c r="G169" s="545" t="s">
+      <c r="G169" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H169" s="554" t="s">
+      <c r="H169" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I169" s="554" t="s">
+      <c r="I169" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J169" s="405">
         <v>8</v>
       </c>
-      <c r="K169" s="544"/>
-      <c r="L169" s="544"/>
-      <c r="M169" s="555"/>
-      <c r="N169" s="544"/>
-      <c r="O169" s="544"/>
-      <c r="P169" s="554" t="s">
+      <c r="K169" s="543"/>
+      <c r="L169" s="543"/>
+      <c r="M169" s="554"/>
+      <c r="N169" s="543"/>
+      <c r="O169" s="543"/>
+      <c r="P169" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q169" s="544"/>
-      <c r="R169" s="556"/>
+      <c r="Q169" s="543"/>
+      <c r="R169" s="555"/>
     </row>
     <row r="170" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A170" s="552">
+      <c r="A170" s="551">
         <v>42741</v>
       </c>
-      <c r="B170" s="553"/>
-      <c r="C170" s="545" t="s">
+      <c r="B170" s="552"/>
+      <c r="C170" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D170" s="547" t="s">
+      <c r="D170" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E170" s="545" t="s">
+      <c r="E170" s="544" t="s">
         <v>87</v>
       </c>
-      <c r="F170" s="544">
+      <c r="F170" s="543">
         <v>9</v>
       </c>
-      <c r="G170" s="545" t="s">
+      <c r="G170" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H170" s="554" t="s">
+      <c r="H170" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I170" s="554" t="s">
+      <c r="I170" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J170" s="405">
         <v>9</v>
       </c>
-      <c r="K170" s="544"/>
-      <c r="L170" s="544"/>
-      <c r="M170" s="555"/>
-      <c r="N170" s="544"/>
-      <c r="O170" s="544"/>
-      <c r="P170" s="554" t="s">
+      <c r="K170" s="543"/>
+      <c r="L170" s="543"/>
+      <c r="M170" s="554"/>
+      <c r="N170" s="543"/>
+      <c r="O170" s="543"/>
+      <c r="P170" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q170" s="544"/>
-      <c r="R170" s="556"/>
+      <c r="Q170" s="543"/>
+      <c r="R170" s="555"/>
     </row>
     <row r="171" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A171" s="552">
+      <c r="A171" s="551">
         <v>42741</v>
       </c>
-      <c r="B171" s="553"/>
-      <c r="C171" s="545" t="s">
+      <c r="B171" s="552"/>
+      <c r="C171" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D171" s="547" t="s">
+      <c r="D171" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E171" s="545" t="s">
+      <c r="E171" s="544" t="s">
         <v>93</v>
       </c>
-      <c r="F171" s="544">
+      <c r="F171" s="543">
         <v>10</v>
       </c>
-      <c r="G171" s="545" t="s">
+      <c r="G171" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H171" s="554" t="s">
+      <c r="H171" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I171" s="554" t="s">
+      <c r="I171" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J171" s="405">
         <v>10</v>
       </c>
-      <c r="K171" s="544"/>
-      <c r="L171" s="544"/>
-      <c r="M171" s="555"/>
-      <c r="N171" s="544"/>
-      <c r="O171" s="544"/>
-      <c r="P171" s="554" t="s">
+      <c r="K171" s="543"/>
+      <c r="L171" s="543"/>
+      <c r="M171" s="554"/>
+      <c r="N171" s="543"/>
+      <c r="O171" s="543"/>
+      <c r="P171" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q171" s="544"/>
-      <c r="R171" s="556"/>
+      <c r="Q171" s="543"/>
+      <c r="R171" s="555"/>
     </row>
     <row r="172" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A172" s="552">
+      <c r="A172" s="551">
         <v>42741</v>
       </c>
-      <c r="B172" s="553"/>
-      <c r="C172" s="545" t="s">
+      <c r="B172" s="552"/>
+      <c r="C172" s="544" t="s">
         <v>1060</v>
       </c>
-      <c r="D172" s="547" t="s">
+      <c r="D172" s="546" t="s">
         <v>392</v>
       </c>
-      <c r="E172" s="545" t="s">
+      <c r="E172" s="544" t="s">
         <v>96</v>
       </c>
-      <c r="F172" s="544">
+      <c r="F172" s="543">
         <v>11</v>
       </c>
-      <c r="G172" s="545" t="s">
+      <c r="G172" s="544" t="s">
         <v>375</v>
       </c>
-      <c r="H172" s="554" t="s">
+      <c r="H172" s="553" t="s">
         <v>597</v>
       </c>
-      <c r="I172" s="554" t="s">
+      <c r="I172" s="553" t="s">
         <v>1059</v>
       </c>
       <c r="J172" s="405">
         <v>11</v>
       </c>
-      <c r="K172" s="544"/>
-      <c r="L172" s="544"/>
-      <c r="M172" s="555"/>
-      <c r="N172" s="544"/>
-      <c r="O172" s="544"/>
-      <c r="P172" s="554" t="s">
+      <c r="K172" s="543"/>
+      <c r="L172" s="543"/>
+      <c r="M172" s="554"/>
+      <c r="N172" s="543"/>
+      <c r="O172" s="543"/>
+      <c r="P172" s="553" t="s">
         <v>836</v>
       </c>
-      <c r="Q172" s="544"/>
-      <c r="R172" s="556"/>
+      <c r="Q172" s="543"/>
+      <c r="R172" s="555"/>
     </row>
     <row r="173" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A173" s="425">
@@ -29425,7 +29441,7 @@
       <c r="C192" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D192" s="568" t="s">
+      <c r="D192" s="567" t="s">
         <v>1089</v>
       </c>
       <c r="E192" s="65" t="s">
@@ -29476,8 +29492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD57"/>
+    <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30493,11 +30509,11 @@
       </c>
     </row>
     <row r="49" spans="1:8" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="557">
+      <c r="A49" s="556">
         <v>42746</v>
       </c>
       <c r="B49" s="393"/>
-      <c r="C49" s="558" t="s">
+      <c r="C49" s="557" t="s">
         <v>1060</v>
       </c>
       <c r="D49" s="393" t="s">
@@ -31872,21 +31888,21 @@
       </c>
     </row>
     <row r="37" spans="1:123" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="559">
-        <v>42736</v>
-      </c>
-      <c r="B37" s="560"/>
-      <c r="C37" s="561" t="s">
+      <c r="A37" s="558">
+        <v>42736</v>
+      </c>
+      <c r="B37" s="559"/>
+      <c r="C37" s="560" t="s">
         <v>1060</v>
       </c>
-      <c r="D37" s="561" t="s">
+      <c r="D37" s="560" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="562" t="s">
+      <c r="E37" s="561" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="562"/>
-      <c r="G37" s="563">
+      <c r="F37" s="561"/>
+      <c r="G37" s="562">
         <v>1</v>
       </c>
     </row>
@@ -31908,8 +31924,8 @@
       <c r="G38" s="173">
         <v>1</v>
       </c>
-      <c r="H38" s="580"/>
-      <c r="I38" s="580"/>
+      <c r="H38" s="579"/>
+      <c r="I38" s="579"/>
     </row>
     <row r="39" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="169">
@@ -31929,8 +31945,8 @@
       <c r="G39" s="174">
         <v>2</v>
       </c>
-      <c r="H39" s="580"/>
-      <c r="I39" s="580"/>
+      <c r="H39" s="579"/>
+      <c r="I39" s="579"/>
     </row>
     <row r="40" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="169">
@@ -31950,8 +31966,8 @@
       <c r="G40" s="174">
         <v>3</v>
       </c>
-      <c r="H40" s="580"/>
-      <c r="I40" s="580"/>
+      <c r="H40" s="579"/>
+      <c r="I40" s="579"/>
     </row>
     <row r="41" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="169">
@@ -31971,8 +31987,8 @@
       <c r="G41" s="174">
         <v>4</v>
       </c>
-      <c r="H41" s="580"/>
-      <c r="I41" s="580"/>
+      <c r="H41" s="579"/>
+      <c r="I41" s="579"/>
     </row>
     <row r="42" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="169">
@@ -31992,8 +32008,8 @@
       <c r="G42" s="174">
         <v>5</v>
       </c>
-      <c r="H42" s="580"/>
-      <c r="I42" s="580"/>
+      <c r="H42" s="579"/>
+      <c r="I42" s="579"/>
     </row>
     <row r="43" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="169">
@@ -32013,8 +32029,8 @@
       <c r="G43" s="173">
         <v>1</v>
       </c>
-      <c r="H43" s="580"/>
-      <c r="I43" s="580"/>
+      <c r="H43" s="579"/>
+      <c r="I43" s="579"/>
     </row>
     <row r="44" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="169">
@@ -32034,8 +32050,8 @@
       <c r="G44" s="174">
         <v>2</v>
       </c>
-      <c r="H44" s="580"/>
-      <c r="I44" s="580"/>
+      <c r="H44" s="579"/>
+      <c r="I44" s="579"/>
     </row>
     <row r="45" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="169">
@@ -32055,8 +32071,8 @@
       <c r="G45" s="174">
         <v>3</v>
       </c>
-      <c r="H45" s="580"/>
-      <c r="I45" s="580"/>
+      <c r="H45" s="579"/>
+      <c r="I45" s="579"/>
     </row>
     <row r="46" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="169">
@@ -32076,8 +32092,8 @@
       <c r="G46" s="174">
         <v>4</v>
       </c>
-      <c r="H46" s="580"/>
-      <c r="I46" s="580"/>
+      <c r="H46" s="579"/>
+      <c r="I46" s="579"/>
     </row>
     <row r="47" spans="1:123" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="169">
@@ -32097,8 +32113,8 @@
       <c r="G47" s="174">
         <v>5</v>
       </c>
-      <c r="H47" s="580"/>
-      <c r="I47" s="580"/>
+      <c r="H47" s="579"/>
+      <c r="I47" s="579"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -32121,8 +32137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD56"/>
+    <sheetView showGridLines="0" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -33158,11 +33174,11 @@
       </c>
     </row>
     <row r="50" spans="1:8" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="557">
+      <c r="A50" s="556">
         <v>42746</v>
       </c>
       <c r="B50" s="393"/>
-      <c r="C50" s="558" t="s">
+      <c r="C50" s="557" t="s">
         <v>1060</v>
       </c>
       <c r="D50" s="393" t="s">
@@ -33437,7 +33453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:BL61"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A47" workbookViewId="0">
       <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
@@ -34729,21 +34745,21 @@
       </c>
     </row>
     <row r="55" spans="1:64" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="559">
-        <v>42736</v>
-      </c>
-      <c r="B55" s="560"/>
-      <c r="C55" s="561" t="s">
+      <c r="A55" s="558">
+        <v>42736</v>
+      </c>
+      <c r="B55" s="559"/>
+      <c r="C55" s="560" t="s">
         <v>1060</v>
       </c>
-      <c r="D55" s="561" t="s">
+      <c r="D55" s="560" t="s">
         <v>54</v>
       </c>
-      <c r="E55" s="562"/>
-      <c r="F55" s="562" t="s">
+      <c r="E55" s="561"/>
+      <c r="F55" s="561" t="s">
         <v>55</v>
       </c>
-      <c r="G55" s="563">
+      <c r="G55" s="562">
         <v>1</v>
       </c>
     </row>
@@ -35028,7 +35044,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -35368,7 +35384,7 @@
       <c r="C22" s="265" t="s">
         <v>1060</v>
       </c>
-      <c r="D22" s="564" t="s">
+      <c r="D22" s="563" t="s">
         <v>776</v>
       </c>
       <c r="E22" s="125" t="s">
@@ -35391,17 +35407,17 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="581">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="582"/>
-      <c r="C24" s="568" t="s">
+      <c r="A24" s="580">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="581"/>
+      <c r="C24" s="567" t="s">
         <v>1062</v>
       </c>
-      <c r="D24" s="583" t="s">
+      <c r="D24" s="582" t="s">
         <v>1119</v>
       </c>
-      <c r="E24" s="584" t="s">
+      <c r="E24" s="583" t="s">
         <v>339</v>
       </c>
     </row>
@@ -35413,7 +35429,7 @@
       <c r="C25" s="62" t="s">
         <v>1062</v>
       </c>
-      <c r="D25" s="585" t="s">
+      <c r="D25" s="584" t="s">
         <v>936</v>
       </c>
       <c r="E25" s="115" t="s">
@@ -35428,7 +35444,7 @@
       <c r="C26" s="62" t="s">
         <v>1062</v>
       </c>
-      <c r="D26" s="585" t="s">
+      <c r="D26" s="584" t="s">
         <v>776</v>
       </c>
       <c r="E26" s="115" t="s">
@@ -35436,17 +35452,17 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="581">
-        <v>42736</v>
-      </c>
-      <c r="B27" s="582"/>
-      <c r="C27" s="586" t="s">
+      <c r="A27" s="580">
+        <v>42736</v>
+      </c>
+      <c r="B27" s="581"/>
+      <c r="C27" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D27" s="583" t="s">
+      <c r="D27" s="582" t="s">
         <v>1119</v>
       </c>
-      <c r="E27" s="584" t="s">
+      <c r="E27" s="583" t="s">
         <v>339</v>
       </c>
     </row>
@@ -35458,7 +35474,7 @@
       <c r="C28" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D28" s="585" t="s">
+      <c r="D28" s="584" t="s">
         <v>936</v>
       </c>
       <c r="E28" s="115" t="s">
@@ -35473,7 +35489,7 @@
       <c r="C29" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D29" s="585" t="s">
+      <c r="D29" s="584" t="s">
         <v>776</v>
       </c>
       <c r="E29" s="115" t="s">
@@ -35496,8 +35512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F215"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A178" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170:XFD215"/>
+    <sheetView showGridLines="0" topLeftCell="A182" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E219" sqref="E219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -38556,128 +38572,128 @@
       </c>
     </row>
     <row r="170" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A170" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B170" s="588"/>
-      <c r="C170" s="586" t="s">
+      <c r="A170" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B170" s="587"/>
+      <c r="C170" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D170" s="586" t="s">
+      <c r="D170" s="585" t="s">
         <v>100</v>
       </c>
-      <c r="E170" s="582" t="s">
+      <c r="E170" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F170" s="584" t="s">
+      <c r="F170" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A171" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B171" s="588"/>
-      <c r="C171" s="586" t="s">
+      <c r="A171" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B171" s="587"/>
+      <c r="C171" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D171" s="586" t="s">
+      <c r="D171" s="585" t="s">
         <v>1068</v>
       </c>
-      <c r="E171" s="582" t="s">
+      <c r="E171" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F171" s="584" t="s">
+      <c r="F171" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A172" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B172" s="588"/>
-      <c r="C172" s="586" t="s">
+      <c r="A172" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B172" s="587"/>
+      <c r="C172" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D172" s="586" t="s">
+      <c r="D172" s="585" t="s">
         <v>1071</v>
       </c>
-      <c r="E172" s="582" t="s">
+      <c r="E172" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F172" s="584" t="s">
+      <c r="F172" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A173" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B173" s="588"/>
-      <c r="C173" s="586" t="s">
+      <c r="A173" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B173" s="587"/>
+      <c r="C173" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D173" s="586" t="s">
+      <c r="D173" s="585" t="s">
         <v>1073</v>
       </c>
-      <c r="E173" s="582" t="s">
+      <c r="E173" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F173" s="584" t="s">
+      <c r="F173" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A174" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B174" s="588"/>
-      <c r="C174" s="586" t="s">
+      <c r="A174" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B174" s="587"/>
+      <c r="C174" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D174" s="586" t="s">
+      <c r="D174" s="585" t="s">
         <v>1075</v>
       </c>
-      <c r="E174" s="582" t="s">
+      <c r="E174" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F174" s="584" t="s">
+      <c r="F174" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A175" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B175" s="588"/>
-      <c r="C175" s="586" t="s">
+      <c r="A175" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B175" s="587"/>
+      <c r="C175" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D175" s="586" t="s">
+      <c r="D175" s="585" t="s">
         <v>1077</v>
       </c>
-      <c r="E175" s="582" t="s">
+      <c r="E175" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F175" s="584" t="s">
+      <c r="F175" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A176" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B176" s="588"/>
-      <c r="C176" s="586" t="s">
+      <c r="A176" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B176" s="587"/>
+      <c r="C176" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D176" s="586" t="s">
+      <c r="D176" s="585" t="s">
         <v>1079</v>
       </c>
-      <c r="E176" s="582" t="s">
+      <c r="E176" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F176" s="584" t="s">
+      <c r="F176" s="583" t="s">
         <v>339</v>
       </c>
     </row>
@@ -38898,56 +38914,56 @@
       </c>
     </row>
     <row r="189" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A189" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B189" s="588"/>
-      <c r="C189" s="586" t="s">
+      <c r="A189" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B189" s="587"/>
+      <c r="C189" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D189" s="586" t="s">
+      <c r="D189" s="585" t="s">
         <v>1075</v>
       </c>
-      <c r="E189" s="582" t="s">
+      <c r="E189" s="581" t="s">
         <v>776</v>
       </c>
-      <c r="F189" s="584" t="s">
+      <c r="F189" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A190" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B190" s="588"/>
-      <c r="C190" s="586" t="s">
+      <c r="A190" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B190" s="587"/>
+      <c r="C190" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D190" s="586" t="s">
+      <c r="D190" s="585" t="s">
         <v>1077</v>
       </c>
-      <c r="E190" s="582" t="s">
+      <c r="E190" s="581" t="s">
         <v>776</v>
       </c>
-      <c r="F190" s="584" t="s">
+      <c r="F190" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A191" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B191" s="588"/>
-      <c r="C191" s="586" t="s">
+      <c r="A191" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B191" s="587"/>
+      <c r="C191" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D191" s="586" t="s">
+      <c r="D191" s="585" t="s">
         <v>1079</v>
       </c>
-      <c r="E191" s="582" t="s">
+      <c r="E191" s="581" t="s">
         <v>776</v>
       </c>
-      <c r="F191" s="584" t="s">
+      <c r="F191" s="583" t="s">
         <v>339</v>
       </c>
     </row>
@@ -38970,128 +38986,128 @@
       </c>
     </row>
     <row r="193" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A193" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B193" s="588"/>
-      <c r="C193" s="586" t="s">
+      <c r="A193" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B193" s="587"/>
+      <c r="C193" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D193" s="586" t="s">
+      <c r="D193" s="585" t="s">
         <v>100</v>
       </c>
-      <c r="E193" s="582" t="s">
+      <c r="E193" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F193" s="584" t="s">
+      <c r="F193" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A194" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B194" s="588"/>
-      <c r="C194" s="586" t="s">
+      <c r="A194" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B194" s="587"/>
+      <c r="C194" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D194" s="586" t="s">
+      <c r="D194" s="585" t="s">
         <v>1068</v>
       </c>
-      <c r="E194" s="582" t="s">
+      <c r="E194" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F194" s="584" t="s">
+      <c r="F194" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="195" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A195" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B195" s="588"/>
-      <c r="C195" s="586" t="s">
+      <c r="A195" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B195" s="587"/>
+      <c r="C195" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D195" s="586" t="s">
+      <c r="D195" s="585" t="s">
         <v>1071</v>
       </c>
-      <c r="E195" s="582" t="s">
+      <c r="E195" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F195" s="584" t="s">
+      <c r="F195" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A196" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B196" s="588"/>
-      <c r="C196" s="586" t="s">
+      <c r="A196" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B196" s="587"/>
+      <c r="C196" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D196" s="586" t="s">
+      <c r="D196" s="585" t="s">
         <v>1073</v>
       </c>
-      <c r="E196" s="582" t="s">
+      <c r="E196" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F196" s="584" t="s">
+      <c r="F196" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A197" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B197" s="589"/>
-      <c r="C197" s="586" t="s">
+      <c r="A197" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B197" s="588"/>
+      <c r="C197" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D197" s="586" t="s">
+      <c r="D197" s="585" t="s">
         <v>1075</v>
       </c>
-      <c r="E197" s="582" t="s">
+      <c r="E197" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F197" s="584" t="s">
+      <c r="F197" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A198" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B198" s="588"/>
-      <c r="C198" s="586" t="s">
+      <c r="A198" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B198" s="587"/>
+      <c r="C198" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D198" s="586" t="s">
+      <c r="D198" s="585" t="s">
         <v>1077</v>
       </c>
-      <c r="E198" s="582" t="s">
+      <c r="E198" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F198" s="584" t="s">
+      <c r="F198" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A199" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B199" s="588"/>
-      <c r="C199" s="586" t="s">
+      <c r="A199" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B199" s="587"/>
+      <c r="C199" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D199" s="586" t="s">
+      <c r="D199" s="585" t="s">
         <v>1079</v>
       </c>
-      <c r="E199" s="582" t="s">
+      <c r="E199" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F199" s="584" t="s">
+      <c r="F199" s="583" t="s">
         <v>339</v>
       </c>
     </row>
@@ -39312,56 +39328,56 @@
       </c>
     </row>
     <row r="212" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A212" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B212" s="588"/>
-      <c r="C212" s="586" t="s">
+      <c r="A212" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B212" s="587"/>
+      <c r="C212" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D212" s="586" t="s">
+      <c r="D212" s="585" t="s">
         <v>1075</v>
       </c>
-      <c r="E212" s="582" t="s">
+      <c r="E212" s="581" t="s">
         <v>776</v>
       </c>
-      <c r="F212" s="584" t="s">
+      <c r="F212" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A213" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B213" s="588"/>
-      <c r="C213" s="586" t="s">
+      <c r="A213" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B213" s="587"/>
+      <c r="C213" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D213" s="586" t="s">
+      <c r="D213" s="585" t="s">
         <v>1077</v>
       </c>
-      <c r="E213" s="582" t="s">
+      <c r="E213" s="581" t="s">
         <v>776</v>
       </c>
-      <c r="F213" s="584" t="s">
+      <c r="F213" s="583" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A214" s="587">
-        <v>42736</v>
-      </c>
-      <c r="B214" s="588"/>
-      <c r="C214" s="586" t="s">
+      <c r="A214" s="586">
+        <v>42736</v>
+      </c>
+      <c r="B214" s="587"/>
+      <c r="C214" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D214" s="586" t="s">
+      <c r="D214" s="585" t="s">
         <v>1079</v>
       </c>
-      <c r="E214" s="582" t="s">
+      <c r="E214" s="581" t="s">
         <v>776</v>
       </c>
-      <c r="F214" s="584" t="s">
+      <c r="F214" s="583" t="s">
         <v>339</v>
       </c>
     </row>
@@ -39645,8 +39661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:EK67"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:XFD67"/>
+    <sheetView showGridLines="0" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -40994,20 +41010,20 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="581">
-        <v>42736</v>
-      </c>
-      <c r="B60" s="582"/>
-      <c r="C60" s="586" t="s">
+      <c r="A60" s="580">
+        <v>42736</v>
+      </c>
+      <c r="B60" s="581"/>
+      <c r="C60" s="585" t="s">
         <v>1062</v>
       </c>
-      <c r="D60" s="568" t="s">
+      <c r="D60" s="567" t="s">
         <v>392</v>
       </c>
-      <c r="E60" s="583" t="s">
+      <c r="E60" s="582" t="s">
         <v>1119</v>
       </c>
-      <c r="F60" s="584" t="s">
+      <c r="F60" s="583" t="s">
         <v>339</v>
       </c>
     </row>
@@ -41022,7 +41038,7 @@
       <c r="D61" s="62" t="s">
         <v>1088</v>
       </c>
-      <c r="E61" s="585" t="s">
+      <c r="E61" s="584" t="s">
         <v>936</v>
       </c>
       <c r="F61" s="115" t="s">
@@ -41040,7 +41056,7 @@
       <c r="D62" s="62" t="s">
         <v>392</v>
       </c>
-      <c r="E62" s="585" t="s">
+      <c r="E62" s="584" t="s">
         <v>776</v>
       </c>
       <c r="F62" s="115" t="s">
@@ -41058,7 +41074,7 @@
       <c r="D63" s="62" t="s">
         <v>1088</v>
       </c>
-      <c r="E63" s="585" t="s">
+      <c r="E63" s="584" t="s">
         <v>776</v>
       </c>
       <c r="F63" s="115" t="s">
@@ -41066,20 +41082,20 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="581">
+      <c r="A64" s="580">
         <v>42737</v>
       </c>
-      <c r="B64" s="582"/>
-      <c r="C64" s="586" t="s">
+      <c r="B64" s="581"/>
+      <c r="C64" s="585" t="s">
         <v>1065</v>
       </c>
-      <c r="D64" s="568" t="s">
+      <c r="D64" s="567" t="s">
         <v>392</v>
       </c>
-      <c r="E64" s="583" t="s">
+      <c r="E64" s="582" t="s">
         <v>1119</v>
       </c>
-      <c r="F64" s="584" t="s">
+      <c r="F64" s="583" t="s">
         <v>339</v>
       </c>
     </row>
@@ -41091,10 +41107,10 @@
       <c r="C65" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D65" s="568" t="s">
+      <c r="D65" s="567" t="s">
         <v>1089</v>
       </c>
-      <c r="E65" s="585" t="s">
+      <c r="E65" s="584" t="s">
         <v>936</v>
       </c>
       <c r="F65" s="115" t="s">
@@ -41112,7 +41128,7 @@
       <c r="D66" s="62" t="s">
         <v>392</v>
       </c>
-      <c r="E66" s="585" t="s">
+      <c r="E66" s="584" t="s">
         <v>776</v>
       </c>
       <c r="F66" s="115" t="s">
@@ -41127,10 +41143,10 @@
       <c r="C67" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D67" s="568" t="s">
+      <c r="D67" s="567" t="s">
         <v>1089</v>
       </c>
-      <c r="E67" s="585" t="s">
+      <c r="E67" s="584" t="s">
         <v>776</v>
       </c>
       <c r="F67" s="115" t="s">
@@ -41153,8 +41169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:CF47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD47"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -42064,20 +42080,20 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="581">
-        <v>42736</v>
-      </c>
-      <c r="B42" s="582"/>
-      <c r="C42" s="568" t="s">
+      <c r="A42" s="580">
+        <v>42736</v>
+      </c>
+      <c r="B42" s="581"/>
+      <c r="C42" s="567" t="s">
         <v>1062</v>
       </c>
-      <c r="D42" s="568" t="s">
+      <c r="D42" s="567" t="s">
         <v>489</v>
       </c>
-      <c r="E42" s="582" t="s">
+      <c r="E42" s="581" t="s">
         <v>1119</v>
       </c>
-      <c r="F42" s="584" t="s">
+      <c r="F42" s="583" t="s">
         <v>339</v>
       </c>
     </row>
@@ -42128,7 +42144,7 @@
       <c r="D45" s="265" t="s">
         <v>489</v>
       </c>
-      <c r="E45" s="590" t="s">
+      <c r="E45" s="589" t="s">
         <v>1119</v>
       </c>
       <c r="F45" s="266" t="s">
@@ -42187,7 +42203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -42673,7 +42689,7 @@
       </c>
       <c r="G20" s="409"/>
       <c r="H20" s="409"/>
-      <c r="I20" s="565" t="s">
+      <c r="I20" s="564" t="s">
         <v>26</v>
       </c>
     </row>
@@ -42696,7 +42712,7 @@
       </c>
       <c r="G21" s="409"/>
       <c r="H21" s="409"/>
-      <c r="I21" s="565" t="s">
+      <c r="I21" s="564" t="s">
         <v>26</v>
       </c>
     </row>
@@ -43060,9 +43076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IO163"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A148" sqref="A148:XFD163"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E172" sqref="E172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -53746,7 +53762,7 @@
       <c r="E149" s="73" t="s">
         <v>1069</v>
       </c>
-      <c r="F149" s="566"/>
+      <c r="F149" s="565"/>
       <c r="G149" s="265" t="s">
         <v>1070</v>
       </c>
@@ -53994,7 +54010,7 @@
       <c r="E157" s="73" t="s">
         <v>1069</v>
       </c>
-      <c r="F157" s="566"/>
+      <c r="F157" s="565"/>
       <c r="G157" s="265" t="s">
         <v>1070</v>
       </c>
@@ -54218,7 +54234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T85"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C49" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A72" workbookViewId="0">
       <selection activeCell="C82" sqref="A82:XFD85"/>
     </sheetView>
   </sheetViews>
@@ -57225,7 +57241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2A25AD-5D69-564D-9511-0323740C2E1F}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -58106,7 +58122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A239" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
@@ -61285,7 +61301,7 @@
       <c r="K112" s="239" t="s">
         <v>375</v>
       </c>
-      <c r="L112" s="567"/>
+      <c r="L112" s="566"/>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A113" s="237">
@@ -61713,7 +61729,7 @@
       <c r="K127" s="239" t="s">
         <v>375</v>
       </c>
-      <c r="L127" s="567"/>
+      <c r="L127" s="566"/>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A128" s="237">
@@ -61915,7 +61931,7 @@
       <c r="K134" s="239" t="s">
         <v>375</v>
       </c>
-      <c r="L134" s="567"/>
+      <c r="L134" s="566"/>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A135" s="237">
@@ -62213,7 +62229,7 @@
       <c r="C145" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D145" s="568" t="s">
+      <c r="D145" s="567" t="s">
         <v>1089</v>
       </c>
       <c r="E145" s="82" t="s">
@@ -62241,7 +62257,7 @@
       <c r="C146" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D146" s="568" t="s">
+      <c r="D146" s="567" t="s">
         <v>1089</v>
       </c>
       <c r="E146" s="82" t="s">
@@ -62269,7 +62285,7 @@
       <c r="C147" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D147" s="568" t="s">
+      <c r="D147" s="567" t="s">
         <v>1089</v>
       </c>
       <c r="E147" s="82" t="s">
@@ -62297,7 +62313,7 @@
       <c r="C148" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D148" s="568" t="s">
+      <c r="D148" s="567" t="s">
         <v>1089</v>
       </c>
       <c r="E148" s="82" t="s">
@@ -62325,7 +62341,7 @@
       <c r="C149" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D149" s="568" t="s">
+      <c r="D149" s="567" t="s">
         <v>1089</v>
       </c>
       <c r="E149" s="88" t="s">
@@ -62353,7 +62369,7 @@
       <c r="C150" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D150" s="568" t="s">
+      <c r="D150" s="567" t="s">
         <v>1089</v>
       </c>
       <c r="E150" s="82" t="s">
@@ -62381,7 +62397,7 @@
       <c r="C151" s="65" t="s">
         <v>1065</v>
       </c>
-      <c r="D151" s="568" t="s">
+      <c r="D151" s="567" t="s">
         <v>1089</v>
       </c>
       <c r="E151" s="82" t="s">

</xml_diff>

<commit_message>
RDM-9587 Conditional Post States
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-api-test-automation-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3B2154-43D5-8942-A3D4-06B269D11151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1CC26F-D7FB-A347-9D23-3D08D66F9AA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="2000" windowWidth="35340" windowHeight="19340" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6675" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6731" uniqueCount="1071">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3319,9 +3319,6 @@
     <t>Delete case</t>
   </si>
   <si>
-    <t>CaseUpdated(TextField="updated" AND EmailField="*"):1;CaseAmended(TextField="amended" AND EmailField="*"):2;CaseRevoked(TextField="revoked" AND EmailField="*"):3;CaseDeleted</t>
-  </si>
-  <si>
     <t>Conditional event post state page</t>
   </si>
   <si>
@@ -3329,6 +3326,36 @@
   </si>
   <si>
     <t>FT-Conditional Post State</t>
+  </si>
+  <si>
+    <t>CaseUpdated2(TextField="updated2" OR EmailField="*"):1;CaseAmended2(TextField="amended2" OR EmailField="matched@test.com"):2;*(TextField="keepstate"):3;CaseRevoked2(EmailField!=""):4;CaseDeleted</t>
+  </si>
+  <si>
+    <t>CaseUpdated(TextField="updated" AND EmailField="*"):1;CaseAmended(TextField="amended" AND EmailField="*"):2;CaseRevoked(AddressField.AddressLine1="Some address" AND EmailField="*"):3;CaseDeleted</t>
+  </si>
+  <si>
+    <t>updateCase2</t>
+  </si>
+  <si>
+    <t>Update a case 2</t>
+  </si>
+  <si>
+    <t>CaseUpdated2</t>
+  </si>
+  <si>
+    <t>CaseAmended2</t>
+  </si>
+  <si>
+    <t>CaseRevoked2</t>
+  </si>
+  <si>
+    <t>Update case 2</t>
+  </si>
+  <si>
+    <t>Amend case 2</t>
+  </si>
+  <si>
+    <t>Revoke case 2</t>
   </si>
 </sst>
 </file>
@@ -13169,7 +13196,7 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:R184" totalsRowShown="0" headerRowDxfId="133" dataDxfId="131" headerRowBorderDxfId="132" tableBorderDxfId="130" totalsRowBorderDxfId="129">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:R189" totalsRowShown="0" headerRowDxfId="133" dataDxfId="131" headerRowBorderDxfId="132" tableBorderDxfId="130" totalsRowBorderDxfId="129">
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="128"/>
     <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="127"/>
@@ -13324,7 +13351,7 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F59" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F60" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
@@ -15408,8 +15435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:CR69"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView showGridLines="0" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17605,7 +17632,7 @@
       </c>
       <c r="B68" s="299"/>
       <c r="C68" s="17" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D68" s="69" t="s">
         <v>455</v>
@@ -17685,10 +17712,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:FH36"/>
+  <dimension ref="A1:FH39"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18513,7 +18540,7 @@
       </c>
       <c r="B31" s="61"/>
       <c r="C31" s="16" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D31" s="62" t="s">
         <v>489</v>
@@ -18533,7 +18560,7 @@
       </c>
       <c r="B32" s="61"/>
       <c r="C32" s="16" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D32" s="62" t="s">
         <v>493</v>
@@ -18553,7 +18580,7 @@
       </c>
       <c r="B33" s="61"/>
       <c r="C33" s="16" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D33" s="62" t="s">
         <v>1052</v>
@@ -18573,7 +18600,7 @@
       </c>
       <c r="B34" s="61"/>
       <c r="C34" s="16" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D34" s="62" t="s">
         <v>1054</v>
@@ -18593,7 +18620,7 @@
       </c>
       <c r="B35" s="61"/>
       <c r="C35" s="16" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D35" s="62" t="s">
         <v>1056</v>
@@ -18607,25 +18634,85 @@
       </c>
       <c r="H35" s="64"/>
     </row>
-    <row r="36" spans="1:8" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="462">
-        <v>42736</v>
-      </c>
-      <c r="B36" s="469"/>
-      <c r="C36" s="469" t="s">
+    <row r="36" spans="1:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B36" s="61"/>
+      <c r="C36" s="16" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D36" s="62" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E36" s="62" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F36" s="81"/>
+      <c r="G36" s="80">
+        <v>1</v>
+      </c>
+      <c r="H36" s="64"/>
+    </row>
+    <row r="37" spans="1:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B37" s="61"/>
+      <c r="C37" s="16" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D37" s="62" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E37" s="62" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F37" s="81"/>
+      <c r="G37" s="80">
+        <v>1</v>
+      </c>
+      <c r="H37" s="64"/>
+    </row>
+    <row r="38" spans="1:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B38" s="61"/>
+      <c r="C38" s="16" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D38" s="62" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E38" s="62" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F38" s="81"/>
+      <c r="G38" s="80">
+        <v>1</v>
+      </c>
+      <c r="H38" s="64"/>
+    </row>
+    <row r="39" spans="1:8" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="462">
+        <v>42736</v>
+      </c>
+      <c r="B39" s="469"/>
+      <c r="C39" s="469" t="s">
         <v>983</v>
       </c>
-      <c r="D36" s="469" t="s">
+      <c r="D39" s="469" t="s">
         <v>489</v>
       </c>
-      <c r="E36" s="469" t="s">
+      <c r="E39" s="469" t="s">
         <v>490</v>
       </c>
-      <c r="F36" s="469"/>
-      <c r="G36" s="469">
+      <c r="F39" s="469"/>
+      <c r="G39" s="469">
         <v>1</v>
       </c>
-      <c r="H36" s="469"/>
+      <c r="H39" s="469"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -18646,10 +18733,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="109" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView showGridLines="0" topLeftCell="A24" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20463,7 +20550,7 @@
       </c>
       <c r="B43" s="544"/>
       <c r="C43" s="544" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D43" s="551" t="s">
         <v>392</v>
@@ -20503,7 +20590,7 @@
       </c>
       <c r="B44" s="544"/>
       <c r="C44" s="544" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D44" s="551" t="s">
         <v>941</v>
@@ -20521,7 +20608,7 @@
         <v>489</v>
       </c>
       <c r="I44" s="547" t="s">
-        <v>1058</v>
+        <v>1062</v>
       </c>
       <c r="J44" s="548"/>
       <c r="K44" s="548"/>
@@ -20539,45 +20626,47 @@
       <c r="S44" s="549"/>
       <c r="T44" s="550"/>
     </row>
-    <row r="45" spans="1:20" s="481" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="480">
-        <v>42739</v>
-      </c>
-      <c r="B45" s="459"/>
-      <c r="C45" s="459" t="s">
-        <v>983</v>
-      </c>
-      <c r="D45" s="459" t="s">
-        <v>996</v>
-      </c>
-      <c r="E45" s="459" t="s">
-        <v>997</v>
-      </c>
-      <c r="F45" s="519" t="s">
-        <v>997</v>
-      </c>
-      <c r="G45" s="459">
-        <v>7</v>
-      </c>
-      <c r="H45" s="459"/>
-      <c r="I45" s="459" t="s">
+    <row r="45" spans="1:20" s="389" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="543">
+        <v>42736</v>
+      </c>
+      <c r="B45" s="544"/>
+      <c r="C45" s="544" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D45" s="551" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E45" s="551" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F45" s="545" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G45" s="546">
+        <v>3</v>
+      </c>
+      <c r="H45" s="547" t="s">
         <v>489</v>
       </c>
-      <c r="J45" s="459"/>
-      <c r="K45" s="459"/>
-      <c r="L45" s="459"/>
-      <c r="M45" s="459"/>
-      <c r="N45" s="459"/>
-      <c r="O45" s="459"/>
-      <c r="P45" s="471" t="s">
+      <c r="I45" s="547" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J45" s="548"/>
+      <c r="K45" s="548"/>
+      <c r="L45" s="548"/>
+      <c r="M45" s="548"/>
+      <c r="N45" s="548"/>
+      <c r="O45" s="548"/>
+      <c r="P45" s="547" t="s">
         <v>26</v>
       </c>
-      <c r="Q45" s="471" t="s">
+      <c r="Q45" s="547" t="s">
         <v>533</v>
       </c>
-      <c r="R45" s="459"/>
-      <c r="S45" s="459"/>
-      <c r="T45" s="459"/>
+      <c r="R45" s="549"/>
+      <c r="S45" s="549"/>
+      <c r="T45" s="550"/>
     </row>
     <row r="46" spans="1:20" s="481" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="480">
@@ -20588,16 +20677,16 @@
         <v>983</v>
       </c>
       <c r="D46" s="459" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E46" s="459" t="s">
-        <v>1004</v>
+        <v>997</v>
       </c>
       <c r="F46" s="519" t="s">
-        <v>1004</v>
+        <v>997</v>
       </c>
       <c r="G46" s="459">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H46" s="459"/>
       <c r="I46" s="459" t="s">
@@ -20628,16 +20717,16 @@
         <v>983</v>
       </c>
       <c r="D47" s="459" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E47" s="459" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="F47" s="519" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="G47" s="459">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H47" s="459"/>
       <c r="I47" s="459" t="s">
@@ -20668,16 +20757,16 @@
         <v>983</v>
       </c>
       <c r="D48" s="459" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E48" s="459" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="F48" s="519" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="G48" s="459">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H48" s="459"/>
       <c r="I48" s="459" t="s">
@@ -20707,17 +20796,17 @@
       <c r="C49" s="459" t="s">
         <v>983</v>
       </c>
-      <c r="D49" s="519" t="s">
-        <v>1001</v>
+      <c r="D49" s="459" t="s">
+        <v>1000</v>
       </c>
       <c r="E49" s="459" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F49" s="519" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="G49" s="459">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H49" s="459"/>
       <c r="I49" s="459" t="s">
@@ -20747,17 +20836,17 @@
       <c r="C50" s="459" t="s">
         <v>983</v>
       </c>
-      <c r="D50" s="459" t="s">
-        <v>1002</v>
+      <c r="D50" s="519" t="s">
+        <v>1001</v>
       </c>
       <c r="E50" s="459" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="F50" s="519" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="G50" s="459">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H50" s="459"/>
       <c r="I50" s="459" t="s">
@@ -20788,16 +20877,16 @@
         <v>983</v>
       </c>
       <c r="D51" s="459" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E51" s="459" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="F51" s="519" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="G51" s="459">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H51" s="459"/>
       <c r="I51" s="459" t="s">
@@ -20818,6 +20907,46 @@
       <c r="R51" s="459"/>
       <c r="S51" s="459"/>
       <c r="T51" s="459"/>
+    </row>
+    <row r="52" spans="1:20" s="481" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="480">
+        <v>42739</v>
+      </c>
+      <c r="B52" s="459"/>
+      <c r="C52" s="459" t="s">
+        <v>983</v>
+      </c>
+      <c r="D52" s="459" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E52" s="459" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F52" s="519" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G52" s="459">
+        <v>1</v>
+      </c>
+      <c r="H52" s="459"/>
+      <c r="I52" s="459" t="s">
+        <v>489</v>
+      </c>
+      <c r="J52" s="459"/>
+      <c r="K52" s="459"/>
+      <c r="L52" s="459"/>
+      <c r="M52" s="459"/>
+      <c r="N52" s="459"/>
+      <c r="O52" s="459"/>
+      <c r="P52" s="471" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q52" s="471" t="s">
+        <v>533</v>
+      </c>
+      <c r="R52" s="459"/>
+      <c r="S52" s="459"/>
+      <c r="T52" s="459"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -20842,10 +20971,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:R184"/>
+  <dimension ref="A1:R189"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A148" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -27415,7 +27544,7 @@
       </c>
       <c r="B162" s="553"/>
       <c r="C162" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D162" s="547" t="s">
         <v>392</v>
@@ -27433,7 +27562,7 @@
         <v>597</v>
       </c>
       <c r="I162" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J162" s="405">
         <v>1</v>
@@ -27455,7 +27584,7 @@
       </c>
       <c r="B163" s="553"/>
       <c r="C163" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D163" s="547" t="s">
         <v>392</v>
@@ -27473,7 +27602,7 @@
         <v>597</v>
       </c>
       <c r="I163" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J163" s="405">
         <v>2</v>
@@ -27495,7 +27624,7 @@
       </c>
       <c r="B164" s="553"/>
       <c r="C164" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D164" s="547" t="s">
         <v>392</v>
@@ -27513,7 +27642,7 @@
         <v>597</v>
       </c>
       <c r="I164" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J164" s="405">
         <v>3</v>
@@ -27535,7 +27664,7 @@
       </c>
       <c r="B165" s="553"/>
       <c r="C165" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D165" s="547" t="s">
         <v>392</v>
@@ -27553,7 +27682,7 @@
         <v>597</v>
       </c>
       <c r="I165" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J165" s="405">
         <v>4</v>
@@ -27575,7 +27704,7 @@
       </c>
       <c r="B166" s="553"/>
       <c r="C166" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D166" s="547" t="s">
         <v>392</v>
@@ -27593,7 +27722,7 @@
         <v>597</v>
       </c>
       <c r="I166" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J166" s="405">
         <v>5</v>
@@ -27615,7 +27744,7 @@
       </c>
       <c r="B167" s="553"/>
       <c r="C167" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D167" s="547" t="s">
         <v>392</v>
@@ -27633,7 +27762,7 @@
         <v>597</v>
       </c>
       <c r="I167" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J167" s="405">
         <v>6</v>
@@ -27655,7 +27784,7 @@
       </c>
       <c r="B168" s="553"/>
       <c r="C168" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D168" s="547" t="s">
         <v>392</v>
@@ -27673,7 +27802,7 @@
         <v>597</v>
       </c>
       <c r="I168" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J168" s="405">
         <v>7</v>
@@ -27695,7 +27824,7 @@
       </c>
       <c r="B169" s="553"/>
       <c r="C169" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D169" s="547" t="s">
         <v>392</v>
@@ -27713,7 +27842,7 @@
         <v>597</v>
       </c>
       <c r="I169" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J169" s="405">
         <v>8</v>
@@ -27735,7 +27864,7 @@
       </c>
       <c r="B170" s="553"/>
       <c r="C170" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D170" s="547" t="s">
         <v>392</v>
@@ -27753,7 +27882,7 @@
         <v>597</v>
       </c>
       <c r="I170" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J170" s="405">
         <v>9</v>
@@ -27775,7 +27904,7 @@
       </c>
       <c r="B171" s="553"/>
       <c r="C171" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D171" s="547" t="s">
         <v>392</v>
@@ -27793,7 +27922,7 @@
         <v>597</v>
       </c>
       <c r="I171" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J171" s="405">
         <v>10</v>
@@ -27815,7 +27944,7 @@
       </c>
       <c r="B172" s="553"/>
       <c r="C172" s="545" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D172" s="547" t="s">
         <v>392</v>
@@ -27833,7 +27962,7 @@
         <v>597</v>
       </c>
       <c r="I172" s="554" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J172" s="405">
         <v>11</v>
@@ -27849,221 +27978,225 @@
       <c r="Q172" s="544"/>
       <c r="R172" s="556"/>
     </row>
-    <row r="173" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A173" s="425">
+    <row r="173" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A173" s="552">
         <v>42741</v>
       </c>
-      <c r="B173" s="482"/>
-      <c r="C173" s="483" t="s">
-        <v>983</v>
-      </c>
-      <c r="D173" s="484" t="s">
-        <v>996</v>
-      </c>
-      <c r="E173" s="483" t="s">
-        <v>986</v>
-      </c>
-      <c r="F173" s="485">
+      <c r="B173" s="553"/>
+      <c r="C173" s="545" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D173" s="547" t="s">
+        <v>941</v>
+      </c>
+      <c r="E173" s="545" t="s">
+        <v>54</v>
+      </c>
+      <c r="F173" s="544">
+        <v>1</v>
+      </c>
+      <c r="G173" s="545" t="s">
+        <v>375</v>
+      </c>
+      <c r="H173" s="554" t="s">
+        <v>597</v>
+      </c>
+      <c r="I173" s="554" t="s">
+        <v>1058</v>
+      </c>
+      <c r="J173" s="405">
+        <v>1</v>
+      </c>
+      <c r="K173" s="544"/>
+      <c r="L173" s="544"/>
+      <c r="M173" s="555"/>
+      <c r="N173" s="544"/>
+      <c r="O173" s="544"/>
+      <c r="P173" s="554" t="s">
+        <v>836</v>
+      </c>
+      <c r="Q173" s="544"/>
+      <c r="R173" s="556"/>
+    </row>
+    <row r="174" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A174" s="552">
+        <v>42741</v>
+      </c>
+      <c r="B174" s="553"/>
+      <c r="C174" s="545" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D174" s="547" t="s">
+        <v>941</v>
+      </c>
+      <c r="E174" s="545" t="s">
+        <v>93</v>
+      </c>
+      <c r="F174" s="544">
         <v>2</v>
       </c>
-      <c r="G173" s="483" t="s">
+      <c r="G174" s="545" t="s">
         <v>375</v>
       </c>
-      <c r="H173" s="426" t="s">
-        <v>843</v>
-      </c>
-      <c r="I173" s="426" t="s">
-        <v>844</v>
-      </c>
-      <c r="J173" s="428">
+      <c r="H174" s="554" t="s">
+        <v>597</v>
+      </c>
+      <c r="I174" s="554" t="s">
+        <v>1058</v>
+      </c>
+      <c r="J174" s="405">
         <v>1</v>
       </c>
-      <c r="K173" s="485"/>
-      <c r="L173" s="485"/>
-      <c r="M173" s="486"/>
-      <c r="N173" s="485"/>
-      <c r="O173" s="485"/>
-      <c r="P173" s="426" t="s">
+      <c r="K174" s="544"/>
+      <c r="L174" s="544"/>
+      <c r="M174" s="555"/>
+      <c r="N174" s="544"/>
+      <c r="O174" s="544"/>
+      <c r="P174" s="554" t="s">
         <v>836</v>
       </c>
-      <c r="Q173" s="485"/>
-      <c r="R173" s="487"/>
-    </row>
-    <row r="174" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A174" s="425">
-        <v>42754</v>
-      </c>
-      <c r="B174" s="482"/>
-      <c r="C174" s="483" t="s">
-        <v>983</v>
-      </c>
-      <c r="D174" s="484" t="s">
-        <v>996</v>
-      </c>
-      <c r="E174" s="483" t="s">
-        <v>987</v>
-      </c>
-      <c r="F174" s="485">
+      <c r="Q174" s="544"/>
+      <c r="R174" s="556"/>
+    </row>
+    <row r="175" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A175" s="552">
+        <v>42741</v>
+      </c>
+      <c r="B175" s="553"/>
+      <c r="C175" s="545" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D175" s="547" t="s">
+        <v>941</v>
+      </c>
+      <c r="E175" s="545" t="s">
+        <v>63</v>
+      </c>
+      <c r="F175" s="544">
+        <v>3</v>
+      </c>
+      <c r="G175" s="545" t="s">
+        <v>375</v>
+      </c>
+      <c r="H175" s="554" t="s">
+        <v>597</v>
+      </c>
+      <c r="I175" s="554" t="s">
+        <v>1058</v>
+      </c>
+      <c r="J175" s="405">
         <v>1</v>
       </c>
-      <c r="G174" s="483" t="s">
+      <c r="K175" s="544"/>
+      <c r="L175" s="544"/>
+      <c r="M175" s="555"/>
+      <c r="N175" s="544"/>
+      <c r="O175" s="544"/>
+      <c r="P175" s="554" t="s">
+        <v>836</v>
+      </c>
+      <c r="Q175" s="544"/>
+      <c r="R175" s="556"/>
+    </row>
+    <row r="176" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A176" s="552">
+        <v>42741</v>
+      </c>
+      <c r="B176" s="553"/>
+      <c r="C176" s="545" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D176" s="547" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E176" s="545" t="s">
+        <v>54</v>
+      </c>
+      <c r="F176" s="544">
+        <v>1</v>
+      </c>
+      <c r="G176" s="545" t="s">
         <v>375</v>
       </c>
-      <c r="H174" s="426" t="s">
-        <v>843</v>
-      </c>
-      <c r="I174" s="426" t="s">
-        <v>844</v>
-      </c>
-      <c r="J174" s="428">
+      <c r="H176" s="554" t="s">
+        <v>597</v>
+      </c>
+      <c r="I176" s="554" t="s">
+        <v>1058</v>
+      </c>
+      <c r="J176" s="405">
         <v>1</v>
       </c>
-      <c r="K174" s="485"/>
-      <c r="L174" s="485"/>
-      <c r="M174" s="486"/>
-      <c r="N174" s="485"/>
-      <c r="O174" s="485"/>
-      <c r="P174" s="426" t="s">
+      <c r="K176" s="544"/>
+      <c r="L176" s="544"/>
+      <c r="M176" s="555"/>
+      <c r="N176" s="544"/>
+      <c r="O176" s="544"/>
+      <c r="P176" s="554" t="s">
         <v>836</v>
       </c>
-      <c r="Q174" s="485"/>
-      <c r="R174" s="487"/>
-    </row>
-    <row r="175" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A175" s="425">
-        <v>42755</v>
-      </c>
-      <c r="B175" s="482"/>
-      <c r="C175" s="483" t="s">
-        <v>983</v>
-      </c>
-      <c r="D175" s="484" t="s">
-        <v>998</v>
-      </c>
-      <c r="E175" s="483" t="s">
-        <v>986</v>
-      </c>
-      <c r="F175" s="485">
+      <c r="Q176" s="544"/>
+      <c r="R176" s="556"/>
+    </row>
+    <row r="177" spans="1:18" s="389" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A177" s="552">
+        <v>42741</v>
+      </c>
+      <c r="B177" s="553"/>
+      <c r="C177" s="545" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D177" s="547" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E177" s="545" t="s">
+        <v>93</v>
+      </c>
+      <c r="F177" s="544">
+        <v>2</v>
+      </c>
+      <c r="G177" s="545" t="s">
+        <v>375</v>
+      </c>
+      <c r="H177" s="554" t="s">
+        <v>597</v>
+      </c>
+      <c r="I177" s="554" t="s">
+        <v>1058</v>
+      </c>
+      <c r="J177" s="405">
         <v>1</v>
       </c>
-      <c r="G175" s="483" t="s">
-        <v>609</v>
-      </c>
-      <c r="H175" s="426" t="s">
-        <v>843</v>
-      </c>
-      <c r="I175" s="426" t="s">
-        <v>844</v>
-      </c>
-      <c r="J175" s="428">
-        <v>1</v>
-      </c>
-      <c r="K175" s="485"/>
-      <c r="L175" s="485"/>
-      <c r="M175" s="486"/>
-      <c r="N175" s="485"/>
-      <c r="O175" s="485"/>
-      <c r="P175" s="426" t="s">
+      <c r="K177" s="544"/>
+      <c r="L177" s="544"/>
+      <c r="M177" s="555"/>
+      <c r="N177" s="544"/>
+      <c r="O177" s="544"/>
+      <c r="P177" s="554" t="s">
         <v>836</v>
       </c>
-      <c r="Q175" s="485"/>
-      <c r="R175" s="487"/>
-    </row>
-    <row r="176" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A176" s="425">
-        <v>42756</v>
-      </c>
-      <c r="B176" s="482"/>
-      <c r="C176" s="483" t="s">
-        <v>983</v>
-      </c>
-      <c r="D176" s="484" t="s">
-        <v>998</v>
-      </c>
-      <c r="E176" s="483" t="s">
-        <v>987</v>
-      </c>
-      <c r="F176" s="485">
-        <v>2</v>
-      </c>
-      <c r="G176" s="483" t="s">
-        <v>609</v>
-      </c>
-      <c r="H176" s="426" t="s">
-        <v>843</v>
-      </c>
-      <c r="I176" s="426" t="s">
-        <v>844</v>
-      </c>
-      <c r="J176" s="488">
-        <v>1</v>
-      </c>
-      <c r="K176" s="485"/>
-      <c r="L176" s="485"/>
-      <c r="M176" s="486"/>
-      <c r="N176" s="485"/>
-      <c r="O176" s="485"/>
-      <c r="P176" s="426" t="s">
-        <v>836</v>
-      </c>
-      <c r="Q176" s="485"/>
-      <c r="R176" s="487"/>
-    </row>
-    <row r="177" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A177" s="425">
-        <v>42741</v>
-      </c>
-      <c r="B177" s="482"/>
-      <c r="C177" s="483" t="s">
-        <v>983</v>
-      </c>
-      <c r="D177" s="484" t="s">
-        <v>999</v>
-      </c>
-      <c r="E177" s="483" t="s">
-        <v>986</v>
-      </c>
-      <c r="F177" s="485"/>
-      <c r="G177" s="483" t="s">
-        <v>609</v>
-      </c>
-      <c r="H177" s="426" t="s">
-        <v>843</v>
-      </c>
-      <c r="I177" s="426" t="s">
-        <v>844</v>
-      </c>
-      <c r="J177" s="428">
-        <v>1</v>
-      </c>
-      <c r="K177" s="485"/>
-      <c r="L177" s="485"/>
-      <c r="M177" s="486"/>
-      <c r="N177" s="485"/>
-      <c r="O177" s="485"/>
-      <c r="P177" s="426" t="s">
-        <v>836</v>
-      </c>
-      <c r="Q177" s="485"/>
-      <c r="R177" s="487"/>
+      <c r="Q177" s="544"/>
+      <c r="R177" s="556"/>
     </row>
     <row r="178" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A178" s="425">
-        <v>42754</v>
+        <v>42741</v>
       </c>
       <c r="B178" s="482"/>
       <c r="C178" s="483" t="s">
         <v>983</v>
       </c>
       <c r="D178" s="484" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="E178" s="483" t="s">
-        <v>987</v>
-      </c>
-      <c r="F178" s="485"/>
+        <v>986</v>
+      </c>
+      <c r="F178" s="485">
+        <v>2</v>
+      </c>
       <c r="G178" s="483" t="s">
-        <v>609</v>
+        <v>375</v>
       </c>
       <c r="H178" s="426" t="s">
         <v>843</v>
@@ -28087,21 +28220,23 @@
     </row>
     <row r="179" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A179" s="425">
-        <v>42755</v>
+        <v>42754</v>
       </c>
       <c r="B179" s="482"/>
       <c r="C179" s="483" t="s">
         <v>983</v>
       </c>
       <c r="D179" s="484" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="E179" s="483" t="s">
-        <v>986</v>
-      </c>
-      <c r="F179" s="485"/>
+        <v>987</v>
+      </c>
+      <c r="F179" s="485">
+        <v>1</v>
+      </c>
       <c r="G179" s="483" t="s">
-        <v>609</v>
+        <v>375</v>
       </c>
       <c r="H179" s="426" t="s">
         <v>843</v>
@@ -28125,21 +28260,23 @@
     </row>
     <row r="180" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A180" s="425">
-        <v>42756</v>
+        <v>42755</v>
       </c>
       <c r="B180" s="482"/>
       <c r="C180" s="483" t="s">
         <v>983</v>
       </c>
       <c r="D180" s="484" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="E180" s="483" t="s">
         <v>986</v>
       </c>
-      <c r="F180" s="485"/>
+      <c r="F180" s="485">
+        <v>1</v>
+      </c>
       <c r="G180" s="483" t="s">
-        <v>375</v>
+        <v>609</v>
       </c>
       <c r="H180" s="426" t="s">
         <v>843</v>
@@ -28147,7 +28284,7 @@
       <c r="I180" s="426" t="s">
         <v>844</v>
       </c>
-      <c r="J180" s="488">
+      <c r="J180" s="428">
         <v>1</v>
       </c>
       <c r="K180" s="485"/>
@@ -28163,23 +28300,23 @@
     </row>
     <row r="181" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A181" s="425">
-        <v>42757</v>
+        <v>42756</v>
       </c>
       <c r="B181" s="482"/>
       <c r="C181" s="483" t="s">
         <v>983</v>
       </c>
       <c r="D181" s="484" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="E181" s="483" t="s">
         <v>987</v>
       </c>
       <c r="F181" s="485">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G181" s="483" t="s">
-        <v>375</v>
+        <v>609</v>
       </c>
       <c r="H181" s="426" t="s">
         <v>843</v>
@@ -28187,7 +28324,7 @@
       <c r="I181" s="426" t="s">
         <v>844</v>
       </c>
-      <c r="J181" s="428">
+      <c r="J181" s="488">
         <v>1</v>
       </c>
       <c r="K181" s="485"/>
@@ -28203,21 +28340,21 @@
     </row>
     <row r="182" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A182" s="425">
-        <v>42758</v>
+        <v>42741</v>
       </c>
       <c r="B182" s="482"/>
       <c r="C182" s="483" t="s">
         <v>983</v>
       </c>
       <c r="D182" s="484" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="E182" s="483" t="s">
-        <v>12</v>
-      </c>
-      <c r="F182" s="489"/>
+        <v>986</v>
+      </c>
+      <c r="F182" s="485"/>
       <c r="G182" s="483" t="s">
-        <v>375</v>
+        <v>609</v>
       </c>
       <c r="H182" s="426" t="s">
         <v>843</v>
@@ -28241,21 +28378,19 @@
     </row>
     <row r="183" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A183" s="425">
-        <v>42759</v>
+        <v>42754</v>
       </c>
       <c r="B183" s="482"/>
       <c r="C183" s="483" t="s">
         <v>983</v>
       </c>
-      <c r="D183" s="483" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E183" s="490" t="s">
-        <v>991</v>
-      </c>
-      <c r="F183" s="485">
-        <v>1</v>
-      </c>
+      <c r="D183" s="484" t="s">
+        <v>999</v>
+      </c>
+      <c r="E183" s="483" t="s">
+        <v>987</v>
+      </c>
+      <c r="F183" s="485"/>
       <c r="G183" s="483" t="s">
         <v>609</v>
       </c>
@@ -28281,21 +28416,19 @@
     </row>
     <row r="184" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A184" s="425">
-        <v>42760</v>
+        <v>42755</v>
       </c>
       <c r="B184" s="482"/>
       <c r="C184" s="483" t="s">
         <v>983</v>
       </c>
       <c r="D184" s="484" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E184" s="483" t="s">
-        <v>991</v>
-      </c>
-      <c r="F184" s="485">
-        <v>1</v>
-      </c>
+        <v>986</v>
+      </c>
+      <c r="F184" s="485"/>
       <c r="G184" s="483" t="s">
         <v>609</v>
       </c>
@@ -28305,7 +28438,7 @@
       <c r="I184" s="426" t="s">
         <v>844</v>
       </c>
-      <c r="J184" s="488">
+      <c r="J184" s="428">
         <v>1</v>
       </c>
       <c r="K184" s="485"/>
@@ -28318,6 +28451,202 @@
       </c>
       <c r="Q184" s="485"/>
       <c r="R184" s="487"/>
+    </row>
+    <row r="185" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A185" s="425">
+        <v>42756</v>
+      </c>
+      <c r="B185" s="482"/>
+      <c r="C185" s="483" t="s">
+        <v>983</v>
+      </c>
+      <c r="D185" s="484" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E185" s="483" t="s">
+        <v>986</v>
+      </c>
+      <c r="F185" s="485"/>
+      <c r="G185" s="483" t="s">
+        <v>375</v>
+      </c>
+      <c r="H185" s="426" t="s">
+        <v>843</v>
+      </c>
+      <c r="I185" s="426" t="s">
+        <v>844</v>
+      </c>
+      <c r="J185" s="488">
+        <v>1</v>
+      </c>
+      <c r="K185" s="485"/>
+      <c r="L185" s="485"/>
+      <c r="M185" s="486"/>
+      <c r="N185" s="485"/>
+      <c r="O185" s="485"/>
+      <c r="P185" s="426" t="s">
+        <v>836</v>
+      </c>
+      <c r="Q185" s="485"/>
+      <c r="R185" s="487"/>
+    </row>
+    <row r="186" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A186" s="425">
+        <v>42757</v>
+      </c>
+      <c r="B186" s="482"/>
+      <c r="C186" s="483" t="s">
+        <v>983</v>
+      </c>
+      <c r="D186" s="484" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E186" s="483" t="s">
+        <v>987</v>
+      </c>
+      <c r="F186" s="485">
+        <v>1</v>
+      </c>
+      <c r="G186" s="483" t="s">
+        <v>375</v>
+      </c>
+      <c r="H186" s="426" t="s">
+        <v>843</v>
+      </c>
+      <c r="I186" s="426" t="s">
+        <v>844</v>
+      </c>
+      <c r="J186" s="428">
+        <v>1</v>
+      </c>
+      <c r="K186" s="485"/>
+      <c r="L186" s="485"/>
+      <c r="M186" s="486"/>
+      <c r="N186" s="485"/>
+      <c r="O186" s="485"/>
+      <c r="P186" s="426" t="s">
+        <v>836</v>
+      </c>
+      <c r="Q186" s="485"/>
+      <c r="R186" s="487"/>
+    </row>
+    <row r="187" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A187" s="425">
+        <v>42758</v>
+      </c>
+      <c r="B187" s="482"/>
+      <c r="C187" s="483" t="s">
+        <v>983</v>
+      </c>
+      <c r="D187" s="484" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E187" s="483" t="s">
+        <v>12</v>
+      </c>
+      <c r="F187" s="489"/>
+      <c r="G187" s="483" t="s">
+        <v>375</v>
+      </c>
+      <c r="H187" s="426" t="s">
+        <v>843</v>
+      </c>
+      <c r="I187" s="426" t="s">
+        <v>844</v>
+      </c>
+      <c r="J187" s="428">
+        <v>1</v>
+      </c>
+      <c r="K187" s="485"/>
+      <c r="L187" s="485"/>
+      <c r="M187" s="486"/>
+      <c r="N187" s="485"/>
+      <c r="O187" s="485"/>
+      <c r="P187" s="426" t="s">
+        <v>836</v>
+      </c>
+      <c r="Q187" s="485"/>
+      <c r="R187" s="487"/>
+    </row>
+    <row r="188" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A188" s="425">
+        <v>42759</v>
+      </c>
+      <c r="B188" s="482"/>
+      <c r="C188" s="483" t="s">
+        <v>983</v>
+      </c>
+      <c r="D188" s="483" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E188" s="490" t="s">
+        <v>991</v>
+      </c>
+      <c r="F188" s="485">
+        <v>1</v>
+      </c>
+      <c r="G188" s="483" t="s">
+        <v>609</v>
+      </c>
+      <c r="H188" s="426" t="s">
+        <v>843</v>
+      </c>
+      <c r="I188" s="426" t="s">
+        <v>844</v>
+      </c>
+      <c r="J188" s="428">
+        <v>1</v>
+      </c>
+      <c r="K188" s="485"/>
+      <c r="L188" s="485"/>
+      <c r="M188" s="486"/>
+      <c r="N188" s="485"/>
+      <c r="O188" s="485"/>
+      <c r="P188" s="426" t="s">
+        <v>836</v>
+      </c>
+      <c r="Q188" s="485"/>
+      <c r="R188" s="487"/>
+    </row>
+    <row r="189" spans="1:18" s="432" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A189" s="425">
+        <v>42760</v>
+      </c>
+      <c r="B189" s="482"/>
+      <c r="C189" s="483" t="s">
+        <v>983</v>
+      </c>
+      <c r="D189" s="484" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E189" s="483" t="s">
+        <v>991</v>
+      </c>
+      <c r="F189" s="485">
+        <v>1</v>
+      </c>
+      <c r="G189" s="483" t="s">
+        <v>609</v>
+      </c>
+      <c r="H189" s="426" t="s">
+        <v>843</v>
+      </c>
+      <c r="I189" s="426" t="s">
+        <v>844</v>
+      </c>
+      <c r="J189" s="488">
+        <v>1</v>
+      </c>
+      <c r="K189" s="485"/>
+      <c r="L189" s="485"/>
+      <c r="M189" s="486"/>
+      <c r="N189" s="485"/>
+      <c r="O189" s="485"/>
+      <c r="P189" s="426" t="s">
+        <v>836</v>
+      </c>
+      <c r="Q189" s="485"/>
+      <c r="R189" s="487"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -29360,7 +29689,7 @@
       </c>
       <c r="B49" s="393"/>
       <c r="C49" s="558" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D49" s="393" t="s">
         <v>54</v>
@@ -30563,7 +30892,7 @@
       </c>
       <c r="B37" s="560"/>
       <c r="C37" s="561" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D37" s="561" t="s">
         <v>54</v>
@@ -31639,7 +31968,7 @@
       </c>
       <c r="B50" s="393"/>
       <c r="C50" s="558" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D50" s="393" t="s">
         <v>54</v>
@@ -33090,7 +33419,7 @@
       </c>
       <c r="B55" s="560"/>
       <c r="C55" s="561" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D55" s="561" t="s">
         <v>54</v>
@@ -33596,7 +33925,7 @@
       </c>
       <c r="B22" s="72"/>
       <c r="C22" s="265" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D22" s="564" t="s">
         <v>776</v>
@@ -33636,7 +33965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F169"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A117" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A125" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
@@ -35963,7 +36292,7 @@
       </c>
       <c r="B129" s="85"/>
       <c r="C129" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D129" s="73" t="s">
         <v>54</v>
@@ -35981,7 +36310,7 @@
       </c>
       <c r="B130" s="85"/>
       <c r="C130" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D130" s="73" t="s">
         <v>57</v>
@@ -35999,7 +36328,7 @@
       </c>
       <c r="B131" s="85"/>
       <c r="C131" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D131" s="73" t="s">
         <v>60</v>
@@ -36017,7 +36346,7 @@
       </c>
       <c r="B132" s="85"/>
       <c r="C132" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D132" s="73" t="s">
         <v>63</v>
@@ -36035,7 +36364,7 @@
       </c>
       <c r="B133" s="85"/>
       <c r="C133" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D133" s="73" t="s">
         <v>66</v>
@@ -36053,7 +36382,7 @@
       </c>
       <c r="B134" s="85"/>
       <c r="C134" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D134" s="73" t="s">
         <v>69</v>
@@ -36071,7 +36400,7 @@
       </c>
       <c r="B135" s="85"/>
       <c r="C135" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D135" s="73" t="s">
         <v>72</v>
@@ -36089,7 +36418,7 @@
       </c>
       <c r="B136" s="85"/>
       <c r="C136" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D136" s="73" t="s">
         <v>83</v>
@@ -36107,7 +36436,7 @@
       </c>
       <c r="B137" s="85"/>
       <c r="C137" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D137" s="73" t="s">
         <v>87</v>
@@ -36125,7 +36454,7 @@
       </c>
       <c r="B138" s="85"/>
       <c r="C138" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D138" s="73" t="s">
         <v>93</v>
@@ -36143,7 +36472,7 @@
       </c>
       <c r="B139" s="85"/>
       <c r="C139" s="73" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D139" s="73" t="s">
         <v>96</v>
@@ -36871,10 +37200,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:EK59"/>
+  <dimension ref="A1:EK60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD51"/>
+    <sheetView showGridLines="0" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -38029,7 +38358,7 @@
       </c>
       <c r="B49" s="84"/>
       <c r="C49" s="68" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D49" s="68" t="s">
         <v>392</v>
@@ -38047,7 +38376,7 @@
       </c>
       <c r="B50" s="84"/>
       <c r="C50" s="68" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D50" s="68" t="s">
         <v>941</v>
@@ -38064,20 +38393,20 @@
         <v>42736</v>
       </c>
       <c r="B51" s="84"/>
-      <c r="C51" s="65" t="s">
-        <v>890</v>
+      <c r="C51" s="68" t="s">
+        <v>1059</v>
       </c>
       <c r="D51" s="68" t="s">
-        <v>392</v>
-      </c>
-      <c r="E51" s="134" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E51" s="84" t="s">
         <v>776</v>
       </c>
       <c r="F51" s="119" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="66">
         <v>42736</v>
       </c>
@@ -38086,7 +38415,7 @@
         <v>890</v>
       </c>
       <c r="D52" s="68" t="s">
-        <v>729</v>
+        <v>392</v>
       </c>
       <c r="E52" s="134" t="s">
         <v>776</v>
@@ -38096,20 +38425,20 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="71">
-        <v>42736</v>
-      </c>
-      <c r="B53" s="90"/>
-      <c r="C53" s="73" t="s">
+      <c r="A53" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B53" s="84"/>
+      <c r="C53" s="65" t="s">
         <v>890</v>
       </c>
-      <c r="D53" s="86" t="s">
-        <v>732</v>
-      </c>
-      <c r="E53" s="195" t="s">
+      <c r="D53" s="68" t="s">
+        <v>729</v>
+      </c>
+      <c r="E53" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F53" s="125" t="s">
+      <c r="F53" s="119" t="s">
         <v>339</v>
       </c>
     </row>
@@ -38117,12 +38446,12 @@
       <c r="A54" s="71">
         <v>42736</v>
       </c>
-      <c r="B54" s="69"/>
-      <c r="C54" s="65" t="s">
-        <v>891</v>
-      </c>
-      <c r="D54" s="82" t="s">
-        <v>834</v>
+      <c r="B54" s="90"/>
+      <c r="C54" s="73" t="s">
+        <v>890</v>
+      </c>
+      <c r="D54" s="86" t="s">
+        <v>732</v>
       </c>
       <c r="E54" s="195" t="s">
         <v>776</v>
@@ -38140,7 +38469,7 @@
         <v>891</v>
       </c>
       <c r="D55" s="82" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="E55" s="195" t="s">
         <v>776</v>
@@ -38158,7 +38487,7 @@
         <v>891</v>
       </c>
       <c r="D56" s="82" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="E56" s="195" t="s">
         <v>776</v>
@@ -38171,12 +38500,12 @@
       <c r="A57" s="71">
         <v>42736</v>
       </c>
-      <c r="B57" s="72"/>
+      <c r="B57" s="69"/>
       <c r="C57" s="65" t="s">
         <v>891</v>
       </c>
-      <c r="D57" s="88" t="s">
-        <v>841</v>
+      <c r="D57" s="82" t="s">
+        <v>839</v>
       </c>
       <c r="E57" s="195" t="s">
         <v>776</v>
@@ -38186,38 +38515,56 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="263">
-        <v>42736</v>
-      </c>
-      <c r="B58" s="419"/>
-      <c r="C58" s="73" t="s">
+      <c r="A58" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B58" s="72"/>
+      <c r="C58" s="65" t="s">
+        <v>891</v>
+      </c>
+      <c r="D58" s="88" t="s">
+        <v>841</v>
+      </c>
+      <c r="E58" s="195" t="s">
+        <v>776</v>
+      </c>
+      <c r="F58" s="125" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="263">
+        <v>42736</v>
+      </c>
+      <c r="B59" s="419"/>
+      <c r="C59" s="73" t="s">
         <v>882</v>
       </c>
-      <c r="D58" s="265" t="s">
+      <c r="D59" s="265" t="s">
         <v>392</v>
-      </c>
-      <c r="E58" s="418" t="s">
-        <v>943</v>
-      </c>
-      <c r="F58" s="266" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B59" s="81"/>
-      <c r="C59" s="62" t="s">
-        <v>882</v>
-      </c>
-      <c r="D59" s="65" t="s">
-        <v>941</v>
       </c>
       <c r="E59" s="418" t="s">
         <v>943</v>
       </c>
-      <c r="F59" s="115" t="s">
+      <c r="F59" s="266" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B60" s="81"/>
+      <c r="C60" s="62" t="s">
+        <v>882</v>
+      </c>
+      <c r="D60" s="65" t="s">
+        <v>941</v>
+      </c>
+      <c r="E60" s="418" t="s">
+        <v>943</v>
+      </c>
+      <c r="F60" s="115" t="s">
         <v>339</v>
       </c>
     </row>
@@ -39045,7 +39392,7 @@
       </c>
       <c r="B36" s="72"/>
       <c r="C36" s="292" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D36" s="293" t="s">
         <v>489</v>
@@ -39063,7 +39410,7 @@
       </c>
       <c r="B37" s="72"/>
       <c r="C37" s="292" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D37" s="293" t="s">
         <v>493</v>
@@ -39081,7 +39428,7 @@
       </c>
       <c r="B38" s="72"/>
       <c r="C38" s="292" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D38" s="293" t="s">
         <v>1052</v>
@@ -39099,7 +39446,7 @@
       </c>
       <c r="B39" s="72"/>
       <c r="C39" s="292" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D39" s="293" t="s">
         <v>1054</v>
@@ -39117,7 +39464,7 @@
       </c>
       <c r="B40" s="72"/>
       <c r="C40" s="292" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D40" s="293" t="s">
         <v>1056</v>
@@ -39613,10 +39960,10 @@
       </c>
       <c r="B19" s="409"/>
       <c r="C19" s="130" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D19" s="130" t="s">
         <v>1060</v>
-      </c>
-      <c r="D19" s="130" t="s">
-        <v>1061</v>
       </c>
       <c r="E19" s="409" t="s">
         <v>1050</v>
@@ -40013,8 +40360,8 @@
   <dimension ref="A1:IO147"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D128" sqref="D128"/>
+      <pane ySplit="3" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -47453,7 +47800,7 @@
       </c>
       <c r="B127" s="463"/>
       <c r="C127" s="385" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D127" s="464" t="s">
         <v>54</v>
@@ -47718,7 +48065,7 @@
       </c>
       <c r="B128" s="463"/>
       <c r="C128" s="464" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D128" s="464" t="s">
         <v>57</v>
@@ -47983,7 +48330,7 @@
       </c>
       <c r="B129" s="463"/>
       <c r="C129" s="464" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D129" s="464" t="s">
         <v>60</v>
@@ -48248,7 +48595,7 @@
       </c>
       <c r="B130" s="463"/>
       <c r="C130" s="464" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D130" s="464" t="s">
         <v>63</v>
@@ -48513,7 +48860,7 @@
       </c>
       <c r="B131" s="463"/>
       <c r="C131" s="464" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D131" s="464" t="s">
         <v>66</v>
@@ -48778,7 +49125,7 @@
       </c>
       <c r="B132" s="463"/>
       <c r="C132" s="464" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D132" s="464" t="s">
         <v>69</v>
@@ -49043,7 +49390,7 @@
       </c>
       <c r="B133" s="463"/>
       <c r="C133" s="464" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D133" s="385" t="s">
         <v>72</v>
@@ -49308,7 +49655,7 @@
       </c>
       <c r="B134" s="463"/>
       <c r="C134" s="464" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D134" s="464" t="s">
         <v>83</v>
@@ -49575,7 +49922,7 @@
       </c>
       <c r="B135" s="463"/>
       <c r="C135" s="464" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D135" s="464" t="s">
         <v>87</v>
@@ -49840,7 +50187,7 @@
       </c>
       <c r="B136" s="463"/>
       <c r="C136" s="464" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D136" s="464" t="s">
         <v>93</v>
@@ -50105,7 +50452,7 @@
       </c>
       <c r="B137" s="463"/>
       <c r="C137" s="464" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D137" s="464" t="s">
         <v>96</v>
@@ -50674,7 +51021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C10" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
@@ -54418,8 +54765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RDM-9587 Conditional Post States - updateCase2 condition update
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-api-test-automation-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1CC26F-D7FB-A347-9D23-3D08D66F9AA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF47493D-62E6-9049-9699-C9BC155A8370}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="2000" windowWidth="35340" windowHeight="19340" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="2000" windowWidth="35340" windowHeight="19340" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -3328,9 +3328,6 @@
     <t>FT-Conditional Post State</t>
   </si>
   <si>
-    <t>CaseUpdated2(TextField="updated2" OR EmailField="*"):1;CaseAmended2(TextField="amended2" OR EmailField="matched@test.com"):2;*(TextField="keepstate"):3;CaseRevoked2(EmailField!=""):4;CaseDeleted</t>
-  </si>
-  <si>
     <t>CaseUpdated(TextField="updated" AND EmailField="*"):1;CaseAmended(TextField="amended" AND EmailField="*"):2;CaseRevoked(AddressField.AddressLine1="Some address" AND EmailField="*"):3;CaseDeleted</t>
   </si>
   <si>
@@ -3356,6 +3353,9 @@
   </si>
   <si>
     <t>Revoke case 2</t>
+  </si>
+  <si>
+    <t>CaseUpdated2(TextField="updated2" AND EmailField="*"):1;CaseAmended2(TextField="amended2" OR EmailField="matched@test.com"):2;*(TextField="keepstate"):3;CaseRevoked2(EmailField!=""):4;CaseDeleted</t>
   </si>
 </sst>
 </file>
@@ -18643,10 +18643,10 @@
         <v>1059</v>
       </c>
       <c r="D36" s="62" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E36" s="62" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="F36" s="81"/>
       <c r="G36" s="80">
@@ -18663,10 +18663,10 @@
         <v>1059</v>
       </c>
       <c r="D37" s="62" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E37" s="62" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F37" s="81"/>
       <c r="G37" s="80">
@@ -18683,10 +18683,10 @@
         <v>1059</v>
       </c>
       <c r="D38" s="62" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E38" s="62" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="F38" s="81"/>
       <c r="G38" s="80">
@@ -18735,8 +18735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A24" zoomScale="109" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="109" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20608,7 +20608,7 @@
         <v>489</v>
       </c>
       <c r="I44" s="547" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="J44" s="548"/>
       <c r="K44" s="548"/>
@@ -20635,13 +20635,13 @@
         <v>1059</v>
       </c>
       <c r="D45" s="551" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E45" s="551" t="s">
         <v>1063</v>
       </c>
-      <c r="E45" s="551" t="s">
-        <v>1064</v>
-      </c>
       <c r="F45" s="545" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="G45" s="546">
         <v>3</v>
@@ -20650,7 +20650,7 @@
         <v>489</v>
       </c>
       <c r="I45" s="547" t="s">
-        <v>1061</v>
+        <v>1070</v>
       </c>
       <c r="J45" s="548"/>
       <c r="K45" s="548"/>
@@ -20973,7 +20973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R189"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A148" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A148" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
@@ -28107,7 +28107,7 @@
         <v>1059</v>
       </c>
       <c r="D176" s="547" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E176" s="545" t="s">
         <v>54</v>
@@ -28147,7 +28147,7 @@
         <v>1059</v>
       </c>
       <c r="D177" s="547" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E177" s="545" t="s">
         <v>93</v>
@@ -38397,7 +38397,7 @@
         <v>1059</v>
       </c>
       <c r="D51" s="68" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E51" s="84" t="s">
         <v>776</v>

</xml_diff>

<commit_message>
RDM-10823 updated master config
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B61840-9AA6-084C-B401-EEB0A8EBC65D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038C75CA-9589-BF4E-AC7B-EED78C90E349}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1720" windowWidth="33600" windowHeight="20540" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="1720" windowWidth="33600" windowHeight="20540" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -22917,8 +22917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S219"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A198" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A220" sqref="A220:XFD1048576"/>
+    <sheetView showGridLines="0" topLeftCell="A202" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C218" sqref="C218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -46066,8 +46066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -56647,8 +56647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M249"/>
   <sheetViews>
-    <sheetView topLeftCell="J165" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N165" sqref="N1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -57059,9 +57059,7 @@
       <c r="L13" s="175" t="s">
         <v>376</v>
       </c>
-      <c r="M13" s="72" t="b">
-        <v>1</v>
-      </c>
+      <c r="M13" s="72"/>
     </row>
     <row r="14" spans="1:13" s="336" customFormat="1" ht="20" customHeight="1">
       <c r="A14" s="194">

</xml_diff>

<commit_message>
RDM-10823 removed empty column
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038C75CA-9589-BF4E-AC7B-EED78C90E349}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F929F9AA-F3CB-EE41-B0C3-3615863E517D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1720" windowWidth="33600" windowHeight="20540" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="1720" windowWidth="33600" windowHeight="20540" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8867" uniqueCount="1166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8869" uniqueCount="1165">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3622,9 +3622,6 @@
   </si>
   <si>
     <t>Case Type for testing RetainHiddenValue</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
   <si>
     <t>1</t>
@@ -5820,7 +5817,7 @@
     <cellStyle name="Normal 2 3" xfId="13" xr:uid="{983C50BB-8B6C-1941-95CA-614B186AEA1E}"/>
     <cellStyle name="Normal 3" xfId="15" xr:uid="{B38533D7-3FBF-F547-ABBC-CA99BE96DA12}"/>
   </cellStyles>
-  <dxfs count="342">
+  <dxfs count="341">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -9039,35 +9036,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -14141,106 +14109,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="341" dataDxfId="339" headerRowBorderDxfId="340" tableBorderDxfId="338" totalsRowBorderDxfId="337">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="340" dataDxfId="338" headerRowBorderDxfId="339" tableBorderDxfId="337" totalsRowBorderDxfId="336">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="336"/>
-    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="335"/>
-    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="334"/>
-    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="333"/>
-    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="332"/>
+    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="335"/>
+    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="334"/>
+    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="333"/>
+    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="332"/>
+    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="331"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L91" totalsRowShown="0" headerRowDxfId="209" dataDxfId="207" headerRowBorderDxfId="208" tableBorderDxfId="206" totalsRowBorderDxfId="205">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L91" totalsRowShown="0" headerRowDxfId="208" dataDxfId="206" headerRowBorderDxfId="207" tableBorderDxfId="205" totalsRowBorderDxfId="204">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="204"/>
-    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="203"/>
-    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="202"/>
-    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="201"/>
-    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="200"/>
-    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="199"/>
-    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="198"/>
-    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="197"/>
-    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="196"/>
-    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="195"/>
-    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="194"/>
-    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="193"/>
+    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="203"/>
+    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="202"/>
+    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="201"/>
+    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="200"/>
+    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="199"/>
+    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="198"/>
+    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="197"/>
+    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="196"/>
+    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="195"/>
+    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="194"/>
+    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="193"/>
+    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="192"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H43" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191" tableBorderDxfId="189" totalsRowBorderDxfId="188">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H43" totalsRowShown="0" headerRowDxfId="191" dataDxfId="189" headerRowBorderDxfId="190" tableBorderDxfId="188" totalsRowBorderDxfId="187">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="187"/>
-    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="186"/>
-    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="185"/>
-    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="184"/>
-    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="183"/>
-    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="182"/>
-    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="181"/>
-    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="180"/>
+    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="186"/>
+    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="185"/>
+    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="184"/>
+    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="183"/>
+    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="182"/>
+    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="181"/>
+    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="180"/>
+    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="179"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:V63" totalsRowShown="0" headerRowDxfId="179" dataDxfId="177" headerRowBorderDxfId="178" tableBorderDxfId="176" totalsRowBorderDxfId="175">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:V63" totalsRowShown="0" headerRowDxfId="178" dataDxfId="176" headerRowBorderDxfId="177" tableBorderDxfId="175" totalsRowBorderDxfId="174">
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="174"/>
-    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="173"/>
-    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="172"/>
-    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="171"/>
-    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="170"/>
-    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="169"/>
-    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="168"/>
-    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="167"/>
-    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="166"/>
-    <tableColumn id="22" xr3:uid="{59B33952-3C10-D94F-9012-529644363CBA}" name="EventEnablingCondition" dataDxfId="165"/>
-    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="164" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="163"/>
-    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="162"/>
-    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="161"/>
-    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="160"/>
-    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="159"/>
-    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="158"/>
-    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="157"/>
-    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="156"/>
-    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="155"/>
-    <tableColumn id="21" xr3:uid="{04E7CE93-2C4A-2C46-91EF-227CE86C5C37}" name="EndButtonLabel" dataDxfId="154"/>
-    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="Publish" dataDxfId="153"/>
+    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="173"/>
+    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="172"/>
+    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="171"/>
+    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="170"/>
+    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="169"/>
+    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="168"/>
+    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="167"/>
+    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="166"/>
+    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="165"/>
+    <tableColumn id="22" xr3:uid="{59B33952-3C10-D94F-9012-529644363CBA}" name="EventEnablingCondition" dataDxfId="164"/>
+    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="163" dataCellStyle="Hyperlink"/>
+    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="162"/>
+    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="161"/>
+    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="160"/>
+    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="159"/>
+    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="158"/>
+    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="157"/>
+    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="156"/>
+    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="155"/>
+    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="154"/>
+    <tableColumn id="21" xr3:uid="{04E7CE93-2C4A-2C46-91EF-227CE86C5C37}" name="EndButtonLabel" dataDxfId="153"/>
+    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="Publish" dataDxfId="152"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:S219" totalsRowShown="0" headerRowDxfId="152" dataDxfId="150" headerRowBorderDxfId="151" tableBorderDxfId="149" totalsRowBorderDxfId="148">
-  <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="147"/>
-    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="146"/>
-    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="145"/>
-    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="144"/>
-    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="143"/>
-    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="142"/>
-    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="141"/>
-    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="140"/>
-    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="139"/>
-    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="138"/>
-    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="137"/>
-    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="136"/>
-    <tableColumn id="18" xr3:uid="{E135335A-D7E2-F744-932E-E0627D2DBFE1}" name="RetainHiddenValue" dataDxfId="135"/>
-    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="134"/>
-    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="133"/>
-    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="132"/>
-    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="131"/>
-    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="130"/>
-    <tableColumn id="19" xr3:uid="{D7143D13-75D4-AD48-8FBF-BDDB0F384091}" name="Column1" dataDxfId="129"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:R219" totalsRowShown="0" headerRowDxfId="151" dataDxfId="149" headerRowBorderDxfId="150" tableBorderDxfId="148" totalsRowBorderDxfId="147">
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="146"/>
+    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="145"/>
+    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="144"/>
+    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="143"/>
+    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="142"/>
+    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="141"/>
+    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="140"/>
+    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="139"/>
+    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="138"/>
+    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="137"/>
+    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="136"/>
+    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="135"/>
+    <tableColumn id="18" xr3:uid="{E135335A-D7E2-F744-932E-E0627D2DBFE1}" name="RetainHiddenValue" dataDxfId="134"/>
+    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="133"/>
+    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="132"/>
+    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="131"/>
+    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="130"/>
+    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14346,12 +14313,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="331" dataDxfId="329" headerRowBorderDxfId="330" tableBorderDxfId="328" totalsRowBorderDxfId="327">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="330" dataDxfId="328" headerRowBorderDxfId="329" tableBorderDxfId="327" totalsRowBorderDxfId="326">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="326"/>
-    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="325"/>
-    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="324"/>
-    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="323" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="325"/>
+    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="324"/>
+    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="323"/>
+    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="322" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14425,137 +14392,137 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I24" totalsRowShown="0" headerRowDxfId="322" dataDxfId="320" headerRowBorderDxfId="321" tableBorderDxfId="319" totalsRowBorderDxfId="318">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I24" totalsRowShown="0" headerRowDxfId="321" dataDxfId="319" headerRowBorderDxfId="320" tableBorderDxfId="318" totalsRowBorderDxfId="317">
   <autoFilter ref="A3:I24" xr:uid="{C0075E79-5DBE-654F-827E-CA137EF61FB4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="317"/>
-    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="316"/>
-    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="315"/>
-    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="314"/>
-    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="313"/>
-    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="312"/>
-    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="311"/>
-    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="310"/>
-    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="309"/>
+    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="316"/>
+    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="315"/>
+    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="314"/>
+    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="313"/>
+    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="312"/>
+    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="311"/>
+    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="310"/>
+    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="309"/>
+    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="308"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:O177" totalsRowShown="0" headerRowDxfId="308" dataDxfId="306" headerRowBorderDxfId="307" tableBorderDxfId="305" totalsRowBorderDxfId="304">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:O177" totalsRowShown="0" headerRowDxfId="307" dataDxfId="305" headerRowBorderDxfId="306" tableBorderDxfId="304" totalsRowBorderDxfId="303">
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="303"/>
-    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="302"/>
-    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="301"/>
-    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="300"/>
-    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="299"/>
-    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="298"/>
-    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="297"/>
-    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="296"/>
-    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="295"/>
-    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="294"/>
-    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="293"/>
-    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="292"/>
-    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="291"/>
-    <tableColumn id="14" xr3:uid="{04523CC4-7DD9-BC4B-BEE9-93E1915A632A}" name="DefaultHidden" dataDxfId="290"/>
-    <tableColumn id="15" xr3:uid="{DB795945-BA18-EE44-815E-AD737CF2E8DD}" name="Searchable" dataDxfId="289"/>
+    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="302"/>
+    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="301"/>
+    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="300"/>
+    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="299"/>
+    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="298"/>
+    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="297"/>
+    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="296"/>
+    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="295"/>
+    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="294"/>
+    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="293"/>
+    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="292"/>
+    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="291"/>
+    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="290"/>
+    <tableColumn id="14" xr3:uid="{04523CC4-7DD9-BC4B-BEE9-93E1915A632A}" name="DefaultHidden" dataDxfId="289"/>
+    <tableColumn id="15" xr3:uid="{DB795945-BA18-EE44-815E-AD737CF2E8DD}" name="Searchable" dataDxfId="288"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:T88" totalsRowShown="0" headerRowDxfId="288" dataDxfId="286" headerRowBorderDxfId="287" tableBorderDxfId="285" totalsRowBorderDxfId="284">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:T88" totalsRowShown="0" headerRowDxfId="287" dataDxfId="285" headerRowBorderDxfId="286" tableBorderDxfId="284" totalsRowBorderDxfId="283">
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="283"/>
-    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="282"/>
-    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="281"/>
-    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="280"/>
-    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="279"/>
-    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="278"/>
-    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="277"/>
-    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="276"/>
-    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="275"/>
-    <tableColumn id="20" xr3:uid="{3056D2D9-052A-4948-A9B6-EA6D4AEEE813}" name="RetainHiddenValue" dataDxfId="274"/>
-    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="273"/>
-    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="272"/>
-    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="271"/>
-    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="270"/>
-    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="269"/>
-    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="268"/>
-    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="267"/>
-    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="266"/>
-    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="265"/>
-    <tableColumn id="19" xr3:uid="{4721EA60-AB43-3A4D-9D3A-D995D789F1AA}" name="Searchable" dataDxfId="264"/>
+    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="282"/>
+    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="281"/>
+    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="280"/>
+    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="279"/>
+    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="278"/>
+    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="277"/>
+    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="276"/>
+    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="275"/>
+    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="274"/>
+    <tableColumn id="20" xr3:uid="{3056D2D9-052A-4948-A9B6-EA6D4AEEE813}" name="RetainHiddenValue" dataDxfId="273"/>
+    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="272"/>
+    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="271"/>
+    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="270"/>
+    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="269"/>
+    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="268"/>
+    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="267"/>
+    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="266"/>
+    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="265"/>
+    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="264"/>
+    <tableColumn id="19" xr3:uid="{4721EA60-AB43-3A4D-9D3A-D995D789F1AA}" name="Searchable" dataDxfId="263"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G48" totalsRowShown="0" headerRowDxfId="263" dataDxfId="261" headerRowBorderDxfId="262" tableBorderDxfId="260" totalsRowBorderDxfId="259" headerRowCellStyle="Normal 2 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G48" totalsRowShown="0" headerRowDxfId="262" dataDxfId="260" headerRowBorderDxfId="261" tableBorderDxfId="259" totalsRowBorderDxfId="258" headerRowCellStyle="Normal 2 3">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="258"/>
-    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="257"/>
-    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="256"/>
-    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="255"/>
-    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="254"/>
-    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="253"/>
-    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="252"/>
+    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="257"/>
+    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="256"/>
+    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="255"/>
+    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="254"/>
+    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="253"/>
+    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="252"/>
+    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="251"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:M249" totalsRowShown="0" headerRowDxfId="251" dataDxfId="249" headerRowBorderDxfId="250" tableBorderDxfId="248" totalsRowBorderDxfId="247">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:M249" totalsRowShown="0" headerRowDxfId="250" dataDxfId="248" headerRowBorderDxfId="249" tableBorderDxfId="247" totalsRowBorderDxfId="246">
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="246"/>
-    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="245"/>
-    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="244"/>
-    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="243"/>
-    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="242"/>
-    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="241"/>
-    <tableColumn id="12" xr3:uid="{4E9EBE21-1E8A-8F42-8DBF-15D634A7D163}" name="DefaultValue" dataDxfId="240"/>
-    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="239"/>
-    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="238"/>
-    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="237"/>
-    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="236"/>
-    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="235"/>
-    <tableColumn id="13" xr3:uid="{A39B3867-9E61-F640-871A-7CF7654CCAC8}" name="RetainHiddenValue" dataDxfId="234"/>
+    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="245"/>
+    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="244"/>
+    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="243"/>
+    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="242"/>
+    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="241"/>
+    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="240"/>
+    <tableColumn id="12" xr3:uid="{4E9EBE21-1E8A-8F42-8DBF-15D634A7D163}" name="DefaultValue" dataDxfId="239"/>
+    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="238"/>
+    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="237"/>
+    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="236"/>
+    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="235"/>
+    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="234"/>
+    <tableColumn id="13" xr3:uid="{A39B3867-9E61-F640-871A-7CF7654CCAC8}" name="RetainHiddenValue" dataDxfId="233"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G33" totalsRowShown="0" headerRowDxfId="233" dataDxfId="231" headerRowBorderDxfId="232" tableBorderDxfId="230" totalsRowBorderDxfId="229">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G33" totalsRowShown="0" headerRowDxfId="232" dataDxfId="230" headerRowBorderDxfId="231" tableBorderDxfId="229" totalsRowBorderDxfId="228">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="228"/>
-    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="227"/>
-    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="226"/>
-    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="225"/>
-    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="224"/>
-    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="223"/>
-    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="222"/>
+    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="227"/>
+    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="226"/>
+    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="225"/>
+    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="224"/>
+    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="223"/>
+    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="222"/>
+    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="221"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A2772D57-E59F-2C49-82BA-2F8A826F981B}" name="Table24" displayName="Table24" ref="A3:I15" totalsRowShown="0" headerRowDxfId="221" dataDxfId="219" headerRowBorderDxfId="220">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A2772D57-E59F-2C49-82BA-2F8A826F981B}" name="Table24" displayName="Table24" ref="A3:I15" totalsRowShown="0" headerRowDxfId="220" dataDxfId="218" headerRowBorderDxfId="219">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{EB3897FA-8398-4645-B06C-A22BA473519E}" name="LiveTo" dataDxfId="218"/>
-    <tableColumn id="2" xr3:uid="{99353927-15FC-BA4C-B4D7-FDA6EA43AF10}" name="CaseTypeID" dataDxfId="217"/>
-    <tableColumn id="3" xr3:uid="{E2107A93-C2C9-FC44-A5C0-F1560E2CFFDB}" name="ID" dataDxfId="216"/>
-    <tableColumn id="4" xr3:uid="{483E458F-23BC-6442-BCE1-4A5DD98775C7}" name="DisplayOrder" dataDxfId="215"/>
-    <tableColumn id="5" xr3:uid="{3129676F-8344-B24B-B2CD-3FD0837952C2}" name="QuestionText" dataDxfId="214"/>
-    <tableColumn id="6" xr3:uid="{000B8220-15DF-854E-A0BC-F1BBBCF401A4}" name="AnswerFieldType" dataDxfId="213"/>
-    <tableColumn id="7" xr3:uid="{A0E53177-56A8-E14F-A7BD-F9796CA3E5D4}" name="DisplayContextParameter" dataDxfId="212"/>
-    <tableColumn id="8" xr3:uid="{8526709A-AE28-FE44-BFBB-69DF75B42A88}" name="Answer" dataDxfId="211"/>
-    <tableColumn id="9" xr3:uid="{D53C393B-D23F-F64C-8796-C256647586C5}" name="QuestionId" dataDxfId="210"/>
+    <tableColumn id="1" xr3:uid="{EB3897FA-8398-4645-B06C-A22BA473519E}" name="LiveTo" dataDxfId="217"/>
+    <tableColumn id="2" xr3:uid="{99353927-15FC-BA4C-B4D7-FDA6EA43AF10}" name="CaseTypeID" dataDxfId="216"/>
+    <tableColumn id="3" xr3:uid="{E2107A93-C2C9-FC44-A5C0-F1560E2CFFDB}" name="ID" dataDxfId="215"/>
+    <tableColumn id="4" xr3:uid="{483E458F-23BC-6442-BCE1-4A5DD98775C7}" name="DisplayOrder" dataDxfId="214"/>
+    <tableColumn id="5" xr3:uid="{3129676F-8344-B24B-B2CD-3FD0837952C2}" name="QuestionText" dataDxfId="213"/>
+    <tableColumn id="6" xr3:uid="{000B8220-15DF-854E-A0BC-F1BBBCF401A4}" name="AnswerFieldType" dataDxfId="212"/>
+    <tableColumn id="7" xr3:uid="{A0E53177-56A8-E14F-A7BD-F9796CA3E5D4}" name="DisplayContextParameter" dataDxfId="211"/>
+    <tableColumn id="8" xr3:uid="{8526709A-AE28-FE44-BFBB-69DF75B42A88}" name="Answer" dataDxfId="210"/>
+    <tableColumn id="9" xr3:uid="{D53C393B-D23F-F64C-8796-C256647586C5}" name="QuestionId" dataDxfId="209"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -22915,10 +22882,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:S219"/>
+  <dimension ref="A1:R219"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A202" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C218" sqref="C218"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -22942,7 +22909,7 @@
     <col min="18" max="16384" width="8.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1">
+    <row r="1" spans="1:18" ht="18" customHeight="1">
       <c r="A1" s="82" t="s">
         <v>574</v>
       </c>
@@ -22970,7 +22937,7 @@
       <c r="Q1" s="90"/>
       <c r="R1" s="34"/>
     </row>
-    <row r="2" spans="1:19" ht="68.75" customHeight="1">
+    <row r="2" spans="1:18" ht="68.75" customHeight="1">
       <c r="A2" s="88" t="s">
         <v>4</v>
       </c>
@@ -23022,7 +22989,7 @@
       </c>
       <c r="R2" s="34"/>
     </row>
-    <row r="3" spans="1:19" s="50" customFormat="1" ht="20" customHeight="1">
+    <row r="3" spans="1:18" s="50" customFormat="1" ht="20" customHeight="1">
       <c r="A3" s="366" t="s">
         <v>9</v>
       </c>
@@ -23077,11 +23044,8 @@
       <c r="R3" s="413" t="s">
         <v>594</v>
       </c>
-      <c r="S3" s="50" t="s">
-        <v>1162</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" s="517" customFormat="1" ht="20" customHeight="1">
+    </row>
+    <row r="4" spans="1:18" s="517" customFormat="1" ht="20" customHeight="1">
       <c r="A4" s="53">
         <v>42736</v>
       </c>
@@ -23121,7 +23085,7 @@
       <c r="Q4" s="72"/>
       <c r="R4" s="72"/>
     </row>
-    <row r="5" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="5" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A5" s="53">
         <v>42736</v>
       </c>
@@ -23154,7 +23118,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="6" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A6" s="53">
         <v>42736</v>
       </c>
@@ -23187,7 +23151,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="7" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A7" s="53">
         <v>42736</v>
       </c>
@@ -23220,7 +23184,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="8" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A8" s="53">
         <v>42736</v>
       </c>
@@ -23253,7 +23217,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="9" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A9" s="53">
         <v>42736</v>
       </c>
@@ -23286,7 +23250,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="10" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A10" s="53">
         <v>42736</v>
       </c>
@@ -23319,7 +23283,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="11" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A11" s="53">
         <v>42736</v>
       </c>
@@ -23352,7 +23316,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="75" customFormat="1" ht="20" customHeight="1">
+    <row r="12" spans="1:18" s="75" customFormat="1" ht="20" customHeight="1">
       <c r="A12" s="59">
         <v>42736</v>
       </c>
@@ -23385,7 +23349,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="13" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A13" s="109">
         <v>42737</v>
       </c>
@@ -23424,7 +23388,7 @@
       </c>
       <c r="Q13" s="110"/>
     </row>
-    <row r="14" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="14" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A14" s="53">
         <v>42736</v>
       </c>
@@ -23457,7 +23421,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="15" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A15" s="53">
         <v>42736</v>
       </c>
@@ -23490,7 +23454,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="16" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A16" s="53">
         <v>42736</v>
       </c>
@@ -30986,7 +30950,7 @@
       <c r="Q208" s="61"/>
       <c r="R208" s="56"/>
     </row>
-    <row r="209" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="209" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A209" s="59">
         <v>42736</v>
       </c>
@@ -31026,7 +30990,7 @@
       <c r="Q209" s="61"/>
       <c r="R209" s="56"/>
     </row>
-    <row r="210" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="210" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A210" s="59">
         <v>42736</v>
       </c>
@@ -31066,7 +31030,7 @@
       <c r="Q210" s="61"/>
       <c r="R210" s="56"/>
     </row>
-    <row r="211" spans="1:19" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="211" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A211" s="59">
         <v>42736</v>
       </c>
@@ -31106,7 +31070,7 @@
       <c r="Q211" s="61"/>
       <c r="R211" s="56"/>
     </row>
-    <row r="212" spans="1:19" s="72" customFormat="1" ht="13.25" customHeight="1">
+    <row r="212" spans="1:18" s="72" customFormat="1" ht="13.25" customHeight="1">
       <c r="A212" s="59">
         <v>42736</v>
       </c>
@@ -31121,7 +31085,7 @@
         <v>69</v>
       </c>
       <c r="F212" s="54" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="G212" s="57" t="s">
         <v>375</v>
@@ -31130,22 +31094,23 @@
         <v>596</v>
       </c>
       <c r="I212" s="57" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J212" s="54" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="K212" s="54"/>
       <c r="L212" s="54"/>
       <c r="M212" s="54"/>
       <c r="N212" s="54"/>
       <c r="O212" s="54"/>
-      <c r="P212" s="54"/>
+      <c r="P212" s="54" t="s">
+        <v>532</v>
+      </c>
       <c r="Q212" s="54"/>
       <c r="R212" s="54"/>
-      <c r="S212" s="54"/>
-    </row>
-    <row r="213" spans="1:19" s="72" customFormat="1" ht="13.25" customHeight="1">
+    </row>
+    <row r="213" spans="1:18" s="72" customFormat="1" ht="13.25" customHeight="1">
       <c r="A213" s="59">
         <v>42736</v>
       </c>
@@ -31160,7 +31125,7 @@
         <v>54</v>
       </c>
       <c r="F213" s="61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G213" s="57" t="s">
         <v>375</v>
@@ -31169,14 +31134,14 @@
         <v>596</v>
       </c>
       <c r="I213" s="57" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J213" s="71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K213" s="61"/>
       <c r="L213" s="54" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="M213" s="61" t="b">
         <v>1</v>
@@ -31189,7 +31154,7 @@
       <c r="Q213" s="61"/>
       <c r="R213" s="56"/>
     </row>
-    <row r="214" spans="1:19" s="72" customFormat="1" ht="13.25" customHeight="1">
+    <row r="214" spans="1:18" s="72" customFormat="1" ht="13.25" customHeight="1">
       <c r="A214" s="59">
         <v>42736</v>
       </c>
@@ -31204,7 +31169,7 @@
         <v>57</v>
       </c>
       <c r="F214" s="61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G214" s="57" t="s">
         <v>375</v>
@@ -31213,14 +31178,14 @@
         <v>596</v>
       </c>
       <c r="I214" s="57" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J214" s="71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K214" s="61"/>
       <c r="L214" s="54" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="M214" s="61" t="b">
         <v>0</v>
@@ -31233,7 +31198,7 @@
       <c r="Q214" s="61"/>
       <c r="R214" s="56"/>
     </row>
-    <row r="215" spans="1:19" s="72" customFormat="1" ht="13.25" customHeight="1">
+    <row r="215" spans="1:18" s="72" customFormat="1" ht="13.25" customHeight="1">
       <c r="A215" s="59">
         <v>42736</v>
       </c>
@@ -31248,7 +31213,7 @@
         <v>60</v>
       </c>
       <c r="F215" s="61">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G215" s="57" t="s">
         <v>375</v>
@@ -31257,14 +31222,14 @@
         <v>596</v>
       </c>
       <c r="I215" s="57" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J215" s="71">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K215" s="61"/>
       <c r="L215" s="54" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="M215" s="61"/>
       <c r="N215" s="61"/>
@@ -31275,7 +31240,7 @@
       <c r="Q215" s="61"/>
       <c r="R215" s="56"/>
     </row>
-    <row r="216" spans="1:19" s="72" customFormat="1" ht="13.25" customHeight="1">
+    <row r="216" spans="1:18" s="72" customFormat="1" ht="13.25" customHeight="1">
       <c r="A216" s="59">
         <v>42736</v>
       </c>
@@ -31290,7 +31255,7 @@
         <v>69</v>
       </c>
       <c r="F216" s="54" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="G216" s="57" t="s">
         <v>375</v>
@@ -31299,22 +31264,23 @@
         <v>596</v>
       </c>
       <c r="I216" s="57" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J216" s="54" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="K216" s="54"/>
       <c r="L216" s="54"/>
       <c r="M216" s="54"/>
       <c r="N216" s="54"/>
       <c r="O216" s="54"/>
-      <c r="P216" s="54"/>
+      <c r="P216" s="54" t="s">
+        <v>532</v>
+      </c>
       <c r="Q216" s="54"/>
       <c r="R216" s="54"/>
-      <c r="S216" s="54"/>
-    </row>
-    <row r="217" spans="1:19" s="72" customFormat="1" ht="13.25" customHeight="1">
+    </row>
+    <row r="217" spans="1:18" s="72" customFormat="1" ht="13.25" customHeight="1">
       <c r="A217" s="59">
         <v>42736</v>
       </c>
@@ -31329,7 +31295,7 @@
         <v>114</v>
       </c>
       <c r="F217" s="61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G217" s="57" t="s">
         <v>375</v>
@@ -31338,14 +31304,14 @@
         <v>596</v>
       </c>
       <c r="I217" s="57" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J217" s="71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K217" s="61"/>
       <c r="L217" s="54" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="M217" s="61" t="b">
         <v>1</v>
@@ -31358,7 +31324,7 @@
       <c r="Q217" s="61"/>
       <c r="R217" s="56"/>
     </row>
-    <row r="218" spans="1:19" s="72" customFormat="1" ht="13.25" customHeight="1">
+    <row r="218" spans="1:18" s="72" customFormat="1" ht="13.25" customHeight="1">
       <c r="A218" s="59">
         <v>42736</v>
       </c>
@@ -31373,7 +31339,7 @@
         <v>69</v>
       </c>
       <c r="F218" s="54" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="G218" s="57" t="s">
         <v>375</v>
@@ -31382,22 +31348,23 @@
         <v>596</v>
       </c>
       <c r="I218" s="57" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J218" s="54" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="K218" s="54"/>
       <c r="L218" s="54"/>
       <c r="M218" s="54"/>
       <c r="N218" s="54"/>
       <c r="O218" s="54"/>
-      <c r="P218" s="54"/>
+      <c r="P218" s="54" t="s">
+        <v>532</v>
+      </c>
       <c r="Q218" s="54"/>
       <c r="R218" s="54"/>
-      <c r="S218" s="54"/>
-    </row>
-    <row r="219" spans="1:19" s="284" customFormat="1" ht="13.25" customHeight="1">
+    </row>
+    <row r="219" spans="1:18" s="284" customFormat="1" ht="13.25" customHeight="1">
       <c r="A219" s="59">
         <v>42736</v>
       </c>
@@ -31412,7 +31379,7 @@
         <v>124</v>
       </c>
       <c r="F219" s="61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G219" s="65" t="s">
         <v>608</v>
@@ -31421,14 +31388,14 @@
         <v>596</v>
       </c>
       <c r="I219" s="57" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J219" s="523">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K219" s="64"/>
       <c r="L219" s="54" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="M219" s="64" t="b">
         <v>1</v>
@@ -56647,7 +56614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RDM-10823 formatted config and tidy up
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587E3777-C131-6543-AC33-1B380F1F3014}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B6E5A5-73B6-BA41-99F4-AFBAC21DDC83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1720" windowWidth="33600" windowHeight="20540" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="1720" windowWidth="33600" windowHeight="20540" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8869" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8870" uniqueCount="1165">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -52517,8 +52517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T88"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView showGridLines="0" topLeftCell="C20" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -53489,7 +53489,9 @@
       <c r="I27" s="54" t="s">
         <v>973</v>
       </c>
-      <c r="J27" s="54"/>
+      <c r="J27" s="54" t="s">
+        <v>424</v>
+      </c>
       <c r="K27" s="72"/>
       <c r="L27" s="72"/>
       <c r="M27" s="54" t="s">
@@ -56626,8 +56628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E224" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D238" sqref="D238"/>
+    <sheetView tabSelected="1" topLeftCell="F220" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M243" sqref="M243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -63713,7 +63715,9 @@
         <v>375</v>
       </c>
       <c r="L240" s="55"/>
-      <c r="M240" s="72"/>
+      <c r="M240" s="72" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="241" spans="1:13" s="336" customFormat="1" ht="20" customHeight="1">
       <c r="A241" s="195">
@@ -63804,9 +63808,7 @@
       <c r="L243" s="175" t="s">
         <v>378</v>
       </c>
-      <c r="M243" s="72" t="b">
-        <v>0</v>
-      </c>
+      <c r="M243" s="72"/>
     </row>
     <row r="244" spans="1:13" s="336" customFormat="1" ht="20" customHeight="1">
       <c r="A244" s="194">

</xml_diff>

<commit_message>
ACA-113: restore BEFTA_Master def file changes
   [ACA-113](https://tools.hmcts.net/jira/browse/ACA-113)

Restore BEFTA_Master def file changes from ACA-113 after merging with
 6.8.0 master branch.
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B6E5A5-73B6-BA41-99F4-AFBAC21DDC83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EFFB6A-7279-FF4E-ADA2-3572A8CC8106}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1720" windowWidth="33600" windowHeight="20540" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="21380" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -3609,28 +3609,28 @@
     <t>${TEST_STUB_SERVICE_BASE_URL:http://ccd-test-stubs-service-aat.service.core-compute-aat.internal}/callback_returning_errors_and_warnings</t>
   </si>
   <si>
-    <t>${TEST_STUB_SERVICE_BASE_URL:http://ccd-test-stubs-service-aat.service.core-compute-aat.internal}/callback_returning_simulated_completed_noc_request</t>
+    <t>FT_RetainHiddenValue</t>
+  </si>
+  <si>
+    <t>FT- Retain Hidden Value</t>
+  </si>
+  <si>
+    <t>Case Type for testing RetainHiddenValue</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Retain Hidden Value Page</t>
+  </si>
+  <si>
+    <t>NumberField!="0"</t>
   </si>
   <si>
     <t>${MCA_API_BASE_URL:http://aac-manage-case-assignment-aat.service.core-compute-aat.internal}/noc/check-noc-approval</t>
   </si>
   <si>
-    <t>FT_RetainHiddenValue</t>
-  </si>
-  <si>
-    <t>FT- Retain Hidden Value</t>
-  </si>
-  <si>
-    <t>Case Type for testing RetainHiddenValue</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Retain Hidden Value Page</t>
-  </si>
-  <si>
-    <t>NumberField!="0"</t>
+    <t>${MCA_API_BASE_URL:http://aac-manage-case-assignment-aat.service.core-compute-aat.internal}/noc/apply-decision</t>
   </si>
 </sst>
 </file>
@@ -4121,6 +4121,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -18765,7 +18766,7 @@
       </c>
       <c r="B84" s="61"/>
       <c r="C84" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D84" s="60" t="s">
         <v>455</v>
@@ -18795,7 +18796,7 @@
       </c>
       <c r="B85" s="61"/>
       <c r="C85" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D85" s="60" t="s">
         <v>455</v>
@@ -18825,7 +18826,7 @@
       </c>
       <c r="B86" s="61"/>
       <c r="C86" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D86" s="60" t="s">
         <v>455</v>
@@ -18855,7 +18856,7 @@
       </c>
       <c r="B87" s="61"/>
       <c r="C87" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D87" s="60" t="s">
         <v>455</v>
@@ -18885,7 +18886,7 @@
       </c>
       <c r="B88" s="61"/>
       <c r="C88" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D88" s="60" t="s">
         <v>455</v>
@@ -18915,7 +18916,7 @@
       </c>
       <c r="B89" s="61"/>
       <c r="C89" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D89" s="60" t="s">
         <v>455</v>
@@ -20018,7 +20019,7 @@
       </c>
       <c r="B43" s="305"/>
       <c r="C43" s="65" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D43" s="306" t="s">
         <v>489</v>
@@ -20053,8 +20054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -22643,7 +22644,7 @@
       <c r="M58" s="516"/>
       <c r="N58" s="98"/>
       <c r="O58" s="516" t="s">
-        <v>1158</v>
+        <v>1163</v>
       </c>
       <c r="P58" s="98"/>
       <c r="Q58" s="54" t="s">
@@ -22687,7 +22688,7 @@
       </c>
       <c r="J59" s="54"/>
       <c r="K59" s="516" t="s">
-        <v>1157</v>
+        <v>1164</v>
       </c>
       <c r="L59" s="98"/>
       <c r="M59" s="516"/>
@@ -22755,7 +22756,7 @@
       </c>
       <c r="B61" s="305"/>
       <c r="C61" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D61" s="306" t="s">
         <v>987</v>
@@ -22797,7 +22798,7 @@
       </c>
       <c r="B62" s="305"/>
       <c r="C62" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D62" s="306" t="s">
         <v>989</v>
@@ -22839,7 +22840,7 @@
       </c>
       <c r="B63" s="305"/>
       <c r="C63" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D63" s="306" t="s">
         <v>990</v>
@@ -22896,8 +22897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R219"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A201" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E223" sqref="E223"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -31088,7 +31089,7 @@
       </c>
       <c r="B212" s="53"/>
       <c r="C212" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D212" s="54" t="s">
         <v>987</v>
@@ -31097,7 +31098,7 @@
         <v>69</v>
       </c>
       <c r="F212" s="54" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="G212" s="57" t="s">
         <v>375</v>
@@ -31106,10 +31107,10 @@
         <v>596</v>
       </c>
       <c r="I212" s="57" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="J212" s="54" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="K212" s="54"/>
       <c r="L212" s="54"/>
@@ -31128,7 +31129,7 @@
       </c>
       <c r="B213" s="53"/>
       <c r="C213" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D213" s="54" t="s">
         <v>987</v>
@@ -31146,14 +31147,14 @@
         <v>596</v>
       </c>
       <c r="I213" s="57" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="J213" s="71">
         <v>1</v>
       </c>
       <c r="K213" s="61"/>
       <c r="L213" s="54" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="M213" s="61" t="b">
         <v>1</v>
@@ -31172,7 +31173,7 @@
       </c>
       <c r="B214" s="53"/>
       <c r="C214" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D214" s="54" t="s">
         <v>987</v>
@@ -31190,14 +31191,14 @@
         <v>596</v>
       </c>
       <c r="I214" s="57" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="J214" s="71">
         <v>1</v>
       </c>
       <c r="K214" s="61"/>
       <c r="L214" s="54" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="M214" s="61" t="b">
         <v>0</v>
@@ -31216,7 +31217,7 @@
       </c>
       <c r="B215" s="53"/>
       <c r="C215" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D215" s="54" t="s">
         <v>987</v>
@@ -31234,14 +31235,14 @@
         <v>596</v>
       </c>
       <c r="I215" s="57" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="J215" s="71">
         <v>1</v>
       </c>
       <c r="K215" s="61"/>
       <c r="L215" s="54" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="M215" s="61"/>
       <c r="N215" s="61"/>
@@ -31258,7 +31259,7 @@
       </c>
       <c r="B216" s="53"/>
       <c r="C216" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D216" s="54" t="s">
         <v>989</v>
@@ -31267,7 +31268,7 @@
         <v>69</v>
       </c>
       <c r="F216" s="54" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="G216" s="57" t="s">
         <v>375</v>
@@ -31276,10 +31277,10 @@
         <v>596</v>
       </c>
       <c r="I216" s="57" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="J216" s="54" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="K216" s="54"/>
       <c r="L216" s="54"/>
@@ -31298,7 +31299,7 @@
       </c>
       <c r="B217" s="53"/>
       <c r="C217" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D217" s="54" t="s">
         <v>989</v>
@@ -31316,14 +31317,14 @@
         <v>596</v>
       </c>
       <c r="I217" s="57" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="J217" s="71">
         <v>1</v>
       </c>
       <c r="K217" s="61"/>
       <c r="L217" s="54" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="M217" s="61" t="b">
         <v>1</v>
@@ -31342,7 +31343,7 @@
       </c>
       <c r="B218" s="53"/>
       <c r="C218" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D218" s="54" t="s">
         <v>990</v>
@@ -31351,7 +31352,7 @@
         <v>69</v>
       </c>
       <c r="F218" s="54" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="G218" s="57" t="s">
         <v>375</v>
@@ -31360,10 +31361,10 @@
         <v>596</v>
       </c>
       <c r="I218" s="57" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="J218" s="54" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="K218" s="54"/>
       <c r="L218" s="54"/>
@@ -31382,7 +31383,7 @@
       </c>
       <c r="B219" s="236"/>
       <c r="C219" s="65" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D219" s="209" t="s">
         <v>990</v>
@@ -31400,14 +31401,14 @@
         <v>596</v>
       </c>
       <c r="I219" s="57" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="J219" s="523">
         <v>1</v>
       </c>
       <c r="K219" s="64"/>
       <c r="L219" s="54" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="M219" s="64" t="b">
         <v>1</v>
@@ -32745,7 +32746,7 @@
       </c>
       <c r="B62" s="128"/>
       <c r="C62" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D62" s="69" t="s">
         <v>54</v>
@@ -34401,7 +34402,7 @@
       </c>
       <c r="B53" s="128"/>
       <c r="C53" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D53" s="69" t="s">
         <v>54</v>
@@ -35726,7 +35727,7 @@
       </c>
       <c r="B60" s="128"/>
       <c r="C60" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D60" s="69" t="s">
         <v>54</v>
@@ -37320,7 +37321,7 @@
       </c>
       <c r="B65" s="128"/>
       <c r="C65" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D65" s="69" t="s">
         <v>54</v>
@@ -38257,7 +38258,7 @@
       </c>
       <c r="B36" s="61"/>
       <c r="C36" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D36" s="461" t="s">
         <v>773</v>
@@ -42743,7 +42744,7 @@
       </c>
       <c r="B246" s="53"/>
       <c r="C246" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D246" s="519" t="s">
         <v>54</v>
@@ -42761,7 +42762,7 @@
       </c>
       <c r="B247" s="53"/>
       <c r="C247" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D247" s="520" t="s">
         <v>57</v>
@@ -42779,7 +42780,7 @@
       </c>
       <c r="B248" s="53"/>
       <c r="C248" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D248" s="519" t="s">
         <v>60</v>
@@ -42797,7 +42798,7 @@
       </c>
       <c r="B249" s="53"/>
       <c r="C249" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D249" s="521" t="s">
         <v>114</v>
@@ -42815,7 +42816,7 @@
       </c>
       <c r="B250" s="53"/>
       <c r="C250" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D250" s="522" t="s">
         <v>124</v>
@@ -42833,7 +42834,7 @@
       </c>
       <c r="B251" s="53"/>
       <c r="C251" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D251" s="54" t="s">
         <v>69</v>
@@ -44797,7 +44798,7 @@
       </c>
       <c r="B75" s="61"/>
       <c r="C75" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D75" s="57" t="s">
         <v>987</v>
@@ -44815,7 +44816,7 @@
       </c>
       <c r="B76" s="61"/>
       <c r="C76" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D76" s="525" t="s">
         <v>989</v>
@@ -44833,7 +44834,7 @@
       </c>
       <c r="B77" s="61"/>
       <c r="C77" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D77" s="57" t="s">
         <v>990</v>
@@ -46001,7 +46002,7 @@
       </c>
       <c r="B54" s="61"/>
       <c r="C54" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D54" s="54" t="s">
         <v>489</v>
@@ -46587,13 +46588,13 @@
       </c>
       <c r="B23" s="341"/>
       <c r="C23" s="271" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D23" s="341" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E23" s="341" t="s">
         <v>1159</v>
-      </c>
-      <c r="D23" s="341" t="s">
-        <v>1160</v>
-      </c>
-      <c r="E23" s="341" t="s">
-        <v>1161</v>
       </c>
       <c r="F23" s="341" t="s">
         <v>770</v>
@@ -52316,7 +52317,7 @@
       </c>
       <c r="B172" s="53"/>
       <c r="C172" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D172" s="54" t="s">
         <v>54</v>
@@ -52347,7 +52348,7 @@
       </c>
       <c r="B173" s="53"/>
       <c r="C173" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D173" s="54" t="s">
         <v>57</v>
@@ -52378,7 +52379,7 @@
       </c>
       <c r="B174" s="53"/>
       <c r="C174" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D174" s="54" t="s">
         <v>60</v>
@@ -52409,7 +52410,7 @@
       </c>
       <c r="B175" s="53"/>
       <c r="C175" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D175" s="104" t="s">
         <v>124</v>
@@ -52440,7 +52441,7 @@
       </c>
       <c r="B176" s="53"/>
       <c r="C176" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D176" s="73" t="s">
         <v>114</v>
@@ -52471,7 +52472,7 @@
       </c>
       <c r="B177" s="53"/>
       <c r="C177" s="271" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D177" s="54" t="s">
         <v>69</v>
@@ -56628,8 +56629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F220" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M243" sqref="M243"/>
+    <sheetView topLeftCell="A153" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -61720,9 +61721,7 @@
       <c r="F173" s="102" t="s">
         <v>967</v>
       </c>
-      <c r="G173" s="102">
-        <v>1</v>
-      </c>
+      <c r="G173" s="102"/>
       <c r="H173" s="72"/>
       <c r="I173" s="72"/>
       <c r="J173" s="72">
@@ -63024,9 +63023,7 @@
       <c r="F217" s="102" t="s">
         <v>967</v>
       </c>
-      <c r="G217" s="102">
-        <v>1</v>
-      </c>
+      <c r="G217" s="102"/>
       <c r="H217" s="72"/>
       <c r="I217" s="72"/>
       <c r="J217" s="72">
@@ -63491,7 +63488,7 @@
       </c>
       <c r="B233" s="72"/>
       <c r="C233" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D233" s="102" t="s">
         <v>990</v>
@@ -63520,7 +63517,7 @@
       </c>
       <c r="B234" s="72"/>
       <c r="C234" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D234" s="102" t="s">
         <v>990</v>
@@ -63549,7 +63546,7 @@
       </c>
       <c r="B235" s="72"/>
       <c r="C235" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D235" s="102" t="s">
         <v>990</v>
@@ -63578,7 +63575,7 @@
       </c>
       <c r="B236" s="72"/>
       <c r="C236" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D236" s="102" t="s">
         <v>990</v>
@@ -63607,7 +63604,7 @@
       </c>
       <c r="B237" s="72"/>
       <c r="C237" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D237" s="102" t="s">
         <v>990</v>
@@ -63636,7 +63633,7 @@
       </c>
       <c r="B238" s="72"/>
       <c r="C238" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D238" s="102" t="s">
         <v>990</v>
@@ -63665,7 +63662,7 @@
       </c>
       <c r="B239" s="72"/>
       <c r="C239" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D239" s="102" t="s">
         <v>990</v>
@@ -63694,7 +63691,7 @@
       </c>
       <c r="B240" s="75"/>
       <c r="C240" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D240" s="102" t="s">
         <v>990</v>
@@ -63725,7 +63722,7 @@
       </c>
       <c r="B241" s="75"/>
       <c r="C241" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D241" s="102" t="s">
         <v>990</v>
@@ -63754,7 +63751,7 @@
       </c>
       <c r="B242" s="72"/>
       <c r="C242" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D242" s="102" t="s">
         <v>990</v>
@@ -63785,7 +63782,7 @@
       </c>
       <c r="B243" s="72"/>
       <c r="C243" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D243" s="102" t="s">
         <v>990</v>
@@ -63816,7 +63813,7 @@
       </c>
       <c r="B244" s="72"/>
       <c r="C244" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D244" s="102" t="s">
         <v>990</v>
@@ -63849,7 +63846,7 @@
       </c>
       <c r="B245" s="72"/>
       <c r="C245" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D245" s="102" t="s">
         <v>990</v>
@@ -63878,7 +63875,7 @@
       </c>
       <c r="B246" s="72"/>
       <c r="C246" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D246" s="102" t="s">
         <v>990</v>
@@ -63907,7 +63904,7 @@
       </c>
       <c r="B247" s="72"/>
       <c r="C247" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D247" s="102" t="s">
         <v>990</v>
@@ -63936,7 +63933,7 @@
       </c>
       <c r="B248" s="72"/>
       <c r="C248" s="525" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D248" s="102" t="s">
         <v>990</v>
@@ -63967,7 +63964,7 @@
       </c>
       <c r="B249" s="72"/>
       <c r="C249" s="57" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D249" s="102" t="s">
         <v>990</v>

</xml_diff>

<commit_message>
ACA-113: resync all Excel & JSON definition files
   [ACA-113](https://tools.hmcts.net/jira/browse/ACA-113)

Resynchronise all Excel and JSON definition files after merger with
 master branch.
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EFFB6A-7279-FF4E-ADA2-3572A8CC8106}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A10E2BE-ED76-FE4D-900B-92CA6450EAC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="21380" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="21380" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -20054,7 +20054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
@@ -22897,8 +22897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R219"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -24039,7 +24039,7 @@
         <v>610</v>
       </c>
       <c r="J32" s="71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P32" s="57" t="s">
         <v>532</v>
@@ -56629,7 +56629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M249"/>
   <sheetViews>
-    <sheetView topLeftCell="A153" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A201" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated spreadsheet with roleToAccessProfiles tab
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7582017-8CF3-FB42-A2CA-7F2ACE29FC81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35571BC8-3102-0B49-B8E0-30A629422331}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="42740" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" firstSheet="16" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,10 @@
     <sheet name="CaseRoles" sheetId="19" r:id="rId23"/>
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId24"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId25"/>
+    <sheet name="RoleToAccessProfiles" sheetId="27" r:id="rId26"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId26"/>
+    <externalReference r:id="rId27"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">CaseEvent!$A$22:$V$22</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9186" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9234" uniqueCount="1212">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3706,6 +3707,72 @@
   </si>
   <si>
     <t>${MCA_API_BASE_URL:http://aac-manage-case-assignment-aat.service.core-compute-aat.internal}/noc/apply-decision</t>
+  </si>
+  <si>
+    <t>RoleToAccessProfiles</t>
+  </si>
+  <si>
+    <t>Role Name</t>
+  </si>
+  <si>
+    <t>Case Type Id</t>
+  </si>
+  <si>
+    <t>Access Profiles</t>
+  </si>
+  <si>
+    <t>Read Only</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>Authorisation</t>
+  </si>
+  <si>
+    <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>Role1</t>
+  </si>
+  <si>
+    <t>auth1</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Role2</t>
+  </si>
+  <si>
+    <t>Role3</t>
+  </si>
+  <si>
+    <t>caseworker-befta_master,caseworker-befta_master-junior</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Role4</t>
+  </si>
+  <si>
+    <t>caseworker-befta_master,caseworker-befta_master-junior,caseworker-befta_master-manager</t>
+  </si>
+  <si>
+    <t>auth2</t>
+  </si>
+  <si>
+    <t>caseworker-befta_master,caseworker-befta_master-solicitor</t>
   </si>
 </sst>
 </file>
@@ -4455,7 +4522,7 @@
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="568">
+  <cellXfs count="574">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -5990,6 +6057,16 @@
     <xf numFmtId="0" fontId="42" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Explanatory Text" xfId="14" builtinId="53"/>
@@ -6009,7 +6086,332 @@
     <cellStyle name="Normal 2 3" xfId="13" xr:uid="{983C50BB-8B6C-1941-95CA-614B186AEA1E}"/>
     <cellStyle name="Normal 3" xfId="15" xr:uid="{B38533D7-3FBF-F547-ABBC-CA99BE96DA12}"/>
   </cellStyles>
-  <dxfs count="345">
+  <dxfs count="357">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -14365,424 +14767,440 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="344" dataDxfId="342" headerRowBorderDxfId="343" tableBorderDxfId="341" totalsRowBorderDxfId="340">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="356" dataDxfId="354" headerRowBorderDxfId="355" tableBorderDxfId="353" totalsRowBorderDxfId="352">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="339"/>
-    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="338"/>
-    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="337"/>
-    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="336"/>
-    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="335"/>
+    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="351"/>
+    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="350"/>
+    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="349"/>
+    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="348"/>
+    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="347"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L91" totalsRowShown="0" headerRowDxfId="210" dataDxfId="208" headerRowBorderDxfId="209" tableBorderDxfId="207" totalsRowBorderDxfId="206">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L91" totalsRowShown="0" headerRowDxfId="222" dataDxfId="220" headerRowBorderDxfId="221" tableBorderDxfId="219" totalsRowBorderDxfId="218">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="205"/>
-    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="204"/>
-    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="203"/>
-    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="202"/>
-    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="201"/>
-    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="200"/>
-    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="199"/>
-    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="198"/>
-    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="197"/>
-    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="196"/>
-    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="195"/>
-    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="194"/>
+    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="217"/>
+    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="216"/>
+    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="215"/>
+    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="214"/>
+    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="213"/>
+    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="212"/>
+    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="211"/>
+    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="210"/>
+    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="209"/>
+    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="208"/>
+    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="207"/>
+    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="206"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H43" totalsRowShown="0" headerRowDxfId="193" dataDxfId="191" headerRowBorderDxfId="192" tableBorderDxfId="190" totalsRowBorderDxfId="189">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H43" totalsRowShown="0" headerRowDxfId="205" dataDxfId="203" headerRowBorderDxfId="204" tableBorderDxfId="202" totalsRowBorderDxfId="201">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="188"/>
-    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="187"/>
-    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="186"/>
-    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="185"/>
-    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="184"/>
-    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="183"/>
-    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="182"/>
-    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="181"/>
+    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="200"/>
+    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="199"/>
+    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="198"/>
+    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="197"/>
+    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="196"/>
+    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="195"/>
+    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="194"/>
+    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="193"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:V63" totalsRowShown="0" headerRowDxfId="180" dataDxfId="178" headerRowBorderDxfId="179" tableBorderDxfId="177" totalsRowBorderDxfId="176">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:V63" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191" tableBorderDxfId="189" totalsRowBorderDxfId="188">
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="175"/>
-    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="174"/>
-    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="173"/>
-    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="172"/>
-    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="171"/>
-    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="170"/>
-    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="169"/>
-    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="168"/>
-    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="167"/>
-    <tableColumn id="22" xr3:uid="{59B33952-3C10-D94F-9012-529644363CBA}" name="EventEnablingCondition" dataDxfId="166"/>
-    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="165" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="164"/>
-    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="163"/>
-    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="162"/>
-    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="161"/>
-    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="160"/>
-    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="159"/>
-    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="158"/>
-    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="157"/>
-    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="156"/>
-    <tableColumn id="21" xr3:uid="{04E7CE93-2C4A-2C46-91EF-227CE86C5C37}" name="EndButtonLabel" dataDxfId="155"/>
-    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="Publish" dataDxfId="154"/>
+    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="187"/>
+    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="186"/>
+    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="185"/>
+    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="184"/>
+    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="183"/>
+    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="182"/>
+    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="181"/>
+    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="180"/>
+    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="179"/>
+    <tableColumn id="22" xr3:uid="{59B33952-3C10-D94F-9012-529644363CBA}" name="EventEnablingCondition" dataDxfId="178"/>
+    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="177" dataCellStyle="Hyperlink"/>
+    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="176"/>
+    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="175"/>
+    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="174"/>
+    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="173"/>
+    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="172"/>
+    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="171"/>
+    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="170"/>
+    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="169"/>
+    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="168"/>
+    <tableColumn id="21" xr3:uid="{04E7CE93-2C4A-2C46-91EF-227CE86C5C37}" name="EndButtonLabel" dataDxfId="167"/>
+    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="Publish" dataDxfId="166"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:T219" totalsRowShown="0" headerRowDxfId="153" dataDxfId="151" headerRowBorderDxfId="152" tableBorderDxfId="150" totalsRowBorderDxfId="149">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:T219" totalsRowShown="0" headerRowDxfId="165" dataDxfId="163" headerRowBorderDxfId="164" tableBorderDxfId="162" totalsRowBorderDxfId="161">
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="148"/>
-    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="147"/>
-    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="146"/>
-    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="145"/>
-    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="144"/>
-    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="143"/>
-    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="142"/>
-    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="141"/>
-    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="140"/>
-    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="139"/>
-    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="138"/>
-    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="137"/>
-    <tableColumn id="18" xr3:uid="{E135335A-D7E2-F744-932E-E0627D2DBFE1}" name="RetainHiddenValue" dataDxfId="136"/>
-    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="135"/>
-    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="134"/>
-    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="133"/>
-    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="132"/>
-    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="131"/>
-    <tableColumn id="19" xr3:uid="{0255F9F3-66BA-7246-ADBF-34F9BD2A0891}" name="Publish" dataDxfId="130"/>
-    <tableColumn id="20" xr3:uid="{E15A3DC7-3833-CD47-A223-0E3415B27FEB}" name="PublishAs" dataDxfId="129"/>
+    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="160"/>
+    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="159"/>
+    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="158"/>
+    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="157"/>
+    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="156"/>
+    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="155"/>
+    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="154"/>
+    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="153"/>
+    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="152"/>
+    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="151"/>
+    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="150"/>
+    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="149"/>
+    <tableColumn id="18" xr3:uid="{E135335A-D7E2-F744-932E-E0627D2DBFE1}" name="RetainHiddenValue" dataDxfId="148"/>
+    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="147"/>
+    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="146"/>
+    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="145"/>
+    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="144"/>
+    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="143"/>
+    <tableColumn id="19" xr3:uid="{0255F9F3-66BA-7246-ADBF-34F9BD2A0891}" name="Publish" dataDxfId="142"/>
+    <tableColumn id="20" xr3:uid="{E15A3DC7-3833-CD47-A223-0E3415B27FEB}" name="PublishAs" dataDxfId="141"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H65" totalsRowShown="0" headerRowDxfId="128" dataDxfId="126" headerRowBorderDxfId="127" tableBorderDxfId="125" totalsRowBorderDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H65" totalsRowShown="0" headerRowDxfId="140" dataDxfId="138" headerRowBorderDxfId="139" tableBorderDxfId="137" totalsRowBorderDxfId="136">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="120"/>
-    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="119"/>
-    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="118"/>
-    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="117"/>
-    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="116"/>
+    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="135"/>
+    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="134"/>
+    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="133"/>
+    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="132"/>
+    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="131"/>
+    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="130"/>
+    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="129"/>
+    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{CF42F456-2174-844D-BD1A-9B3267933793}" name="Table25" displayName="Table25" ref="A3:K8" totalsRowShown="0" headerRowDxfId="115" dataDxfId="113" headerRowBorderDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{CF42F456-2174-844D-BD1A-9B3267933793}" name="Table25" displayName="Table25" ref="A3:K8" totalsRowShown="0" headerRowDxfId="127" dataDxfId="125" headerRowBorderDxfId="126">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{301CF7DA-51FC-2841-B0AF-CFD23525E5C6}" name="LiveFrom" dataDxfId="112" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" xr3:uid="{89A7417A-B1D1-F646-9354-5A772207AE0E}" name="LiveTo" dataDxfId="111" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" xr3:uid="{F1404EC3-6170-8D49-AE3C-527B0FC5DB6E}" name="CaseTypeID" dataDxfId="110" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" xr3:uid="{95ED0AF5-1B8E-9C40-BFB3-3AF78C4508E0}" name="UserRole" dataDxfId="109"/>
-    <tableColumn id="5" xr3:uid="{C19CA352-EB67-B74E-B3C8-117768BA9CDE}" name="CaseFieldID" dataDxfId="108" dataCellStyle="Normal 3"/>
-    <tableColumn id="6" xr3:uid="{C591A817-E1FA-8444-B21B-B966CAD14309}" name="ListElementCode" dataDxfId="107" dataCellStyle="Normal 3"/>
-    <tableColumn id="7" xr3:uid="{5487859C-EBA3-C640-995F-D3FFDA9D05BE}" name="Label" dataDxfId="106" dataCellStyle="Normal 3"/>
-    <tableColumn id="8" xr3:uid="{43381613-E419-A942-B697-B0AAC102ABEF}" name="DisplayOrder" dataDxfId="105" dataCellStyle="Normal 3"/>
-    <tableColumn id="9" xr3:uid="{58E7B797-431B-F449-A1C3-4EEAE5581C98}" name="ResultsOrdering" dataDxfId="104"/>
-    <tableColumn id="10" xr3:uid="{3BDA7798-6F1A-5E41-9E0E-7CA85DF8CFBE}" name="DisplayContextParameter" dataDxfId="103" dataCellStyle="Normal 3"/>
-    <tableColumn id="11" xr3:uid="{C4812D4E-DF32-4646-A206-97EEE7C4AC49}" name="UseCase" dataDxfId="102" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{301CF7DA-51FC-2841-B0AF-CFD23525E5C6}" name="LiveFrom" dataDxfId="124" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{89A7417A-B1D1-F646-9354-5A772207AE0E}" name="LiveTo" dataDxfId="123" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{F1404EC3-6170-8D49-AE3C-527B0FC5DB6E}" name="CaseTypeID" dataDxfId="122" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{95ED0AF5-1B8E-9C40-BFB3-3AF78C4508E0}" name="UserRole" dataDxfId="121"/>
+    <tableColumn id="5" xr3:uid="{C19CA352-EB67-B74E-B3C8-117768BA9CDE}" name="CaseFieldID" dataDxfId="120" dataCellStyle="Normal 3"/>
+    <tableColumn id="6" xr3:uid="{C591A817-E1FA-8444-B21B-B966CAD14309}" name="ListElementCode" dataDxfId="119" dataCellStyle="Normal 3"/>
+    <tableColumn id="7" xr3:uid="{5487859C-EBA3-C640-995F-D3FFDA9D05BE}" name="Label" dataDxfId="118" dataCellStyle="Normal 3"/>
+    <tableColumn id="8" xr3:uid="{43381613-E419-A942-B697-B0AAC102ABEF}" name="DisplayOrder" dataDxfId="117" dataCellStyle="Normal 3"/>
+    <tableColumn id="9" xr3:uid="{58E7B797-431B-F449-A1C3-4EEAE5581C98}" name="ResultsOrdering" dataDxfId="116"/>
+    <tableColumn id="10" xr3:uid="{3BDA7798-6F1A-5E41-9E0E-7CA85DF8CFBE}" name="DisplayContextParameter" dataDxfId="115" dataCellStyle="Normal 3"/>
+    <tableColumn id="11" xr3:uid="{C4812D4E-DF32-4646-A206-97EEE7C4AC49}" name="UseCase" dataDxfId="114" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:I57" totalsRowShown="0" headerRowDxfId="101" dataDxfId="99" headerRowBorderDxfId="100" tableBorderDxfId="98" totalsRowBorderDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:I57" totalsRowShown="0" headerRowDxfId="113" dataDxfId="111" headerRowBorderDxfId="112" tableBorderDxfId="110" totalsRowBorderDxfId="109">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="95"/>
-    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="94"/>
-    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="93"/>
-    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="92"/>
-    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="91"/>
-    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="90"/>
-    <tableColumn id="8" xr3:uid="{657A9DAE-71A1-9C4B-9DA1-6389E9ABA071}" name="ResultsOrdering" dataDxfId="89"/>
-    <tableColumn id="9" xr3:uid="{E69EB06A-51D8-2244-9D47-AD56CDDD3A73}" name="DisplayContextParameter" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="107"/>
+    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="106"/>
+    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="105"/>
+    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="104"/>
+    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="103"/>
+    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="102"/>
+    <tableColumn id="8" xr3:uid="{657A9DAE-71A1-9C4B-9DA1-6389E9ABA071}" name="ResultsOrdering" dataDxfId="101"/>
+    <tableColumn id="9" xr3:uid="{E69EB06A-51D8-2244-9D47-AD56CDDD3A73}" name="DisplayContextParameter" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H65" totalsRowShown="0" headerRowDxfId="87" dataDxfId="85" headerRowBorderDxfId="86" tableBorderDxfId="84" totalsRowBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H65" totalsRowShown="0" headerRowDxfId="99" dataDxfId="97" headerRowBorderDxfId="98" tableBorderDxfId="96" totalsRowBorderDxfId="95">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="78"/>
-    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="77"/>
-    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="76"/>
-    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="91"/>
+    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="89"/>
+    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="88"/>
+    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I74" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71" totalsRowBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I74" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83" totalsRowBorderDxfId="82">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="66"/>
-    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="63"/>
-    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="78"/>
+    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="75"/>
+    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="74"/>
+    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="60" dataDxfId="58" headerRowBorderDxfId="59" tableBorderDxfId="57" totalsRowBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="334" dataDxfId="332" headerRowBorderDxfId="333" tableBorderDxfId="331" totalsRowBorderDxfId="330">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="346" dataDxfId="344" headerRowBorderDxfId="345" tableBorderDxfId="343" totalsRowBorderDxfId="342">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="329"/>
-    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="328"/>
-    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="327"/>
-    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="326" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="341"/>
+    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="340"/>
+    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="339"/>
+    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="338" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E40" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E40" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F251" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F251" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D23" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D23" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="22" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="34" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F77" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F77" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F56" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F56" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A3BF40E7-D513-8F4C-84E2-9360695087C6}" name="Table2214" displayName="Table2214" ref="A3:H56" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{09FC8A4F-739A-B146-9FE9-53F353067853}" name="LiveFrom" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{55191203-C618-2645-A397-D76EC379BC5B}" name="LiveTo" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{367C5031-E752-5E46-9E8A-F9F4D6B8D984}" name="RoleName" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{8F4653C6-E57E-944C-993E-C18678C97B81}" name="Authorisation" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{6B939F73-E9A2-144F-8A42-E2C7E93EF63B}" name="CaseTypeID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{8E45FC73-BD15-5D4A-A5D3-B823B0F4B8BA}" name="AccessProfiles" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D92BBEC4-9549-0242-BAFC-9F6DEE98FE8E}" name="ReadOnly" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{71E500C3-F5AF-ED45-A12E-4107F3E9BA2A}" name="Disabled" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I24" totalsRowShown="0" headerRowDxfId="325" dataDxfId="323" headerRowBorderDxfId="324" tableBorderDxfId="322" totalsRowBorderDxfId="321">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I24" totalsRowShown="0" headerRowDxfId="337" dataDxfId="335" headerRowBorderDxfId="336" tableBorderDxfId="334" totalsRowBorderDxfId="333">
   <autoFilter ref="A3:I24" xr:uid="{C0075E79-5DBE-654F-827E-CA137EF61FB4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="320"/>
-    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="319"/>
-    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="318"/>
-    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="317"/>
-    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="316"/>
-    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="315"/>
-    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="314"/>
-    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="313"/>
-    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="312"/>
+    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="332"/>
+    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="331"/>
+    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="330"/>
+    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="329"/>
+    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="328"/>
+    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="327"/>
+    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="326"/>
+    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="325"/>
+    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="324"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:O177" totalsRowShown="0" headerRowDxfId="311" dataDxfId="309" headerRowBorderDxfId="310" tableBorderDxfId="308" totalsRowBorderDxfId="307">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:O177" totalsRowShown="0" headerRowDxfId="323" dataDxfId="321" headerRowBorderDxfId="322" tableBorderDxfId="320" totalsRowBorderDxfId="319">
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="306"/>
-    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="305"/>
-    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="304"/>
-    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="303"/>
-    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="302"/>
-    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="301"/>
-    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="300"/>
-    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="299"/>
-    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="298"/>
-    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="297"/>
-    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="296"/>
-    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="295"/>
-    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="294"/>
-    <tableColumn id="14" xr3:uid="{04523CC4-7DD9-BC4B-BEE9-93E1915A632A}" name="DefaultHidden" dataDxfId="293"/>
-    <tableColumn id="15" xr3:uid="{DB795945-BA18-EE44-815E-AD737CF2E8DD}" name="Searchable" dataDxfId="292"/>
+    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="318"/>
+    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="317"/>
+    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="316"/>
+    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="315"/>
+    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="314"/>
+    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="313"/>
+    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="312"/>
+    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="311"/>
+    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="310"/>
+    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="309"/>
+    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="308"/>
+    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="307"/>
+    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="306"/>
+    <tableColumn id="14" xr3:uid="{04523CC4-7DD9-BC4B-BEE9-93E1915A632A}" name="DefaultHidden" dataDxfId="305"/>
+    <tableColumn id="15" xr3:uid="{DB795945-BA18-EE44-815E-AD737CF2E8DD}" name="Searchable" dataDxfId="304"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:T88" totalsRowShown="0" headerRowDxfId="291" dataDxfId="289" headerRowBorderDxfId="290" tableBorderDxfId="288" totalsRowBorderDxfId="287">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:T88" totalsRowShown="0" headerRowDxfId="303" dataDxfId="301" headerRowBorderDxfId="302" tableBorderDxfId="300" totalsRowBorderDxfId="299">
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="286"/>
-    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="285"/>
-    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="284"/>
-    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="283"/>
-    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="282"/>
-    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="281"/>
-    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="280"/>
-    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="279"/>
-    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="278"/>
-    <tableColumn id="20" xr3:uid="{3056D2D9-052A-4948-A9B6-EA6D4AEEE813}" name="RetainHiddenValue" dataDxfId="277"/>
-    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="276"/>
-    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="275"/>
-    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="274"/>
-    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="273"/>
-    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="272"/>
-    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="271"/>
-    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="270"/>
-    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="269"/>
-    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="268"/>
-    <tableColumn id="19" xr3:uid="{4721EA60-AB43-3A4D-9D3A-D995D789F1AA}" name="Searchable" dataDxfId="267"/>
+    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="298"/>
+    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="297"/>
+    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="296"/>
+    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="295"/>
+    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="294"/>
+    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="293"/>
+    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="292"/>
+    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="291"/>
+    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="290"/>
+    <tableColumn id="20" xr3:uid="{3056D2D9-052A-4948-A9B6-EA6D4AEEE813}" name="RetainHiddenValue" dataDxfId="289"/>
+    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="288"/>
+    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="287"/>
+    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="286"/>
+    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="285"/>
+    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="284"/>
+    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="283"/>
+    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="282"/>
+    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="281"/>
+    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="280"/>
+    <tableColumn id="19" xr3:uid="{4721EA60-AB43-3A4D-9D3A-D995D789F1AA}" name="Searchable" dataDxfId="279"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G48" totalsRowShown="0" headerRowDxfId="266" dataDxfId="264" headerRowBorderDxfId="265" tableBorderDxfId="263" totalsRowBorderDxfId="262" headerRowCellStyle="Normal 2 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G48" totalsRowShown="0" headerRowDxfId="278" dataDxfId="276" headerRowBorderDxfId="277" tableBorderDxfId="275" totalsRowBorderDxfId="274" headerRowCellStyle="Normal 2 3">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="261"/>
-    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="260"/>
-    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="259"/>
-    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="258"/>
-    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="257"/>
-    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="256"/>
-    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="255"/>
+    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="273"/>
+    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="272"/>
+    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="271"/>
+    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="270"/>
+    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="269"/>
+    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="268"/>
+    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="267"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:O249" totalsRowShown="0" headerRowDxfId="254" dataDxfId="252" headerRowBorderDxfId="253" tableBorderDxfId="251" totalsRowBorderDxfId="250">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:O249" totalsRowShown="0" headerRowDxfId="266" dataDxfId="264" headerRowBorderDxfId="265" tableBorderDxfId="263" totalsRowBorderDxfId="262">
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="249"/>
-    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="248"/>
-    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="247"/>
-    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="246"/>
-    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="245"/>
-    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="244"/>
-    <tableColumn id="12" xr3:uid="{4E9EBE21-1E8A-8F42-8DBF-15D634A7D163}" name="DefaultValue" dataDxfId="243"/>
-    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="242"/>
-    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="241"/>
-    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="240"/>
-    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="239"/>
-    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="238"/>
-    <tableColumn id="13" xr3:uid="{A39B3867-9E61-F640-871A-7CF7654CCAC8}" name="RetainHiddenValue" dataDxfId="237"/>
-    <tableColumn id="14" xr3:uid="{638D9B64-7234-F442-B2B1-C5399AD1FC50}" name="Publish" dataDxfId="236"/>
-    <tableColumn id="15" xr3:uid="{047F01DA-F30A-D049-BA08-EC2A6DAC2AAE}" name="PublishAs" dataDxfId="235"/>
+    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="261"/>
+    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="260"/>
+    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="259"/>
+    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="258"/>
+    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="257"/>
+    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="256"/>
+    <tableColumn id="12" xr3:uid="{4E9EBE21-1E8A-8F42-8DBF-15D634A7D163}" name="DefaultValue" dataDxfId="255"/>
+    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="254"/>
+    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="253"/>
+    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="252"/>
+    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="251"/>
+    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="250"/>
+    <tableColumn id="13" xr3:uid="{A39B3867-9E61-F640-871A-7CF7654CCAC8}" name="RetainHiddenValue" dataDxfId="249"/>
+    <tableColumn id="14" xr3:uid="{638D9B64-7234-F442-B2B1-C5399AD1FC50}" name="Publish" dataDxfId="248"/>
+    <tableColumn id="15" xr3:uid="{047F01DA-F30A-D049-BA08-EC2A6DAC2AAE}" name="PublishAs" dataDxfId="247"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G33" totalsRowShown="0" headerRowDxfId="234" dataDxfId="232" headerRowBorderDxfId="233" tableBorderDxfId="231" totalsRowBorderDxfId="230">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G33" totalsRowShown="0" headerRowDxfId="246" dataDxfId="244" headerRowBorderDxfId="245" tableBorderDxfId="243" totalsRowBorderDxfId="242">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="229"/>
-    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="228"/>
-    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="227"/>
-    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="226"/>
-    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="225"/>
-    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="224"/>
-    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="223"/>
+    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="241"/>
+    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="240"/>
+    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="239"/>
+    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="238"/>
+    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="237"/>
+    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="236"/>
+    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="235"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A2772D57-E59F-2C49-82BA-2F8A826F981B}" name="Table24" displayName="Table24" ref="A3:I15" totalsRowShown="0" headerRowDxfId="222" dataDxfId="220" headerRowBorderDxfId="221">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A2772D57-E59F-2C49-82BA-2F8A826F981B}" name="Table24" displayName="Table24" ref="A3:I15" totalsRowShown="0" headerRowDxfId="234" dataDxfId="232" headerRowBorderDxfId="233">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{EB3897FA-8398-4645-B06C-A22BA473519E}" name="LiveTo" dataDxfId="219"/>
-    <tableColumn id="2" xr3:uid="{99353927-15FC-BA4C-B4D7-FDA6EA43AF10}" name="CaseTypeID" dataDxfId="218"/>
-    <tableColumn id="3" xr3:uid="{E2107A93-C2C9-FC44-A5C0-F1560E2CFFDB}" name="ID" dataDxfId="217"/>
-    <tableColumn id="4" xr3:uid="{483E458F-23BC-6442-BCE1-4A5DD98775C7}" name="DisplayOrder" dataDxfId="216"/>
-    <tableColumn id="5" xr3:uid="{3129676F-8344-B24B-B2CD-3FD0837952C2}" name="QuestionText" dataDxfId="215"/>
-    <tableColumn id="6" xr3:uid="{000B8220-15DF-854E-A0BC-F1BBBCF401A4}" name="AnswerFieldType" dataDxfId="214"/>
-    <tableColumn id="7" xr3:uid="{A0E53177-56A8-E14F-A7BD-F9796CA3E5D4}" name="DisplayContextParameter" dataDxfId="213"/>
-    <tableColumn id="8" xr3:uid="{8526709A-AE28-FE44-BFBB-69DF75B42A88}" name="Answer" dataDxfId="212"/>
-    <tableColumn id="9" xr3:uid="{D53C393B-D23F-F64C-8796-C256647586C5}" name="QuestionId" dataDxfId="211"/>
+    <tableColumn id="1" xr3:uid="{EB3897FA-8398-4645-B06C-A22BA473519E}" name="LiveTo" dataDxfId="231"/>
+    <tableColumn id="2" xr3:uid="{99353927-15FC-BA4C-B4D7-FDA6EA43AF10}" name="CaseTypeID" dataDxfId="230"/>
+    <tableColumn id="3" xr3:uid="{E2107A93-C2C9-FC44-A5C0-F1560E2CFFDB}" name="ID" dataDxfId="229"/>
+    <tableColumn id="4" xr3:uid="{483E458F-23BC-6442-BCE1-4A5DD98775C7}" name="DisplayOrder" dataDxfId="228"/>
+    <tableColumn id="5" xr3:uid="{3129676F-8344-B24B-B2CD-3FD0837952C2}" name="QuestionText" dataDxfId="227"/>
+    <tableColumn id="6" xr3:uid="{000B8220-15DF-854E-A0BC-F1BBBCF401A4}" name="AnswerFieldType" dataDxfId="226"/>
+    <tableColumn id="7" xr3:uid="{A0E53177-56A8-E14F-A7BD-F9796CA3E5D4}" name="DisplayContextParameter" dataDxfId="225"/>
+    <tableColumn id="8" xr3:uid="{8526709A-AE28-FE44-BFBB-69DF75B42A88}" name="Answer" dataDxfId="224"/>
+    <tableColumn id="9" xr3:uid="{D53C393B-D23F-F64C-8796-C256647586C5}" name="QuestionId" dataDxfId="223"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -20377,7 +20795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
@@ -34102,7 +34520,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{6F3568F8-75DC-994A-9CD6-5C91B079C7DC}">
           <x14:formula1>
-            <xm:f>'/Users/matt/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\dev\Documents\Definition Files\[RDM-8509.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>'/Users/matt/Library/Containers/com.microsoft.Excel/Data/Documents/Users\dev\Documents\Definition Files\[RDM-8509.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
@@ -47365,6 +47783,766 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C46E332-1601-DB46-9E37-4B0D4219E272}">
+  <dimension ref="A1:I57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="38.5" customWidth="1"/>
+    <col min="6" max="6" width="75.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18">
+      <c r="A1" s="568" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B1" s="568"/>
+      <c r="C1" s="569"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="570" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="570"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" ht="56">
+      <c r="A2" s="571" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="571" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="571" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D2" s="571"/>
+      <c r="E2" s="571" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F2" s="571" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G2" s="571" t="s">
+        <v>1194</v>
+      </c>
+      <c r="H2" s="571" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="362" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="362" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="362" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D3" s="362" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E3" s="362" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="362" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G3" s="362" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H3" s="362" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="59">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="59"/>
+      <c r="C4" s="75" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E4" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="114" t="s">
+        <v>568</v>
+      </c>
+      <c r="G4" s="114" t="s">
+        <v>233</v>
+      </c>
+      <c r="H4" s="60" t="s">
+        <v>1202</v>
+      </c>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="59">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="59"/>
+      <c r="C5" s="75" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D5" s="75"/>
+      <c r="E5" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="114" t="s">
+        <v>568</v>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>229</v>
+      </c>
+      <c r="H5" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="59">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="75" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D6" s="75"/>
+      <c r="E6" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="114" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G6" s="57" t="s">
+        <v>1206</v>
+      </c>
+      <c r="H6" s="57" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="59">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="59"/>
+      <c r="C7" s="75" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D7" s="75"/>
+      <c r="E7" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="114" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G7" s="114" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="60" t="s">
+        <v>233</v>
+      </c>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="59">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="75" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D8" s="75" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E8" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="114" t="s">
+        <v>1211</v>
+      </c>
+      <c r="G8" s="114" t="s">
+        <v>229</v>
+      </c>
+      <c r="H8" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="59">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="59"/>
+      <c r="C9" s="75" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D9" s="75"/>
+      <c r="E9" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="106" t="s">
+        <v>1161</v>
+      </c>
+      <c r="G9" s="114" t="s">
+        <v>153</v>
+      </c>
+      <c r="H9" s="60" t="s">
+        <v>952</v>
+      </c>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="17"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="59"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="114"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="59"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="59"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="59"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="114"/>
+      <c r="G14" s="114"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="59"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="59"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="17"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="59"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="114"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="59"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="114"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="59"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="114"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="59"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="114"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="59"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="114"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="17"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="59"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="114"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="59"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="114"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="59"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="114"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="59"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="114"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="59"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="114"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="59"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="59"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="59"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="17"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="59"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="17"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="59"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="114"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="59"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="114"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="59"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="572"/>
+      <c r="F33" s="354"/>
+      <c r="G33" s="114"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="59"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="106"/>
+      <c r="D34" s="106"/>
+      <c r="E34" s="572"/>
+      <c r="F34" s="354"/>
+      <c r="G34" s="114"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="59"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="106"/>
+      <c r="D35" s="106"/>
+      <c r="E35" s="572"/>
+      <c r="F35" s="354"/>
+      <c r="G35" s="114"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="59"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="106"/>
+      <c r="E36" s="572"/>
+      <c r="F36" s="354"/>
+      <c r="G36" s="114"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="59"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="106"/>
+      <c r="D37" s="106"/>
+      <c r="E37" s="572"/>
+      <c r="F37" s="354"/>
+      <c r="G37" s="114"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="59"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="572"/>
+      <c r="F38" s="354"/>
+      <c r="G38" s="114"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="59"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="106"/>
+      <c r="E39" s="572"/>
+      <c r="F39" s="354"/>
+      <c r="G39" s="114"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="17"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="59"/>
+      <c r="B40" s="59"/>
+      <c r="C40" s="106"/>
+      <c r="D40" s="106"/>
+      <c r="E40" s="572"/>
+      <c r="F40" s="354"/>
+      <c r="G40" s="114"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="59"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="447"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="59"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="106"/>
+      <c r="D42" s="106"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="106"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="59"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="106"/>
+      <c r="D43" s="106"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="106"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="17"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="59"/>
+      <c r="B44" s="59"/>
+      <c r="C44" s="106"/>
+      <c r="D44" s="106"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="106"/>
+      <c r="H44" s="60"/>
+      <c r="I44" s="17"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="59"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="106"/>
+      <c r="D45" s="106"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="106"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="17"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="59"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="106"/>
+      <c r="D46" s="106"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="106"/>
+      <c r="H46" s="103"/>
+      <c r="I46" s="17"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="59"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="106"/>
+      <c r="D47" s="106"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="106"/>
+      <c r="H47" s="103"/>
+      <c r="I47" s="17"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="59"/>
+      <c r="B48" s="59"/>
+      <c r="C48" s="106"/>
+      <c r="D48" s="106"/>
+      <c r="E48" s="60"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="106"/>
+      <c r="H48" s="103"/>
+      <c r="I48" s="17"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="59"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="106"/>
+      <c r="D49" s="106"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="106"/>
+      <c r="H49" s="103"/>
+      <c r="I49" s="17"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="59"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="106"/>
+      <c r="D50" s="106"/>
+      <c r="E50" s="60"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="106"/>
+      <c r="H50" s="103"/>
+      <c r="I50" s="17"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="59"/>
+      <c r="B51" s="59"/>
+      <c r="C51" s="106"/>
+      <c r="D51" s="106"/>
+      <c r="E51" s="60"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="106"/>
+      <c r="H51" s="103"/>
+      <c r="I51" s="17"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="59"/>
+      <c r="B52" s="59"/>
+      <c r="C52" s="106"/>
+      <c r="D52" s="106"/>
+      <c r="E52" s="60"/>
+      <c r="F52" s="60"/>
+      <c r="G52" s="106"/>
+      <c r="H52" s="103"/>
+      <c r="I52" s="17"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="59"/>
+      <c r="B53" s="59"/>
+      <c r="C53" s="106"/>
+      <c r="D53" s="106"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="106"/>
+      <c r="H53" s="103"/>
+      <c r="I53" s="17"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="58"/>
+      <c r="B54" s="58"/>
+      <c r="C54" s="106"/>
+      <c r="D54" s="106"/>
+      <c r="E54" s="60"/>
+      <c r="F54" s="60"/>
+      <c r="G54" s="106"/>
+      <c r="H54" s="103"/>
+      <c r="I54" s="17"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="58"/>
+      <c r="B55" s="58"/>
+      <c r="C55" s="106"/>
+      <c r="D55" s="106"/>
+      <c r="E55" s="60"/>
+      <c r="F55" s="60"/>
+      <c r="G55" s="106"/>
+      <c r="H55" s="103"/>
+      <c r="I55" s="17"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="63"/>
+      <c r="B56" s="63"/>
+      <c r="C56" s="573"/>
+      <c r="D56" s="573"/>
+      <c r="E56" s="77"/>
+      <c r="F56" s="77"/>
+      <c r="G56" s="573"/>
+      <c r="H56" s="107"/>
+      <c r="I56" s="17"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="17"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>